<commit_message>
Update to E-Team weekly report
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -360,7 +360,7 @@
     <t>MAVRIC</t>
   </si>
   <si>
-    <t>All members have been assigned areas to become SME's in, except Morgan who could not attend the meeting. I am trying to work out her assignment over email. I am also trying to get an estimate on an E-Box prototype to begin building. We are making progress, though most of this semester will likely be training-oriented. I cannot comment on the work ethic or motivation of the team yet.</t>
+    <t>All members have been assigned areas to become SME's, things are going well, people are learning in their areas.</t>
   </si>
 </sst>
 </file>
@@ -1175,6 +1175,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1202,15 +1235,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1229,12 +1253,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1251,24 +1269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1836,8 +1836,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2508,228 +2508,228 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="104" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="107" t="s">
+      <c r="I2" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="108"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="108"/>
-      <c r="AD2" s="108"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="108"/>
-      <c r="AG2" s="108"/>
-      <c r="AH2" s="108"/>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="108"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="109"/>
-      <c r="AM2" s="110" t="s">
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="119"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="120"/>
+      <c r="AM2" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="111"/>
-      <c r="AO2" s="111"/>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="111"/>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AU2" s="111"/>
-      <c r="AV2" s="111"/>
-      <c r="AW2" s="111"/>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="111"/>
-      <c r="AZ2" s="111"/>
-      <c r="BA2" s="112"/>
-      <c r="BB2" s="113" t="s">
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="122"/>
+      <c r="AP2" s="122"/>
+      <c r="AQ2" s="122"/>
+      <c r="AR2" s="122"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="122"/>
+      <c r="AU2" s="122"/>
+      <c r="AV2" s="122"/>
+      <c r="AW2" s="122"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="122"/>
+      <c r="AZ2" s="122"/>
+      <c r="BA2" s="123"/>
+      <c r="BB2" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="114"/>
-      <c r="BD2" s="114"/>
-      <c r="BE2" s="114"/>
-      <c r="BF2" s="114"/>
-      <c r="BG2" s="114"/>
-      <c r="BH2" s="114"/>
-      <c r="BI2" s="114"/>
-      <c r="BJ2" s="114"/>
-      <c r="BK2" s="114"/>
-      <c r="BL2" s="114"/>
-      <c r="BM2" s="114"/>
-      <c r="BN2" s="114"/>
-      <c r="BO2" s="114"/>
-      <c r="BP2" s="115"/>
-      <c r="BQ2" s="113" t="s">
+      <c r="BC2" s="107"/>
+      <c r="BD2" s="107"/>
+      <c r="BE2" s="107"/>
+      <c r="BF2" s="107"/>
+      <c r="BG2" s="107"/>
+      <c r="BH2" s="107"/>
+      <c r="BI2" s="107"/>
+      <c r="BJ2" s="107"/>
+      <c r="BK2" s="107"/>
+      <c r="BL2" s="107"/>
+      <c r="BM2" s="107"/>
+      <c r="BN2" s="107"/>
+      <c r="BO2" s="107"/>
+      <c r="BP2" s="108"/>
+      <c r="BQ2" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="114"/>
-      <c r="BS2" s="114"/>
-      <c r="BT2" s="114"/>
-      <c r="BU2" s="114"/>
-      <c r="BV2" s="114"/>
-      <c r="BW2" s="114"/>
-      <c r="BX2" s="114"/>
-      <c r="BY2" s="114"/>
-      <c r="BZ2" s="114"/>
-      <c r="CA2" s="114"/>
-      <c r="CB2" s="114"/>
-      <c r="CC2" s="114"/>
-      <c r="CD2" s="114"/>
-      <c r="CE2" s="115"/>
+      <c r="BR2" s="107"/>
+      <c r="BS2" s="107"/>
+      <c r="BT2" s="107"/>
+      <c r="BU2" s="107"/>
+      <c r="BV2" s="107"/>
+      <c r="BW2" s="107"/>
+      <c r="BX2" s="107"/>
+      <c r="BY2" s="107"/>
+      <c r="BZ2" s="107"/>
+      <c r="CA2" s="107"/>
+      <c r="CB2" s="107"/>
+      <c r="CC2" s="107"/>
+      <c r="CD2" s="107"/>
+      <c r="CE2" s="108"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="120" t="s">
+      <c r="G3" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="126" t="s">
+      <c r="I3" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127" t="s">
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
-      <c r="S3" s="127" t="s">
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="133"/>
+      <c r="S3" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="127"/>
-      <c r="U3" s="127"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="128"/>
-      <c r="X3" s="129" t="s">
+      <c r="T3" s="133"/>
+      <c r="U3" s="133"/>
+      <c r="V3" s="133"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="130"/>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="130"/>
-      <c r="AB3" s="130"/>
-      <c r="AC3" s="130" t="s">
+      <c r="Y3" s="110"/>
+      <c r="Z3" s="110"/>
+      <c r="AA3" s="110"/>
+      <c r="AB3" s="110"/>
+      <c r="AC3" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="130"/>
-      <c r="AE3" s="130"/>
-      <c r="AF3" s="130"/>
-      <c r="AG3" s="130"/>
-      <c r="AH3" s="130" t="s">
+      <c r="AD3" s="110"/>
+      <c r="AE3" s="110"/>
+      <c r="AF3" s="110"/>
+      <c r="AG3" s="110"/>
+      <c r="AH3" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="130"/>
-      <c r="AK3" s="130"/>
-      <c r="AL3" s="131"/>
-      <c r="AM3" s="132" t="s">
+      <c r="AI3" s="110"/>
+      <c r="AJ3" s="110"/>
+      <c r="AK3" s="110"/>
+      <c r="AL3" s="111"/>
+      <c r="AM3" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="133"/>
-      <c r="AO3" s="133"/>
-      <c r="AP3" s="133"/>
-      <c r="AQ3" s="133"/>
-      <c r="AR3" s="133" t="s">
+      <c r="AN3" s="113"/>
+      <c r="AO3" s="113"/>
+      <c r="AP3" s="113"/>
+      <c r="AQ3" s="113"/>
+      <c r="AR3" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="133"/>
-      <c r="AT3" s="133"/>
-      <c r="AU3" s="133"/>
-      <c r="AV3" s="133"/>
-      <c r="AW3" s="133" t="s">
+      <c r="AS3" s="113"/>
+      <c r="AT3" s="113"/>
+      <c r="AU3" s="113"/>
+      <c r="AV3" s="113"/>
+      <c r="AW3" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="133"/>
-      <c r="AY3" s="133"/>
-      <c r="AZ3" s="133"/>
-      <c r="BA3" s="134"/>
-      <c r="BB3" s="122" t="s">
+      <c r="AX3" s="113"/>
+      <c r="AY3" s="113"/>
+      <c r="AZ3" s="113"/>
+      <c r="BA3" s="114"/>
+      <c r="BB3" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="123"/>
-      <c r="BD3" s="123"/>
-      <c r="BE3" s="123"/>
-      <c r="BF3" s="123"/>
-      <c r="BG3" s="123" t="s">
+      <c r="BC3" s="104"/>
+      <c r="BD3" s="104"/>
+      <c r="BE3" s="104"/>
+      <c r="BF3" s="104"/>
+      <c r="BG3" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="123"/>
-      <c r="BI3" s="123"/>
-      <c r="BJ3" s="123"/>
-      <c r="BK3" s="123"/>
-      <c r="BL3" s="123" t="s">
+      <c r="BH3" s="104"/>
+      <c r="BI3" s="104"/>
+      <c r="BJ3" s="104"/>
+      <c r="BK3" s="104"/>
+      <c r="BL3" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="123"/>
-      <c r="BN3" s="123"/>
-      <c r="BO3" s="123"/>
-      <c r="BP3" s="135"/>
-      <c r="BQ3" s="122" t="s">
+      <c r="BM3" s="104"/>
+      <c r="BN3" s="104"/>
+      <c r="BO3" s="104"/>
+      <c r="BP3" s="105"/>
+      <c r="BQ3" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="123"/>
-      <c r="BS3" s="123"/>
-      <c r="BT3" s="123"/>
-      <c r="BU3" s="123"/>
-      <c r="BV3" s="123" t="s">
+      <c r="BR3" s="104"/>
+      <c r="BS3" s="104"/>
+      <c r="BT3" s="104"/>
+      <c r="BU3" s="104"/>
+      <c r="BV3" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="123"/>
-      <c r="BX3" s="123"/>
-      <c r="BY3" s="123"/>
-      <c r="BZ3" s="123"/>
-      <c r="CA3" s="123" t="s">
+      <c r="BW3" s="104"/>
+      <c r="BX3" s="104"/>
+      <c r="BY3" s="104"/>
+      <c r="BZ3" s="104"/>
+      <c r="CA3" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="123"/>
-      <c r="CC3" s="123"/>
-      <c r="CD3" s="123"/>
-      <c r="CE3" s="135"/>
+      <c r="CB3" s="104"/>
+      <c r="CC3" s="104"/>
+      <c r="CD3" s="104"/>
+      <c r="CE3" s="105"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="117"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="125"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="131"/>
       <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
@@ -5440,17 +5440,6 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5467,6 +5456,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
Updated report with milestones 2 and 3
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -361,6 +361,30 @@
   </si>
   <si>
     <t>All members have been assigned areas to become SME's, things are going well, people are learning in their areas.</t>
+  </si>
+  <si>
+    <t>Circuits/CAD</t>
+  </si>
+  <si>
+    <t>Morgan Foley</t>
+  </si>
+  <si>
+    <t>Refinement</t>
+  </si>
+  <si>
+    <t>Circuits</t>
+  </si>
+  <si>
+    <t>Arm Control</t>
+  </si>
+  <si>
+    <t>Hardware Drivers</t>
+  </si>
+  <si>
+    <t>Firmware Drivers</t>
+  </si>
+  <si>
+    <t>Controls</t>
   </si>
 </sst>
 </file>
@@ -1175,22 +1199,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1208,67 +1292,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1836,7 +1860,7 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:E20"/>
     </sheetView>
   </sheetViews>
@@ -2028,7 +2052,7 @@
       </c>
       <c r="B23" s="57">
         <f>'Team Task Chart'!F5</f>
-        <v>43005</v>
+        <v>42984</v>
       </c>
       <c r="C23" s="58">
         <f>'Team Task Chart'!H5</f>
@@ -2158,13 +2182,13 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="56">
+      <c r="A31" s="56" t="str">
         <f>'Team Task Chart'!C13</f>
-        <v>0</v>
+        <v>Circuits/CAD</v>
       </c>
       <c r="B31" s="57">
         <f>'Team Task Chart'!F13</f>
-        <v>0</v>
+        <v>43019</v>
       </c>
       <c r="C31" s="58">
         <f>'Team Task Chart'!H13</f>
@@ -2192,9 +2216,9 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="56">
+      <c r="A33" s="56" t="str">
         <f>'Team Task Chart'!C15</f>
-        <v>0</v>
+        <v>Refinement</v>
       </c>
       <c r="B33" s="57">
         <f>'Team Task Chart'!F15</f>
@@ -2209,9 +2233,9 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="56">
+      <c r="A34" s="56" t="str">
         <f>'Team Task Chart'!C16</f>
-        <v>0</v>
+        <v>Firmware</v>
       </c>
       <c r="B34" s="57">
         <f>'Team Task Chart'!F16</f>
@@ -2226,9 +2250,9 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="56">
+      <c r="A35" s="56" t="str">
         <f>'Team Task Chart'!C17</f>
-        <v>0</v>
+        <v>Circuits</v>
       </c>
       <c r="B35" s="57">
         <f>'Team Task Chart'!F17</f>
@@ -2243,9 +2267,9 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="56">
+      <c r="A36" s="56" t="str">
         <f>'Team Task Chart'!C18</f>
-        <v>0</v>
+        <v>Controls</v>
       </c>
       <c r="B36" s="57">
         <f>'Team Task Chart'!F18</f>
@@ -2277,9 +2301,9 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="56">
+      <c r="A38" s="56" t="str">
         <f>'Team Task Chart'!C20</f>
-        <v>0</v>
+        <v>Arm Control</v>
       </c>
       <c r="B38" s="57">
         <f>'Team Task Chart'!F20</f>
@@ -2294,9 +2318,9 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="56">
+      <c r="A39" s="56" t="str">
         <f>'Team Task Chart'!C21</f>
-        <v>0</v>
+        <v>Hardware Drivers</v>
       </c>
       <c r="B39" s="57">
         <f>'Team Task Chart'!F21</f>
@@ -2311,9 +2335,9 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="56">
+      <c r="A40" s="56" t="str">
         <f>'Team Task Chart'!C22</f>
-        <v>0</v>
+        <v>Firmware Drivers</v>
       </c>
       <c r="B40" s="57">
         <f>'Team Task Chart'!F22</f>
@@ -2328,9 +2352,9 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="56">
+      <c r="A41" s="56" t="str">
         <f>'Team Task Chart'!C23</f>
-        <v>0</v>
+        <v>Controls</v>
       </c>
       <c r="B41" s="57">
         <f>'Team Task Chart'!F23</f>
@@ -2406,9 +2430,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2508,228 +2532,228 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="115" t="s">
+      <c r="I2" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="116"/>
-      <c r="V2" s="116"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="118" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="119"/>
-      <c r="AI2" s="119"/>
-      <c r="AJ2" s="119"/>
-      <c r="AK2" s="119"/>
-      <c r="AL2" s="120"/>
-      <c r="AM2" s="121" t="s">
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="108"/>
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="108"/>
+      <c r="AG2" s="108"/>
+      <c r="AH2" s="108"/>
+      <c r="AI2" s="108"/>
+      <c r="AJ2" s="108"/>
+      <c r="AK2" s="108"/>
+      <c r="AL2" s="109"/>
+      <c r="AM2" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="122"/>
-      <c r="AO2" s="122"/>
-      <c r="AP2" s="122"/>
-      <c r="AQ2" s="122"/>
-      <c r="AR2" s="122"/>
-      <c r="AS2" s="122"/>
-      <c r="AT2" s="122"/>
-      <c r="AU2" s="122"/>
-      <c r="AV2" s="122"/>
-      <c r="AW2" s="122"/>
-      <c r="AX2" s="122"/>
-      <c r="AY2" s="122"/>
-      <c r="AZ2" s="122"/>
-      <c r="BA2" s="123"/>
-      <c r="BB2" s="106" t="s">
+      <c r="AN2" s="111"/>
+      <c r="AO2" s="111"/>
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="111"/>
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="111"/>
+      <c r="AU2" s="111"/>
+      <c r="AV2" s="111"/>
+      <c r="AW2" s="111"/>
+      <c r="AX2" s="111"/>
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="111"/>
+      <c r="BA2" s="112"/>
+      <c r="BB2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="107"/>
-      <c r="BD2" s="107"/>
-      <c r="BE2" s="107"/>
-      <c r="BF2" s="107"/>
-      <c r="BG2" s="107"/>
-      <c r="BH2" s="107"/>
-      <c r="BI2" s="107"/>
-      <c r="BJ2" s="107"/>
-      <c r="BK2" s="107"/>
-      <c r="BL2" s="107"/>
-      <c r="BM2" s="107"/>
-      <c r="BN2" s="107"/>
-      <c r="BO2" s="107"/>
-      <c r="BP2" s="108"/>
-      <c r="BQ2" s="106" t="s">
+      <c r="BC2" s="114"/>
+      <c r="BD2" s="114"/>
+      <c r="BE2" s="114"/>
+      <c r="BF2" s="114"/>
+      <c r="BG2" s="114"/>
+      <c r="BH2" s="114"/>
+      <c r="BI2" s="114"/>
+      <c r="BJ2" s="114"/>
+      <c r="BK2" s="114"/>
+      <c r="BL2" s="114"/>
+      <c r="BM2" s="114"/>
+      <c r="BN2" s="114"/>
+      <c r="BO2" s="114"/>
+      <c r="BP2" s="115"/>
+      <c r="BQ2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="107"/>
-      <c r="BS2" s="107"/>
-      <c r="BT2" s="107"/>
-      <c r="BU2" s="107"/>
-      <c r="BV2" s="107"/>
-      <c r="BW2" s="107"/>
-      <c r="BX2" s="107"/>
-      <c r="BY2" s="107"/>
-      <c r="BZ2" s="107"/>
-      <c r="CA2" s="107"/>
-      <c r="CB2" s="107"/>
-      <c r="CC2" s="107"/>
-      <c r="CD2" s="107"/>
-      <c r="CE2" s="108"/>
+      <c r="BR2" s="114"/>
+      <c r="BS2" s="114"/>
+      <c r="BT2" s="114"/>
+      <c r="BU2" s="114"/>
+      <c r="BV2" s="114"/>
+      <c r="BW2" s="114"/>
+      <c r="BX2" s="114"/>
+      <c r="BY2" s="114"/>
+      <c r="BZ2" s="114"/>
+      <c r="CA2" s="114"/>
+      <c r="CB2" s="114"/>
+      <c r="CC2" s="114"/>
+      <c r="CD2" s="114"/>
+      <c r="CE2" s="115"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="130" t="s">
+      <c r="H3" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="132" t="s">
+      <c r="I3" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="N3" s="133" t="s">
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="133"/>
-      <c r="P3" s="133"/>
-      <c r="Q3" s="133"/>
-      <c r="R3" s="133"/>
-      <c r="S3" s="133" t="s">
+      <c r="O3" s="127"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="127"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="133"/>
-      <c r="U3" s="133"/>
-      <c r="V3" s="133"/>
-      <c r="W3" s="134"/>
-      <c r="X3" s="135" t="s">
+      <c r="T3" s="127"/>
+      <c r="U3" s="127"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="128"/>
+      <c r="X3" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110" t="s">
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="130"/>
+      <c r="AB3" s="130"/>
+      <c r="AC3" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
-      <c r="AG3" s="110"/>
-      <c r="AH3" s="110" t="s">
+      <c r="AD3" s="130"/>
+      <c r="AE3" s="130"/>
+      <c r="AF3" s="130"/>
+      <c r="AG3" s="130"/>
+      <c r="AH3" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="111"/>
-      <c r="AM3" s="112" t="s">
+      <c r="AI3" s="130"/>
+      <c r="AJ3" s="130"/>
+      <c r="AK3" s="130"/>
+      <c r="AL3" s="131"/>
+      <c r="AM3" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="113"/>
-      <c r="AO3" s="113"/>
-      <c r="AP3" s="113"/>
-      <c r="AQ3" s="113"/>
-      <c r="AR3" s="113" t="s">
+      <c r="AN3" s="133"/>
+      <c r="AO3" s="133"/>
+      <c r="AP3" s="133"/>
+      <c r="AQ3" s="133"/>
+      <c r="AR3" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="113"/>
-      <c r="AT3" s="113"/>
-      <c r="AU3" s="113"/>
-      <c r="AV3" s="113"/>
-      <c r="AW3" s="113" t="s">
+      <c r="AS3" s="133"/>
+      <c r="AT3" s="133"/>
+      <c r="AU3" s="133"/>
+      <c r="AV3" s="133"/>
+      <c r="AW3" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="113"/>
-      <c r="AY3" s="113"/>
-      <c r="AZ3" s="113"/>
-      <c r="BA3" s="114"/>
-      <c r="BB3" s="109" t="s">
+      <c r="AX3" s="133"/>
+      <c r="AY3" s="133"/>
+      <c r="AZ3" s="133"/>
+      <c r="BA3" s="134"/>
+      <c r="BB3" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="104"/>
-      <c r="BD3" s="104"/>
-      <c r="BE3" s="104"/>
-      <c r="BF3" s="104"/>
-      <c r="BG3" s="104" t="s">
+      <c r="BC3" s="123"/>
+      <c r="BD3" s="123"/>
+      <c r="BE3" s="123"/>
+      <c r="BF3" s="123"/>
+      <c r="BG3" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="104"/>
-      <c r="BI3" s="104"/>
-      <c r="BJ3" s="104"/>
-      <c r="BK3" s="104"/>
-      <c r="BL3" s="104" t="s">
+      <c r="BH3" s="123"/>
+      <c r="BI3" s="123"/>
+      <c r="BJ3" s="123"/>
+      <c r="BK3" s="123"/>
+      <c r="BL3" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="104"/>
-      <c r="BN3" s="104"/>
-      <c r="BO3" s="104"/>
-      <c r="BP3" s="105"/>
-      <c r="BQ3" s="109" t="s">
+      <c r="BM3" s="123"/>
+      <c r="BN3" s="123"/>
+      <c r="BO3" s="123"/>
+      <c r="BP3" s="135"/>
+      <c r="BQ3" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="104"/>
-      <c r="BS3" s="104"/>
-      <c r="BT3" s="104"/>
-      <c r="BU3" s="104"/>
-      <c r="BV3" s="104" t="s">
+      <c r="BR3" s="123"/>
+      <c r="BS3" s="123"/>
+      <c r="BT3" s="123"/>
+      <c r="BU3" s="123"/>
+      <c r="BV3" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="104"/>
-      <c r="BX3" s="104"/>
-      <c r="BY3" s="104"/>
-      <c r="BZ3" s="104"/>
-      <c r="CA3" s="104" t="s">
+      <c r="BW3" s="123"/>
+      <c r="BX3" s="123"/>
+      <c r="BY3" s="123"/>
+      <c r="BZ3" s="123"/>
+      <c r="CA3" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="104"/>
-      <c r="CC3" s="104"/>
-      <c r="CD3" s="104"/>
-      <c r="CE3" s="105"/>
+      <c r="CB3" s="123"/>
+      <c r="CC3" s="123"/>
+      <c r="CD3" s="123"/>
+      <c r="CE3" s="135"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="125"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="131"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="125"/>
       <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
@@ -2966,8 +2990,7 @@
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18">
-        <f>MAX(F6:F7)</f>
-        <v>43005</v>
+        <v>42984</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="20">
@@ -3258,11 +3281,11 @@
       <c r="AJ7" s="71"/>
       <c r="AK7" s="71"/>
       <c r="AL7" s="72"/>
-      <c r="AM7" s="76"/>
-      <c r="AN7" s="77"/>
-      <c r="AO7" s="77"/>
-      <c r="AP7" s="77"/>
-      <c r="AQ7" s="77"/>
+      <c r="AM7" s="70"/>
+      <c r="AN7" s="71"/>
+      <c r="AO7" s="71"/>
+      <c r="AP7" s="71"/>
+      <c r="AQ7" s="71"/>
       <c r="AR7" s="78"/>
       <c r="AS7" s="78"/>
       <c r="AT7" s="78"/>
@@ -3808,11 +3831,21 @@
       <c r="CE12" s="79"/>
     </row>
     <row r="13" spans="2:83" ht="18" customHeight="1">
-      <c r="B13" s="21"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="B13" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="24">
+        <v>42999</v>
+      </c>
+      <c r="F13" s="24">
+        <v>43019</v>
+      </c>
       <c r="G13" s="25"/>
       <c r="H13" s="26">
         <v>0</v>
@@ -3980,8 +4013,12 @@
       <c r="CE14" s="79"/>
     </row>
     <row r="15" spans="2:83" ht="18" customHeight="1">
-      <c r="B15" s="21"/>
-      <c r="C15" s="29"/>
+      <c r="B15" s="21">
+        <v>2</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>112</v>
+      </c>
       <c r="D15" s="30"/>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
@@ -4064,9 +4101,15 @@
       <c r="CE15" s="75"/>
     </row>
     <row r="16" spans="2:83" ht="18" customHeight="1">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="B16" s="21">
+        <v>2.1</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>106</v>
+      </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
@@ -4150,9 +4193,15 @@
       <c r="CE16" s="79"/>
     </row>
     <row r="17" spans="2:83" ht="18" customHeight="1">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="B17" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="25"/>
@@ -4237,8 +4286,12 @@
     </row>
     <row r="18" spans="2:83" ht="18" customHeight="1">
       <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>104</v>
+      </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="25"/>
@@ -4408,8 +4461,12 @@
       <c r="CE19" s="79"/>
     </row>
     <row r="20" spans="2:83">
-      <c r="B20" s="21"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="21">
+        <v>3</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>114</v>
+      </c>
       <c r="D20" s="30"/>
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
@@ -4492,9 +4549,15 @@
       <c r="CE20" s="75"/>
     </row>
     <row r="21" spans="2:83">
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
+      <c r="B21" s="21">
+        <v>3.1</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="25"/>
@@ -4578,9 +4641,15 @@
       <c r="CE21" s="79"/>
     </row>
     <row r="22" spans="2:83">
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
+      <c r="B22" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>106</v>
+      </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
@@ -4664,9 +4733,15 @@
       <c r="CE22" s="79"/>
     </row>
     <row r="23" spans="2:83">
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="21">
+        <v>3.3</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>104</v>
+      </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="25"/>
@@ -4750,9 +4825,15 @@
       <c r="CE23" s="79"/>
     </row>
     <row r="24" spans="2:83">
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
+      <c r="B24" s="21">
+        <v>3.4</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25"/>
@@ -5357,7 +5438,7 @@
       <c r="F31" s="36"/>
       <c r="G31" s="37"/>
       <c r="H31" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="89"/>
       <c r="J31" s="90"/>
@@ -5440,6 +5521,17 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5456,17 +5548,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
E-Team report (wk 8)
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We are still doing research into the kwnoledge bases while we wait for a final E-Box design from Mechanical. We've found BLDC motor drivers (cheaper than out VEX ESC units) and the mechanical team is searching for motors. The electronics mounting plate should be ordered soon to start building the system.</t>
+    <t>We hit hangups slecting motors (supporting mechanical). It seems that BLDC motors don't carry the advantages I've been led to believe they should. We may go back to DC motors. I've come to the conclusion that without electronics experience, the team is at risk. I've spent most of the time trying (and mostly failing due to lack of information) to support mechanical and soil science on motor selection, and have made little progress on the E-Box and firmware setup.</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,6 +676,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -992,7 +998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1111,7 +1117,6 @@
     <xf numFmtId="0" fontId="11" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1168,22 +1173,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1201,67 +1266,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1316,6 +1321,9 @@
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1697,174 +1705,174 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="86"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="86"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1881,512 +1889,512 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="120" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="120"/>
+    <col min="1" max="1" width="32.875" style="119" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="119"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="118" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="123" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="121" t="s">
+    <row r="2" spans="1:5" s="122" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A2" s="120" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="126" t="s">
+      <c r="A4" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="126" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="127"/>
+      <c r="C4" s="126"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="126" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="127"/>
+      <c r="C5" s="126"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="127"/>
+      <c r="C6" s="126"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="128">
+      <c r="B7" s="127">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="128" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="129" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="130">
+        <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="129" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="130">
+        <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="129" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="130" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="131">
-        <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="130" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="131">
-        <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
-        <v>5</v>
-      </c>
-    </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="128" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="133" t="s">
-        <v>58</v>
+      <c r="B12" s="132" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="135" t="s">
+      <c r="A14" s="134" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="135"/>
-      <c r="C14" s="135"/>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="135"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
+      <c r="A15" s="134"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="135"/>
-      <c r="B16" s="135"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
+      <c r="A16" s="134"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="135"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="135"/>
+      <c r="A17" s="134"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="135"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
+      <c r="A18" s="134"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="135"/>
-      <c r="B19" s="135"/>
-      <c r="C19" s="135"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
+      <c r="A19" s="134"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="135"/>
-      <c r="B20" s="135"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
+      <c r="A20" s="134"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="136" t="s">
+      <c r="A21" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="137"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
+      <c r="B21" s="136"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="138" t="s">
+      <c r="A22" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="138" t="s">
+      <c r="C22" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="138" t="s">
+      <c r="D22" s="137" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="133" t="str">
+      <c r="A23" s="132" t="str">
         <f>'Team Task Chart'!C5</f>
         <v>Setting Up</v>
       </c>
-      <c r="B23" s="139">
+      <c r="B23" s="138">
         <f>'Team Task Chart'!F5</f>
         <v>42984</v>
       </c>
-      <c r="C23" s="140">
+      <c r="C23" s="139">
         <f>'Team Task Chart'!H5</f>
         <v>0.75</v>
       </c>
-      <c r="D23" s="133" t="s">
+      <c r="D23" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="133" t="str">
+      <c r="A24" s="132" t="str">
         <f>'Team Task Chart'!C6</f>
         <v>Assign Roles (Domain Areas)</v>
       </c>
-      <c r="B24" s="139">
+      <c r="B24" s="138">
         <f>'Team Task Chart'!F6</f>
         <v>42998</v>
       </c>
-      <c r="C24" s="140">
+      <c r="C24" s="139">
         <f>'Team Task Chart'!H6</f>
         <v>1</v>
       </c>
-      <c r="D24" s="133" t="s">
+      <c r="D24" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="133" t="str">
+      <c r="A25" s="132" t="str">
         <f>'Team Task Chart'!C7</f>
         <v>Get an E-Box from mechanical</v>
       </c>
-      <c r="B25" s="139">
+      <c r="B25" s="138">
         <f>'Team Task Chart'!F7</f>
         <v>43005</v>
       </c>
-      <c r="C25" s="140">
+      <c r="C25" s="139">
         <f>'Team Task Chart'!H7</f>
         <v>0.25</v>
       </c>
-      <c r="D25" s="133" t="s">
+      <c r="D25" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="133" t="str">
+      <c r="A26" s="132" t="str">
         <f>'Team Task Chart'!C8</f>
         <v>Drive System</v>
       </c>
-      <c r="B26" s="139">
+      <c r="B26" s="138">
         <f>'Team Task Chart'!F8</f>
         <v>43051</v>
       </c>
-      <c r="C26" s="140">
+      <c r="C26" s="139">
         <f>'Team Task Chart'!H8</f>
-        <v>0.3</v>
-      </c>
-      <c r="D26" s="133" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="133" t="str">
+      <c r="A27" s="132" t="str">
         <f>'Team Task Chart'!C9</f>
         <v>Do Research in needed Domains</v>
       </c>
-      <c r="B27" s="139">
+      <c r="B27" s="138">
         <f>'Team Task Chart'!F9</f>
         <v>43051</v>
       </c>
-      <c r="C27" s="140">
+      <c r="C27" s="139">
         <f>'Team Task Chart'!H9</f>
-        <v>0.25</v>
-      </c>
-      <c r="D27" s="133" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="D27" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="133" t="str">
+      <c r="A28" s="132" t="str">
         <f>'Team Task Chart'!C10</f>
         <v>Power Systems</v>
       </c>
-      <c r="B28" s="139">
+      <c r="B28" s="138">
         <f>'Team Task Chart'!F10</f>
         <v>43051</v>
       </c>
-      <c r="C28" s="140">
+      <c r="C28" s="139">
         <f>'Team Task Chart'!H10</f>
-        <v>0.2</v>
-      </c>
-      <c r="D28" s="133" t="s">
-        <v>58</v>
+        <v>0.4</v>
+      </c>
+      <c r="D28" s="132" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="133" t="str">
+      <c r="A29" s="132" t="str">
         <f>'Team Task Chart'!C11</f>
         <v>Control Systems</v>
       </c>
-      <c r="B29" s="139">
+      <c r="B29" s="138">
         <f>'Team Task Chart'!F11</f>
         <v>43051</v>
       </c>
-      <c r="C29" s="140">
+      <c r="C29" s="139">
         <f>'Team Task Chart'!H11</f>
-        <v>0.6</v>
-      </c>
-      <c r="D29" s="133" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="D29" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="133" t="str">
+      <c r="A30" s="132" t="str">
         <f>'Team Task Chart'!C12</f>
         <v>Firmware</v>
       </c>
-      <c r="B30" s="139">
+      <c r="B30" s="138">
         <f>'Team Task Chart'!F12</f>
         <v>43051</v>
       </c>
-      <c r="C30" s="140">
+      <c r="C30" s="139">
         <f>'Team Task Chart'!H12</f>
-        <v>0.15</v>
-      </c>
-      <c r="D30" s="133" t="s">
-        <v>58</v>
+        <v>0.3</v>
+      </c>
+      <c r="D30" s="132" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="133" t="str">
+      <c r="A31" s="132" t="str">
         <f>'Team Task Chart'!C13</f>
         <v>Circuits/CAD</v>
       </c>
-      <c r="B31" s="139">
+      <c r="B31" s="138">
         <f>'Team Task Chart'!F13</f>
         <v>43051</v>
       </c>
-      <c r="C31" s="140">
+      <c r="C31" s="139">
         <f>'Team Task Chart'!H13</f>
-        <v>0.2</v>
-      </c>
-      <c r="D31" s="133" t="s">
-        <v>58</v>
+        <v>0.3</v>
+      </c>
+      <c r="D31" s="132" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="133">
+      <c r="A32" s="132">
         <f>'Team Task Chart'!C14</f>
         <v>0</v>
       </c>
-      <c r="B32" s="139">
+      <c r="B32" s="138">
         <f>'Team Task Chart'!F14</f>
         <v>0</v>
       </c>
-      <c r="C32" s="140">
+      <c r="C32" s="139">
         <f>'Team Task Chart'!H14</f>
         <v>0</v>
       </c>
-      <c r="D32" s="133" t="s">
+      <c r="D32" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="133" t="str">
+      <c r="A33" s="132" t="str">
         <f>'Team Task Chart'!C15</f>
         <v>Refinement</v>
       </c>
-      <c r="B33" s="139">
+      <c r="B33" s="138">
         <f>'Team Task Chart'!F15</f>
         <v>43066</v>
       </c>
-      <c r="C33" s="140">
+      <c r="C33" s="139">
         <f>'Team Task Chart'!H15</f>
         <v>0</v>
       </c>
-      <c r="D33" s="133" t="s">
+      <c r="D33" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="133" t="str">
+      <c r="A34" s="132" t="str">
         <f>'Team Task Chart'!C16</f>
         <v>Firmware</v>
       </c>
-      <c r="B34" s="139">
+      <c r="B34" s="138">
         <f>'Team Task Chart'!F16</f>
         <v>43066</v>
       </c>
-      <c r="C34" s="140">
+      <c r="C34" s="139">
         <f>'Team Task Chart'!H16</f>
         <v>0</v>
       </c>
-      <c r="D34" s="133" t="s">
+      <c r="D34" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="133" t="str">
+      <c r="A35" s="132" t="str">
         <f>'Team Task Chart'!C17</f>
         <v>Circuits</v>
       </c>
-      <c r="B35" s="139">
+      <c r="B35" s="138">
         <f>'Team Task Chart'!F17</f>
         <v>43066</v>
       </c>
-      <c r="C35" s="140">
+      <c r="C35" s="139">
         <f>'Team Task Chart'!H17</f>
         <v>0</v>
       </c>
-      <c r="D35" s="133" t="s">
+      <c r="D35" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="133" t="str">
+      <c r="A36" s="132" t="str">
         <f>'Team Task Chart'!C18</f>
         <v>Controls</v>
       </c>
-      <c r="B36" s="139">
+      <c r="B36" s="138">
         <f>'Team Task Chart'!F18</f>
         <v>43066</v>
       </c>
-      <c r="C36" s="140">
+      <c r="C36" s="139">
         <f>'Team Task Chart'!H18</f>
         <v>0</v>
       </c>
-      <c r="D36" s="133" t="s">
+      <c r="D36" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="133">
+      <c r="A37" s="132">
         <f>'Team Task Chart'!C19</f>
         <v>0</v>
       </c>
-      <c r="B37" s="139">
+      <c r="B37" s="138">
         <f>'Team Task Chart'!F19</f>
         <v>0</v>
       </c>
-      <c r="C37" s="140">
+      <c r="C37" s="139">
         <f>'Team Task Chart'!H19</f>
         <v>0</v>
       </c>
-      <c r="D37" s="133" t="s">
+      <c r="D37" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="133" t="str">
+      <c r="A38" s="132" t="str">
         <f>'Team Task Chart'!C20</f>
         <v>Arm Control</v>
       </c>
-      <c r="B38" s="139">
+      <c r="B38" s="138">
         <f>'Team Task Chart'!F20</f>
         <v>43072</v>
       </c>
-      <c r="C38" s="140">
+      <c r="C38" s="139">
         <f>'Team Task Chart'!H20</f>
         <v>0</v>
       </c>
-      <c r="D38" s="133" t="s">
+      <c r="D38" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="133" t="str">
+      <c r="A39" s="132" t="str">
         <f>'Team Task Chart'!C21</f>
         <v>Hardware Drivers</v>
       </c>
-      <c r="B39" s="139">
+      <c r="B39" s="138">
         <f>'Team Task Chart'!F21</f>
         <v>43072</v>
       </c>
-      <c r="C39" s="140">
+      <c r="C39" s="139">
         <f>'Team Task Chart'!H21</f>
         <v>0</v>
       </c>
-      <c r="D39" s="133" t="s">
+      <c r="D39" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="133" t="str">
+      <c r="A40" s="132" t="str">
         <f>'Team Task Chart'!C22</f>
         <v>Firmware Drivers</v>
       </c>
-      <c r="B40" s="139">
+      <c r="B40" s="138">
         <f>'Team Task Chart'!F22</f>
         <v>43072</v>
       </c>
-      <c r="C40" s="140">
+      <c r="C40" s="139">
         <f>'Team Task Chart'!H22</f>
         <v>0</v>
       </c>
-      <c r="D40" s="133" t="s">
+      <c r="D40" s="132" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="133" t="str">
+      <c r="A41" s="132" t="str">
         <f>'Team Task Chart'!C23</f>
         <v>Controls</v>
       </c>
-      <c r="B41" s="139">
+      <c r="B41" s="138">
         <f>'Team Task Chart'!F23</f>
         <v>43072</v>
       </c>
-      <c r="C41" s="140">
+      <c r="C41" s="139">
         <f>'Team Task Chart'!H23</f>
         <v>0</v>
       </c>
-      <c r="D41" s="133" t="s">
+      <c r="D41" s="132" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2452,9 +2460,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR14" sqref="AR14"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2555,228 +2563,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="101" t="s">
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="102"/>
-      <c r="AA2" s="102"/>
-      <c r="AB2" s="102"/>
-      <c r="AC2" s="102"/>
-      <c r="AD2" s="102"/>
-      <c r="AE2" s="102"/>
-      <c r="AF2" s="102"/>
-      <c r="AG2" s="102"/>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="102"/>
-      <c r="AL2" s="103"/>
-      <c r="AM2" s="104" t="s">
+      <c r="Y2" s="90"/>
+      <c r="Z2" s="90"/>
+      <c r="AA2" s="90"/>
+      <c r="AB2" s="90"/>
+      <c r="AC2" s="90"/>
+      <c r="AD2" s="90"/>
+      <c r="AE2" s="90"/>
+      <c r="AF2" s="90"/>
+      <c r="AG2" s="90"/>
+      <c r="AH2" s="90"/>
+      <c r="AI2" s="90"/>
+      <c r="AJ2" s="90"/>
+      <c r="AK2" s="90"/>
+      <c r="AL2" s="91"/>
+      <c r="AM2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="105"/>
-      <c r="AO2" s="105"/>
-      <c r="AP2" s="105"/>
-      <c r="AQ2" s="105"/>
-      <c r="AR2" s="105"/>
-      <c r="AS2" s="105"/>
-      <c r="AT2" s="105"/>
-      <c r="AU2" s="105"/>
-      <c r="AV2" s="105"/>
-      <c r="AW2" s="105"/>
-      <c r="AX2" s="105"/>
-      <c r="AY2" s="105"/>
-      <c r="AZ2" s="105"/>
-      <c r="BA2" s="106"/>
-      <c r="BB2" s="89" t="s">
+      <c r="AN2" s="93"/>
+      <c r="AO2" s="93"/>
+      <c r="AP2" s="93"/>
+      <c r="AQ2" s="93"/>
+      <c r="AR2" s="93"/>
+      <c r="AS2" s="93"/>
+      <c r="AT2" s="93"/>
+      <c r="AU2" s="93"/>
+      <c r="AV2" s="93"/>
+      <c r="AW2" s="93"/>
+      <c r="AX2" s="93"/>
+      <c r="AY2" s="93"/>
+      <c r="AZ2" s="93"/>
+      <c r="BA2" s="94"/>
+      <c r="BB2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="90"/>
-      <c r="BD2" s="90"/>
-      <c r="BE2" s="90"/>
-      <c r="BF2" s="90"/>
-      <c r="BG2" s="90"/>
-      <c r="BH2" s="90"/>
-      <c r="BI2" s="90"/>
-      <c r="BJ2" s="90"/>
-      <c r="BK2" s="90"/>
-      <c r="BL2" s="90"/>
-      <c r="BM2" s="90"/>
-      <c r="BN2" s="90"/>
-      <c r="BO2" s="90"/>
-      <c r="BP2" s="91"/>
-      <c r="BQ2" s="89" t="s">
+      <c r="BC2" s="96"/>
+      <c r="BD2" s="96"/>
+      <c r="BE2" s="96"/>
+      <c r="BF2" s="96"/>
+      <c r="BG2" s="96"/>
+      <c r="BH2" s="96"/>
+      <c r="BI2" s="96"/>
+      <c r="BJ2" s="96"/>
+      <c r="BK2" s="96"/>
+      <c r="BL2" s="96"/>
+      <c r="BM2" s="96"/>
+      <c r="BN2" s="96"/>
+      <c r="BO2" s="96"/>
+      <c r="BP2" s="97"/>
+      <c r="BQ2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="90"/>
-      <c r="BS2" s="90"/>
-      <c r="BT2" s="90"/>
-      <c r="BU2" s="90"/>
-      <c r="BV2" s="90"/>
-      <c r="BW2" s="90"/>
-      <c r="BX2" s="90"/>
-      <c r="BY2" s="90"/>
-      <c r="BZ2" s="90"/>
-      <c r="CA2" s="90"/>
-      <c r="CB2" s="90"/>
-      <c r="CC2" s="90"/>
-      <c r="CD2" s="90"/>
-      <c r="CE2" s="91"/>
+      <c r="BR2" s="96"/>
+      <c r="BS2" s="96"/>
+      <c r="BT2" s="96"/>
+      <c r="BU2" s="96"/>
+      <c r="BV2" s="96"/>
+      <c r="BW2" s="96"/>
+      <c r="BX2" s="96"/>
+      <c r="BY2" s="96"/>
+      <c r="BZ2" s="96"/>
+      <c r="CA2" s="96"/>
+      <c r="CB2" s="96"/>
+      <c r="CC2" s="96"/>
+      <c r="CD2" s="96"/>
+      <c r="CE2" s="97"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="111" t="s">
+      <c r="F3" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="111" t="s">
+      <c r="G3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="113" t="s">
+      <c r="H3" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116" t="s">
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116" t="s">
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="116"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="118" t="s">
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
-      <c r="AB3" s="93"/>
-      <c r="AC3" s="93" t="s">
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="112"/>
+      <c r="AA3" s="112"/>
+      <c r="AB3" s="112"/>
+      <c r="AC3" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="93"/>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
-      <c r="AH3" s="93" t="s">
+      <c r="AD3" s="112"/>
+      <c r="AE3" s="112"/>
+      <c r="AF3" s="112"/>
+      <c r="AG3" s="112"/>
+      <c r="AH3" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="93"/>
-      <c r="AJ3" s="93"/>
-      <c r="AK3" s="93"/>
-      <c r="AL3" s="94"/>
-      <c r="AM3" s="95" t="s">
+      <c r="AI3" s="112"/>
+      <c r="AJ3" s="112"/>
+      <c r="AK3" s="112"/>
+      <c r="AL3" s="113"/>
+      <c r="AM3" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="96"/>
-      <c r="AO3" s="96"/>
-      <c r="AP3" s="96"/>
-      <c r="AQ3" s="96"/>
-      <c r="AR3" s="96" t="s">
+      <c r="AN3" s="115"/>
+      <c r="AO3" s="115"/>
+      <c r="AP3" s="115"/>
+      <c r="AQ3" s="115"/>
+      <c r="AR3" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="96"/>
-      <c r="AT3" s="96"/>
-      <c r="AU3" s="96"/>
-      <c r="AV3" s="96"/>
-      <c r="AW3" s="96" t="s">
+      <c r="AS3" s="115"/>
+      <c r="AT3" s="115"/>
+      <c r="AU3" s="115"/>
+      <c r="AV3" s="115"/>
+      <c r="AW3" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="96"/>
-      <c r="AY3" s="96"/>
-      <c r="AZ3" s="96"/>
-      <c r="BA3" s="97"/>
-      <c r="BB3" s="92" t="s">
+      <c r="AX3" s="115"/>
+      <c r="AY3" s="115"/>
+      <c r="AZ3" s="115"/>
+      <c r="BA3" s="116"/>
+      <c r="BB3" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="87"/>
-      <c r="BD3" s="87"/>
-      <c r="BE3" s="87"/>
-      <c r="BF3" s="87"/>
-      <c r="BG3" s="87" t="s">
+      <c r="BC3" s="105"/>
+      <c r="BD3" s="105"/>
+      <c r="BE3" s="105"/>
+      <c r="BF3" s="105"/>
+      <c r="BG3" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="87"/>
-      <c r="BI3" s="87"/>
-      <c r="BJ3" s="87"/>
-      <c r="BK3" s="87"/>
-      <c r="BL3" s="87" t="s">
+      <c r="BH3" s="105"/>
+      <c r="BI3" s="105"/>
+      <c r="BJ3" s="105"/>
+      <c r="BK3" s="105"/>
+      <c r="BL3" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="87"/>
-      <c r="BN3" s="87"/>
-      <c r="BO3" s="87"/>
-      <c r="BP3" s="88"/>
-      <c r="BQ3" s="92" t="s">
+      <c r="BM3" s="105"/>
+      <c r="BN3" s="105"/>
+      <c r="BO3" s="105"/>
+      <c r="BP3" s="117"/>
+      <c r="BQ3" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="87"/>
-      <c r="BS3" s="87"/>
-      <c r="BT3" s="87"/>
-      <c r="BU3" s="87"/>
-      <c r="BV3" s="87" t="s">
+      <c r="BR3" s="105"/>
+      <c r="BS3" s="105"/>
+      <c r="BT3" s="105"/>
+      <c r="BU3" s="105"/>
+      <c r="BV3" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="87"/>
-      <c r="BX3" s="87"/>
-      <c r="BY3" s="87"/>
-      <c r="BZ3" s="87"/>
-      <c r="CA3" s="87" t="s">
+      <c r="BW3" s="105"/>
+      <c r="BX3" s="105"/>
+      <c r="BY3" s="105"/>
+      <c r="BZ3" s="105"/>
+      <c r="CA3" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="87"/>
-      <c r="CC3" s="87"/>
-      <c r="CD3" s="87"/>
-      <c r="CE3" s="88"/>
+      <c r="CB3" s="105"/>
+      <c r="CC3" s="105"/>
+      <c r="CD3" s="105"/>
+      <c r="CE3" s="117"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="108"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="114"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="107"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3384,7 +3392,7 @@
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
@@ -3479,7 +3487,7 @@
       </c>
       <c r="G9" s="41"/>
       <c r="H9" s="42">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="I9" s="43"/>
       <c r="J9" s="44"/>
@@ -3550,31 +3558,41 @@
       <c r="AQ9" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="AR9" s="48"/>
-      <c r="AS9" s="48"/>
-      <c r="AT9" s="48"/>
-      <c r="AU9" s="48"/>
-      <c r="AV9" s="45"/>
-      <c r="AW9" s="45"/>
-      <c r="AX9" s="45"/>
-      <c r="AY9" s="45"/>
-      <c r="AZ9" s="45"/>
-      <c r="BA9" s="56"/>
-      <c r="BB9" s="43"/>
-      <c r="BC9" s="44"/>
-      <c r="BD9" s="44"/>
-      <c r="BE9" s="44"/>
-      <c r="BF9" s="44"/>
-      <c r="BG9" s="45"/>
-      <c r="BH9" s="45"/>
-      <c r="BI9" s="45"/>
-      <c r="BJ9" s="45"/>
-      <c r="BK9" s="45"/>
-      <c r="BL9" s="44"/>
-      <c r="BM9" s="44"/>
-      <c r="BN9" s="44"/>
-      <c r="BO9" s="44"/>
-      <c r="BP9" s="49"/>
+      <c r="AR9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW9" s="48"/>
+      <c r="AX9" s="48"/>
+      <c r="AY9" s="48"/>
+      <c r="AZ9" s="48"/>
+      <c r="BA9" s="54"/>
+      <c r="BB9" s="55"/>
+      <c r="BC9" s="48"/>
+      <c r="BD9" s="48"/>
+      <c r="BE9" s="48"/>
+      <c r="BF9" s="48"/>
+      <c r="BG9" s="48"/>
+      <c r="BH9" s="48"/>
+      <c r="BI9" s="48"/>
+      <c r="BJ9" s="48"/>
+      <c r="BK9" s="48"/>
+      <c r="BL9" s="48"/>
+      <c r="BM9" s="48"/>
+      <c r="BN9" s="48"/>
+      <c r="BO9" s="48"/>
+      <c r="BP9" s="54"/>
       <c r="BQ9" s="43"/>
       <c r="BR9" s="44"/>
       <c r="BS9" s="44"/>
@@ -3608,7 +3626,7 @@
       </c>
       <c r="G10" s="41"/>
       <c r="H10" s="42">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="44"/>
@@ -3665,31 +3683,41 @@
       <c r="AQ10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="AR10" s="52"/>
-      <c r="AS10" s="52"/>
-      <c r="AT10" s="52"/>
-      <c r="AU10" s="52"/>
-      <c r="AV10" s="45"/>
-      <c r="AW10" s="44"/>
-      <c r="AX10" s="44"/>
-      <c r="AY10" s="44"/>
-      <c r="AZ10" s="44"/>
-      <c r="BA10" s="49"/>
-      <c r="BB10" s="43"/>
-      <c r="BC10" s="44"/>
-      <c r="BD10" s="44"/>
-      <c r="BE10" s="44"/>
-      <c r="BF10" s="44"/>
-      <c r="BG10" s="45"/>
-      <c r="BH10" s="45"/>
-      <c r="BI10" s="45"/>
-      <c r="BJ10" s="45"/>
-      <c r="BK10" s="45"/>
-      <c r="BL10" s="44"/>
-      <c r="BM10" s="44"/>
-      <c r="BN10" s="44"/>
-      <c r="BO10" s="44"/>
-      <c r="BP10" s="49"/>
+      <c r="AR10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW10" s="52"/>
+      <c r="AX10" s="52"/>
+      <c r="AY10" s="52"/>
+      <c r="AZ10" s="52"/>
+      <c r="BA10" s="53"/>
+      <c r="BB10" s="51"/>
+      <c r="BC10" s="52"/>
+      <c r="BD10" s="52"/>
+      <c r="BE10" s="52"/>
+      <c r="BF10" s="52"/>
+      <c r="BG10" s="52"/>
+      <c r="BH10" s="52"/>
+      <c r="BI10" s="52"/>
+      <c r="BJ10" s="52"/>
+      <c r="BK10" s="52"/>
+      <c r="BL10" s="52"/>
+      <c r="BM10" s="52"/>
+      <c r="BN10" s="52"/>
+      <c r="BO10" s="52"/>
+      <c r="BP10" s="53"/>
       <c r="BQ10" s="43"/>
       <c r="BR10" s="44"/>
       <c r="BS10" s="44"/>
@@ -3723,7 +3751,7 @@
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="42">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="44"/>
@@ -3750,61 +3778,71 @@
       <c r="AE11" s="45"/>
       <c r="AF11" s="45"/>
       <c r="AG11" s="45"/>
-      <c r="AH11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL11" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM11" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ11" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR11" s="57"/>
-      <c r="AS11" s="57"/>
-      <c r="AT11" s="57"/>
-      <c r="AU11" s="57"/>
-      <c r="AV11" s="45"/>
-      <c r="AW11" s="44"/>
-      <c r="AX11" s="44"/>
-      <c r="AY11" s="44"/>
-      <c r="AZ11" s="44"/>
-      <c r="BA11" s="49"/>
-      <c r="BB11" s="43"/>
-      <c r="BC11" s="44"/>
-      <c r="BD11" s="44"/>
-      <c r="BE11" s="44"/>
-      <c r="BF11" s="44"/>
-      <c r="BG11" s="45"/>
-      <c r="BH11" s="45"/>
-      <c r="BI11" s="45"/>
-      <c r="BJ11" s="45"/>
-      <c r="BK11" s="45"/>
-      <c r="BL11" s="44"/>
-      <c r="BM11" s="44"/>
-      <c r="BN11" s="44"/>
-      <c r="BO11" s="44"/>
-      <c r="BP11" s="49"/>
+      <c r="AH11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL11" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM11" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV11" s="140" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW11" s="140"/>
+      <c r="AX11" s="140"/>
+      <c r="AY11" s="140"/>
+      <c r="AZ11" s="140"/>
+      <c r="BA11" s="141"/>
+      <c r="BB11" s="142"/>
+      <c r="BC11" s="140"/>
+      <c r="BD11" s="140"/>
+      <c r="BE11" s="140"/>
+      <c r="BF11" s="140"/>
+      <c r="BG11" s="140"/>
+      <c r="BH11" s="140"/>
+      <c r="BI11" s="140"/>
+      <c r="BJ11" s="140"/>
+      <c r="BK11" s="140"/>
+      <c r="BL11" s="140"/>
+      <c r="BM11" s="140"/>
+      <c r="BN11" s="140"/>
+      <c r="BO11" s="140"/>
+      <c r="BP11" s="141"/>
       <c r="BQ11" s="43"/>
       <c r="BR11" s="44"/>
       <c r="BS11" s="44"/>
@@ -3838,7 +3876,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -3865,61 +3903,71 @@
       <c r="AE12" s="45"/>
       <c r="AF12" s="45"/>
       <c r="AG12" s="45"/>
-      <c r="AH12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL12" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM12" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ12" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR12" s="60"/>
-      <c r="AS12" s="60"/>
-      <c r="AT12" s="60"/>
-      <c r="AU12" s="60"/>
-      <c r="AV12" s="45"/>
-      <c r="AW12" s="44"/>
-      <c r="AX12" s="44"/>
-      <c r="AY12" s="44"/>
-      <c r="AZ12" s="44"/>
-      <c r="BA12" s="49"/>
-      <c r="BB12" s="43"/>
-      <c r="BC12" s="44"/>
-      <c r="BD12" s="44"/>
-      <c r="BE12" s="44"/>
-      <c r="BF12" s="44"/>
-      <c r="BG12" s="45"/>
-      <c r="BH12" s="45"/>
-      <c r="BI12" s="45"/>
-      <c r="BJ12" s="45"/>
-      <c r="BK12" s="45"/>
-      <c r="BL12" s="44"/>
-      <c r="BM12" s="44"/>
-      <c r="BN12" s="44"/>
-      <c r="BO12" s="44"/>
-      <c r="BP12" s="49"/>
+      <c r="AH12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL12" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM12" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW12" s="59"/>
+      <c r="AX12" s="59"/>
+      <c r="AY12" s="59"/>
+      <c r="AZ12" s="59"/>
+      <c r="BA12" s="60"/>
+      <c r="BB12" s="61"/>
+      <c r="BC12" s="59"/>
+      <c r="BD12" s="59"/>
+      <c r="BE12" s="59"/>
+      <c r="BF12" s="59"/>
+      <c r="BG12" s="59"/>
+      <c r="BH12" s="59"/>
+      <c r="BI12" s="59"/>
+      <c r="BJ12" s="59"/>
+      <c r="BK12" s="59"/>
+      <c r="BL12" s="59"/>
+      <c r="BM12" s="59"/>
+      <c r="BN12" s="59"/>
+      <c r="BO12" s="59"/>
+      <c r="BP12" s="60"/>
       <c r="BQ12" s="43"/>
       <c r="BR12" s="44"/>
       <c r="BS12" s="44"/>
@@ -3953,7 +4001,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -3980,61 +4028,71 @@
       <c r="AE13" s="45"/>
       <c r="AF13" s="45"/>
       <c r="AG13" s="45"/>
-      <c r="AH13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL13" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM13" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ13" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR13" s="63"/>
-      <c r="AS13" s="63"/>
-      <c r="AT13" s="63"/>
-      <c r="AU13" s="63"/>
-      <c r="AV13" s="45"/>
-      <c r="AW13" s="44"/>
-      <c r="AX13" s="44"/>
-      <c r="AY13" s="44"/>
-      <c r="AZ13" s="44"/>
-      <c r="BA13" s="49"/>
-      <c r="BB13" s="43"/>
-      <c r="BC13" s="44"/>
-      <c r="BD13" s="44"/>
-      <c r="BE13" s="44"/>
-      <c r="BF13" s="44"/>
-      <c r="BG13" s="45"/>
-      <c r="BH13" s="45"/>
-      <c r="BI13" s="45"/>
-      <c r="BJ13" s="45"/>
-      <c r="BK13" s="45"/>
-      <c r="BL13" s="44"/>
-      <c r="BM13" s="44"/>
-      <c r="BN13" s="44"/>
-      <c r="BO13" s="44"/>
-      <c r="BP13" s="49"/>
+      <c r="AH13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL13" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM13" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW13" s="62"/>
+      <c r="AX13" s="62"/>
+      <c r="AY13" s="62"/>
+      <c r="AZ13" s="62"/>
+      <c r="BA13" s="63"/>
+      <c r="BB13" s="64"/>
+      <c r="BC13" s="62"/>
+      <c r="BD13" s="62"/>
+      <c r="BE13" s="62"/>
+      <c r="BF13" s="62"/>
+      <c r="BG13" s="62"/>
+      <c r="BH13" s="62"/>
+      <c r="BI13" s="62"/>
+      <c r="BJ13" s="62"/>
+      <c r="BK13" s="62"/>
+      <c r="BL13" s="62"/>
+      <c r="BM13" s="62"/>
+      <c r="BN13" s="62"/>
+      <c r="BO13" s="62"/>
+      <c r="BP13" s="63"/>
       <c r="BQ13" s="43"/>
       <c r="BR13" s="44"/>
       <c r="BS13" s="44"/>
@@ -4141,16 +4199,16 @@
       <c r="B15" s="37">
         <v>2</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68">
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67">
         <v>43066</v>
       </c>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -4281,11 +4339,11 @@
       <c r="AO16" s="44"/>
       <c r="AP16" s="44"/>
       <c r="AQ16" s="44"/>
-      <c r="AR16" s="57"/>
-      <c r="AS16" s="57"/>
-      <c r="AT16" s="57"/>
-      <c r="AU16" s="57"/>
-      <c r="AV16" s="57"/>
+      <c r="AR16" s="56"/>
+      <c r="AS16" s="56"/>
+      <c r="AT16" s="56"/>
+      <c r="AU16" s="56"/>
+      <c r="AV16" s="56"/>
       <c r="AW16" s="44"/>
       <c r="AX16" s="44"/>
       <c r="AY16" s="44"/>
@@ -4296,11 +4354,11 @@
       <c r="BD16" s="44"/>
       <c r="BE16" s="44"/>
       <c r="BF16" s="44"/>
-      <c r="BG16" s="63"/>
-      <c r="BH16" s="63"/>
-      <c r="BI16" s="63"/>
-      <c r="BJ16" s="63"/>
-      <c r="BK16" s="63"/>
+      <c r="BG16" s="62"/>
+      <c r="BH16" s="62"/>
+      <c r="BI16" s="62"/>
+      <c r="BJ16" s="62"/>
+      <c r="BK16" s="62"/>
       <c r="BL16" s="44"/>
       <c r="BM16" s="44"/>
       <c r="BN16" s="44"/>
@@ -4376,11 +4434,11 @@
       <c r="AO17" s="44"/>
       <c r="AP17" s="44"/>
       <c r="AQ17" s="44"/>
-      <c r="AR17" s="57"/>
-      <c r="AS17" s="57"/>
-      <c r="AT17" s="57"/>
-      <c r="AU17" s="57"/>
-      <c r="AV17" s="57"/>
+      <c r="AR17" s="56"/>
+      <c r="AS17" s="56"/>
+      <c r="AT17" s="56"/>
+      <c r="AU17" s="56"/>
+      <c r="AV17" s="56"/>
       <c r="AW17" s="44"/>
       <c r="AX17" s="44"/>
       <c r="AY17" s="44"/>
@@ -4391,11 +4449,11 @@
       <c r="BD17" s="44"/>
       <c r="BE17" s="44"/>
       <c r="BF17" s="44"/>
-      <c r="BG17" s="63"/>
-      <c r="BH17" s="63"/>
-      <c r="BI17" s="63"/>
-      <c r="BJ17" s="63"/>
-      <c r="BK17" s="63"/>
+      <c r="BG17" s="62"/>
+      <c r="BH17" s="62"/>
+      <c r="BI17" s="62"/>
+      <c r="BJ17" s="62"/>
+      <c r="BK17" s="62"/>
       <c r="BL17" s="44"/>
       <c r="BM17" s="44"/>
       <c r="BN17" s="44"/>
@@ -4469,11 +4527,11 @@
       <c r="AO18" s="44"/>
       <c r="AP18" s="44"/>
       <c r="AQ18" s="44"/>
-      <c r="AR18" s="57"/>
-      <c r="AS18" s="57"/>
-      <c r="AT18" s="57"/>
-      <c r="AU18" s="57"/>
-      <c r="AV18" s="57"/>
+      <c r="AR18" s="56"/>
+      <c r="AS18" s="56"/>
+      <c r="AT18" s="56"/>
+      <c r="AU18" s="56"/>
+      <c r="AV18" s="56"/>
       <c r="AW18" s="44"/>
       <c r="AX18" s="44"/>
       <c r="AY18" s="44"/>
@@ -4484,11 +4542,11 @@
       <c r="BD18" s="44"/>
       <c r="BE18" s="44"/>
       <c r="BF18" s="44"/>
-      <c r="BG18" s="63"/>
-      <c r="BH18" s="63"/>
-      <c r="BI18" s="63"/>
-      <c r="BJ18" s="63"/>
-      <c r="BK18" s="63"/>
+      <c r="BG18" s="62"/>
+      <c r="BH18" s="62"/>
+      <c r="BI18" s="62"/>
+      <c r="BJ18" s="62"/>
+      <c r="BK18" s="62"/>
       <c r="BL18" s="44"/>
       <c r="BM18" s="44"/>
       <c r="BN18" s="44"/>
@@ -4555,11 +4613,11 @@
       <c r="AO19" s="44"/>
       <c r="AP19" s="44"/>
       <c r="AQ19" s="44"/>
-      <c r="AR19" s="57"/>
-      <c r="AS19" s="57"/>
-      <c r="AT19" s="57"/>
-      <c r="AU19" s="57"/>
-      <c r="AV19" s="57"/>
+      <c r="AR19" s="56"/>
+      <c r="AS19" s="56"/>
+      <c r="AT19" s="56"/>
+      <c r="AU19" s="56"/>
+      <c r="AV19" s="56"/>
       <c r="AW19" s="44"/>
       <c r="AX19" s="44"/>
       <c r="AY19" s="44"/>
@@ -4570,11 +4628,11 @@
       <c r="BD19" s="44"/>
       <c r="BE19" s="44"/>
       <c r="BF19" s="44"/>
-      <c r="BG19" s="63"/>
-      <c r="BH19" s="63"/>
-      <c r="BI19" s="63"/>
-      <c r="BJ19" s="63"/>
-      <c r="BK19" s="63"/>
+      <c r="BG19" s="62"/>
+      <c r="BH19" s="62"/>
+      <c r="BI19" s="62"/>
+      <c r="BJ19" s="62"/>
+      <c r="BK19" s="62"/>
       <c r="BL19" s="44"/>
       <c r="BM19" s="44"/>
       <c r="BN19" s="44"/>
@@ -4600,16 +4658,16 @@
       <c r="B20" s="37">
         <v>3</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68">
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67">
         <v>43072</v>
       </c>
-      <c r="G20" s="69"/>
-      <c r="H20" s="70"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="69"/>
       <c r="I20" s="33"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -4740,11 +4798,11 @@
       <c r="AO21" s="44"/>
       <c r="AP21" s="44"/>
       <c r="AQ21" s="44"/>
-      <c r="AR21" s="57"/>
-      <c r="AS21" s="57"/>
-      <c r="AT21" s="57"/>
-      <c r="AU21" s="57"/>
-      <c r="AV21" s="57"/>
+      <c r="AR21" s="56"/>
+      <c r="AS21" s="56"/>
+      <c r="AT21" s="56"/>
+      <c r="AU21" s="56"/>
+      <c r="AV21" s="56"/>
       <c r="AW21" s="44"/>
       <c r="AX21" s="44"/>
       <c r="AY21" s="44"/>
@@ -4755,11 +4813,11 @@
       <c r="BD21" s="44"/>
       <c r="BE21" s="44"/>
       <c r="BF21" s="44"/>
-      <c r="BG21" s="63"/>
-      <c r="BH21" s="63"/>
-      <c r="BI21" s="63"/>
-      <c r="BJ21" s="63"/>
-      <c r="BK21" s="63"/>
+      <c r="BG21" s="62"/>
+      <c r="BH21" s="62"/>
+      <c r="BI21" s="62"/>
+      <c r="BJ21" s="62"/>
+      <c r="BK21" s="62"/>
       <c r="BL21" s="44"/>
       <c r="BM21" s="44"/>
       <c r="BN21" s="44"/>
@@ -4835,11 +4893,11 @@
       <c r="AO22" s="44"/>
       <c r="AP22" s="44"/>
       <c r="AQ22" s="44"/>
-      <c r="AR22" s="57"/>
-      <c r="AS22" s="57"/>
-      <c r="AT22" s="57"/>
-      <c r="AU22" s="57"/>
-      <c r="AV22" s="57"/>
+      <c r="AR22" s="56"/>
+      <c r="AS22" s="56"/>
+      <c r="AT22" s="56"/>
+      <c r="AU22" s="56"/>
+      <c r="AV22" s="56"/>
       <c r="AW22" s="44"/>
       <c r="AX22" s="44"/>
       <c r="AY22" s="44"/>
@@ -4850,11 +4908,11 @@
       <c r="BD22" s="44"/>
       <c r="BE22" s="44"/>
       <c r="BF22" s="44"/>
-      <c r="BG22" s="63"/>
-      <c r="BH22" s="63"/>
-      <c r="BI22" s="63"/>
-      <c r="BJ22" s="63"/>
-      <c r="BK22" s="63"/>
+      <c r="BG22" s="62"/>
+      <c r="BH22" s="62"/>
+      <c r="BI22" s="62"/>
+      <c r="BJ22" s="62"/>
+      <c r="BK22" s="62"/>
       <c r="BL22" s="44"/>
       <c r="BM22" s="44"/>
       <c r="BN22" s="44"/>
@@ -4930,11 +4988,11 @@
       <c r="AO23" s="44"/>
       <c r="AP23" s="44"/>
       <c r="AQ23" s="44"/>
-      <c r="AR23" s="57"/>
-      <c r="AS23" s="57"/>
-      <c r="AT23" s="57"/>
-      <c r="AU23" s="57"/>
-      <c r="AV23" s="57"/>
+      <c r="AR23" s="56"/>
+      <c r="AS23" s="56"/>
+      <c r="AT23" s="56"/>
+      <c r="AU23" s="56"/>
+      <c r="AV23" s="56"/>
       <c r="AW23" s="44"/>
       <c r="AX23" s="44"/>
       <c r="AY23" s="44"/>
@@ -4945,11 +5003,11 @@
       <c r="BD23" s="44"/>
       <c r="BE23" s="44"/>
       <c r="BF23" s="44"/>
-      <c r="BG23" s="63"/>
-      <c r="BH23" s="63"/>
-      <c r="BI23" s="63"/>
-      <c r="BJ23" s="63"/>
-      <c r="BK23" s="63"/>
+      <c r="BG23" s="62"/>
+      <c r="BH23" s="62"/>
+      <c r="BI23" s="62"/>
+      <c r="BJ23" s="62"/>
+      <c r="BK23" s="62"/>
       <c r="BL23" s="44"/>
       <c r="BM23" s="44"/>
       <c r="BN23" s="44"/>
@@ -5025,11 +5083,11 @@
       <c r="AO24" s="44"/>
       <c r="AP24" s="44"/>
       <c r="AQ24" s="44"/>
-      <c r="AR24" s="57"/>
-      <c r="AS24" s="57"/>
-      <c r="AT24" s="57"/>
-      <c r="AU24" s="57"/>
-      <c r="AV24" s="57"/>
+      <c r="AR24" s="56"/>
+      <c r="AS24" s="56"/>
+      <c r="AT24" s="56"/>
+      <c r="AU24" s="56"/>
+      <c r="AV24" s="56"/>
       <c r="AW24" s="44"/>
       <c r="AX24" s="44"/>
       <c r="AY24" s="44"/>
@@ -5040,11 +5098,11 @@
       <c r="BD24" s="44"/>
       <c r="BE24" s="44"/>
       <c r="BF24" s="44"/>
-      <c r="BG24" s="63"/>
-      <c r="BH24" s="63"/>
-      <c r="BI24" s="63"/>
-      <c r="BJ24" s="63"/>
-      <c r="BK24" s="63"/>
+      <c r="BG24" s="62"/>
+      <c r="BH24" s="62"/>
+      <c r="BI24" s="62"/>
+      <c r="BJ24" s="62"/>
+      <c r="BK24" s="62"/>
       <c r="BL24" s="44"/>
       <c r="BM24" s="44"/>
       <c r="BN24" s="44"/>
@@ -5111,11 +5169,11 @@
       <c r="AO25" s="44"/>
       <c r="AP25" s="44"/>
       <c r="AQ25" s="44"/>
-      <c r="AR25" s="57"/>
-      <c r="AS25" s="57"/>
-      <c r="AT25" s="57"/>
-      <c r="AU25" s="57"/>
-      <c r="AV25" s="57"/>
+      <c r="AR25" s="56"/>
+      <c r="AS25" s="56"/>
+      <c r="AT25" s="56"/>
+      <c r="AU25" s="56"/>
+      <c r="AV25" s="56"/>
       <c r="AW25" s="44"/>
       <c r="AX25" s="44"/>
       <c r="AY25" s="44"/>
@@ -5126,11 +5184,11 @@
       <c r="BD25" s="44"/>
       <c r="BE25" s="44"/>
       <c r="BF25" s="44"/>
-      <c r="BG25" s="63"/>
-      <c r="BH25" s="63"/>
-      <c r="BI25" s="63"/>
-      <c r="BJ25" s="63"/>
-      <c r="BK25" s="63"/>
+      <c r="BG25" s="62"/>
+      <c r="BH25" s="62"/>
+      <c r="BI25" s="62"/>
+      <c r="BJ25" s="62"/>
+      <c r="BK25" s="62"/>
       <c r="BL25" s="44"/>
       <c r="BM25" s="44"/>
       <c r="BN25" s="44"/>
@@ -5154,7 +5212,7 @@
     </row>
     <row r="26" spans="2:83">
       <c r="B26" s="37"/>
-      <c r="C26" s="71"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
@@ -5197,11 +5255,11 @@
       <c r="AO26" s="44"/>
       <c r="AP26" s="44"/>
       <c r="AQ26" s="44"/>
-      <c r="AR26" s="57"/>
-      <c r="AS26" s="57"/>
-      <c r="AT26" s="57"/>
-      <c r="AU26" s="57"/>
-      <c r="AV26" s="57"/>
+      <c r="AR26" s="56"/>
+      <c r="AS26" s="56"/>
+      <c r="AT26" s="56"/>
+      <c r="AU26" s="56"/>
+      <c r="AV26" s="56"/>
       <c r="AW26" s="44"/>
       <c r="AX26" s="44"/>
       <c r="AY26" s="44"/>
@@ -5212,11 +5270,11 @@
       <c r="BD26" s="44"/>
       <c r="BE26" s="44"/>
       <c r="BF26" s="44"/>
-      <c r="BG26" s="63"/>
-      <c r="BH26" s="63"/>
-      <c r="BI26" s="63"/>
-      <c r="BJ26" s="63"/>
-      <c r="BK26" s="63"/>
+      <c r="BG26" s="62"/>
+      <c r="BH26" s="62"/>
+      <c r="BI26" s="62"/>
+      <c r="BJ26" s="62"/>
+      <c r="BK26" s="62"/>
       <c r="BL26" s="44"/>
       <c r="BM26" s="44"/>
       <c r="BN26" s="44"/>
@@ -5240,12 +5298,12 @@
     </row>
     <row r="27" spans="2:83">
       <c r="B27" s="37"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="69"/>
       <c r="I27" s="33"/>
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
@@ -5367,11 +5425,11 @@
       <c r="AO28" s="44"/>
       <c r="AP28" s="44"/>
       <c r="AQ28" s="44"/>
-      <c r="AR28" s="57"/>
-      <c r="AS28" s="57"/>
-      <c r="AT28" s="57"/>
-      <c r="AU28" s="57"/>
-      <c r="AV28" s="57"/>
+      <c r="AR28" s="56"/>
+      <c r="AS28" s="56"/>
+      <c r="AT28" s="56"/>
+      <c r="AU28" s="56"/>
+      <c r="AV28" s="56"/>
       <c r="AW28" s="44"/>
       <c r="AX28" s="44"/>
       <c r="AY28" s="44"/>
@@ -5382,11 +5440,11 @@
       <c r="BD28" s="44"/>
       <c r="BE28" s="44"/>
       <c r="BF28" s="44"/>
-      <c r="BG28" s="63"/>
-      <c r="BH28" s="63"/>
-      <c r="BI28" s="63"/>
-      <c r="BJ28" s="63"/>
-      <c r="BK28" s="63"/>
+      <c r="BG28" s="62"/>
+      <c r="BH28" s="62"/>
+      <c r="BI28" s="62"/>
+      <c r="BJ28" s="62"/>
+      <c r="BK28" s="62"/>
       <c r="BL28" s="44"/>
       <c r="BM28" s="44"/>
       <c r="BN28" s="44"/>
@@ -5453,11 +5511,11 @@
       <c r="AO29" s="44"/>
       <c r="AP29" s="44"/>
       <c r="AQ29" s="44"/>
-      <c r="AR29" s="57"/>
-      <c r="AS29" s="57"/>
-      <c r="AT29" s="57"/>
-      <c r="AU29" s="57"/>
-      <c r="AV29" s="57"/>
+      <c r="AR29" s="56"/>
+      <c r="AS29" s="56"/>
+      <c r="AT29" s="56"/>
+      <c r="AU29" s="56"/>
+      <c r="AV29" s="56"/>
       <c r="AW29" s="44"/>
       <c r="AX29" s="44"/>
       <c r="AY29" s="44"/>
@@ -5468,11 +5526,11 @@
       <c r="BD29" s="44"/>
       <c r="BE29" s="44"/>
       <c r="BF29" s="44"/>
-      <c r="BG29" s="63"/>
-      <c r="BH29" s="63"/>
-      <c r="BI29" s="63"/>
-      <c r="BJ29" s="63"/>
-      <c r="BK29" s="63"/>
+      <c r="BG29" s="62"/>
+      <c r="BH29" s="62"/>
+      <c r="BI29" s="62"/>
+      <c r="BJ29" s="62"/>
+      <c r="BK29" s="62"/>
       <c r="BL29" s="44"/>
       <c r="BM29" s="44"/>
       <c r="BN29" s="44"/>
@@ -5539,11 +5597,11 @@
       <c r="AO30" s="44"/>
       <c r="AP30" s="44"/>
       <c r="AQ30" s="44"/>
-      <c r="AR30" s="57"/>
-      <c r="AS30" s="57"/>
-      <c r="AT30" s="57"/>
-      <c r="AU30" s="57"/>
-      <c r="AV30" s="57"/>
+      <c r="AR30" s="56"/>
+      <c r="AS30" s="56"/>
+      <c r="AT30" s="56"/>
+      <c r="AU30" s="56"/>
+      <c r="AV30" s="56"/>
       <c r="AW30" s="44"/>
       <c r="AX30" s="44"/>
       <c r="AY30" s="44"/>
@@ -5554,11 +5612,11 @@
       <c r="BD30" s="44"/>
       <c r="BE30" s="44"/>
       <c r="BF30" s="44"/>
-      <c r="BG30" s="63"/>
-      <c r="BH30" s="63"/>
-      <c r="BI30" s="63"/>
-      <c r="BJ30" s="63"/>
-      <c r="BK30" s="63"/>
+      <c r="BG30" s="62"/>
+      <c r="BH30" s="62"/>
+      <c r="BI30" s="62"/>
+      <c r="BJ30" s="62"/>
+      <c r="BK30" s="62"/>
       <c r="BL30" s="44"/>
       <c r="BM30" s="44"/>
       <c r="BN30" s="44"/>
@@ -5581,96 +5639,107 @@
       <c r="CE30" s="49"/>
     </row>
     <row r="31" spans="2:83" ht="16.5" thickBot="1">
-      <c r="B31" s="72"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="76">
+      <c r="B31" s="71"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="75">
         <v>0</v>
       </c>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="79"/>
-      <c r="O31" s="79"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="79"/>
-      <c r="R31" s="79"/>
-      <c r="S31" s="78"/>
-      <c r="T31" s="78"/>
-      <c r="U31" s="78"/>
-      <c r="V31" s="78"/>
-      <c r="W31" s="80"/>
-      <c r="X31" s="77"/>
-      <c r="Y31" s="78"/>
-      <c r="Z31" s="78"/>
-      <c r="AA31" s="78"/>
-      <c r="AB31" s="78"/>
-      <c r="AC31" s="81"/>
-      <c r="AD31" s="81"/>
-      <c r="AE31" s="81"/>
-      <c r="AF31" s="81"/>
-      <c r="AG31" s="81"/>
-      <c r="AH31" s="78"/>
-      <c r="AI31" s="78"/>
-      <c r="AJ31" s="78"/>
-      <c r="AK31" s="78"/>
-      <c r="AL31" s="80"/>
-      <c r="AM31" s="77"/>
-      <c r="AN31" s="78"/>
-      <c r="AO31" s="78"/>
-      <c r="AP31" s="78"/>
-      <c r="AQ31" s="78"/>
-      <c r="AR31" s="82"/>
-      <c r="AS31" s="82"/>
-      <c r="AT31" s="82"/>
-      <c r="AU31" s="82"/>
-      <c r="AV31" s="82"/>
-      <c r="AW31" s="78"/>
-      <c r="AX31" s="78"/>
-      <c r="AY31" s="78"/>
-      <c r="AZ31" s="78"/>
-      <c r="BA31" s="80"/>
-      <c r="BB31" s="77"/>
-      <c r="BC31" s="78"/>
-      <c r="BD31" s="78"/>
-      <c r="BE31" s="78"/>
-      <c r="BF31" s="78"/>
-      <c r="BG31" s="83"/>
-      <c r="BH31" s="83"/>
-      <c r="BI31" s="83"/>
-      <c r="BJ31" s="83"/>
-      <c r="BK31" s="83"/>
-      <c r="BL31" s="78"/>
-      <c r="BM31" s="78"/>
-      <c r="BN31" s="78"/>
-      <c r="BO31" s="78"/>
-      <c r="BP31" s="80"/>
-      <c r="BQ31" s="77"/>
-      <c r="BR31" s="78"/>
-      <c r="BS31" s="78"/>
-      <c r="BT31" s="78"/>
-      <c r="BU31" s="78"/>
-      <c r="BV31" s="84"/>
-      <c r="BW31" s="84"/>
-      <c r="BX31" s="84"/>
-      <c r="BY31" s="84"/>
-      <c r="BZ31" s="84"/>
-      <c r="CA31" s="78"/>
-      <c r="CB31" s="78"/>
-      <c r="CC31" s="78"/>
-      <c r="CD31" s="78"/>
-      <c r="CE31" s="80"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
+      <c r="R31" s="78"/>
+      <c r="S31" s="77"/>
+      <c r="T31" s="77"/>
+      <c r="U31" s="77"/>
+      <c r="V31" s="77"/>
+      <c r="W31" s="79"/>
+      <c r="X31" s="76"/>
+      <c r="Y31" s="77"/>
+      <c r="Z31" s="77"/>
+      <c r="AA31" s="77"/>
+      <c r="AB31" s="77"/>
+      <c r="AC31" s="80"/>
+      <c r="AD31" s="80"/>
+      <c r="AE31" s="80"/>
+      <c r="AF31" s="80"/>
+      <c r="AG31" s="80"/>
+      <c r="AH31" s="77"/>
+      <c r="AI31" s="77"/>
+      <c r="AJ31" s="77"/>
+      <c r="AK31" s="77"/>
+      <c r="AL31" s="79"/>
+      <c r="AM31" s="76"/>
+      <c r="AN31" s="77"/>
+      <c r="AO31" s="77"/>
+      <c r="AP31" s="77"/>
+      <c r="AQ31" s="77"/>
+      <c r="AR31" s="81"/>
+      <c r="AS31" s="81"/>
+      <c r="AT31" s="81"/>
+      <c r="AU31" s="81"/>
+      <c r="AV31" s="81"/>
+      <c r="AW31" s="77"/>
+      <c r="AX31" s="77"/>
+      <c r="AY31" s="77"/>
+      <c r="AZ31" s="77"/>
+      <c r="BA31" s="79"/>
+      <c r="BB31" s="76"/>
+      <c r="BC31" s="77"/>
+      <c r="BD31" s="77"/>
+      <c r="BE31" s="77"/>
+      <c r="BF31" s="77"/>
+      <c r="BG31" s="82"/>
+      <c r="BH31" s="82"/>
+      <c r="BI31" s="82"/>
+      <c r="BJ31" s="82"/>
+      <c r="BK31" s="82"/>
+      <c r="BL31" s="77"/>
+      <c r="BM31" s="77"/>
+      <c r="BN31" s="77"/>
+      <c r="BO31" s="77"/>
+      <c r="BP31" s="79"/>
+      <c r="BQ31" s="76"/>
+      <c r="BR31" s="77"/>
+      <c r="BS31" s="77"/>
+      <c r="BT31" s="77"/>
+      <c r="BU31" s="77"/>
+      <c r="BV31" s="83"/>
+      <c r="BW31" s="83"/>
+      <c r="BX31" s="83"/>
+      <c r="BY31" s="83"/>
+      <c r="BZ31" s="83"/>
+      <c r="CA31" s="77"/>
+      <c r="CB31" s="77"/>
+      <c r="CC31" s="77"/>
+      <c r="CD31" s="77"/>
+      <c r="CE31" s="79"/>
     </row>
     <row r="33" ht="15.95" customHeight="1"/>
     <row r="34" ht="15.95" customHeight="1"/>
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5687,17 +5756,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -5776,7 +5834,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5862,7 +5920,9 @@
       <c r="H2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -5873,7 +5933,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -5904,7 +5964,9 @@
       <c r="H3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -5946,7 +6008,9 @@
       <c r="H4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -5957,7 +6021,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -5988,7 +6052,9 @@
       <c r="H5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -6027,7 +6093,9 @@
       <c r="H6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -6038,7 +6106,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
Week 9 report for E-Team
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We hit hangups slecting motors (supporting mechanical). It seems that BLDC motors don't carry the advantages I've been led to believe they should. We may go back to DC motors. I've come to the conclusion that without electronics experience, the team is at risk. I've spent most of the time trying (and mostly failing due to lack of information) to support mechanical and soil science on motor selection, and have made little progress on the E-Box and firmware setup.</t>
+    <t>The team is still strugling with getting power to the motors. We don't have information on obtaining batteries yet, and haven't completed motor power consumption calculations (started). I've been sick, so some of the component selection has not gotten as far as I wanted.</t>
   </si>
 </sst>
 </file>
@@ -1167,12 +1167,48 @@
     <xf numFmtId="0" fontId="11" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,15 +1236,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1227,12 +1254,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,24 +1270,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1321,9 +1324,6 @@
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,174 +1705,174 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="85"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="85"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="85"/>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="85"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="85"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="85"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="85"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="85"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="85"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="85"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="85"/>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="85"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1889,512 +1889,512 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="119" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="119"/>
+    <col min="1" max="1" width="32.875" style="122" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="122"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="121" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="122" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="120" t="s">
+    <row r="2" spans="1:5" s="125" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A2" s="123" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="126" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="129" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="126"/>
+      <c r="C4" s="129"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="126"/>
+      <c r="C5" s="129"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="128" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="129" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="126"/>
+      <c r="C6" s="129"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="127">
-        <v>8</v>
+      <c r="B7" s="130">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="128" t="s">
+      <c r="A8" s="131" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="130">
+      <c r="B9" s="133">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="129" t="s">
+      <c r="A10" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="130">
+      <c r="B10" s="133">
         <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="131" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="131" t="s">
+      <c r="A12" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="132" t="s">
+      <c r="B12" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="133"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="134"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
+      <c r="A15" s="137"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="137"/>
+      <c r="E15" s="137"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="134"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="137"/>
+      <c r="E16" s="137"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="134"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="134"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
+      <c r="A18" s="137"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="134"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="134"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="138" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="136"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="139"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="137" t="s">
+      <c r="A22" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="137" t="s">
+      <c r="B22" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="137" t="s">
+      <c r="C22" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="137" t="s">
+      <c r="D22" s="140" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="132" t="str">
+      <c r="A23" s="135" t="str">
         <f>'Team Task Chart'!C5</f>
         <v>Setting Up</v>
       </c>
-      <c r="B23" s="138">
+      <c r="B23" s="141">
         <f>'Team Task Chart'!F5</f>
         <v>42984</v>
       </c>
-      <c r="C23" s="139">
+      <c r="C23" s="142">
         <f>'Team Task Chart'!H5</f>
-        <v>0.75</v>
-      </c>
-      <c r="D23" s="132" t="s">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="D23" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="132" t="str">
+      <c r="A24" s="135" t="str">
         <f>'Team Task Chart'!C6</f>
         <v>Assign Roles (Domain Areas)</v>
       </c>
-      <c r="B24" s="138">
+      <c r="B24" s="141">
         <f>'Team Task Chart'!F6</f>
         <v>42998</v>
       </c>
-      <c r="C24" s="139">
+      <c r="C24" s="142">
         <f>'Team Task Chart'!H6</f>
         <v>1</v>
       </c>
-      <c r="D24" s="132" t="s">
+      <c r="D24" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="132" t="str">
+      <c r="A25" s="135" t="str">
         <f>'Team Task Chart'!C7</f>
         <v>Get an E-Box from mechanical</v>
       </c>
-      <c r="B25" s="138">
+      <c r="B25" s="141">
         <f>'Team Task Chart'!F7</f>
         <v>43005</v>
       </c>
-      <c r="C25" s="139">
+      <c r="C25" s="142">
         <f>'Team Task Chart'!H7</f>
-        <v>0.25</v>
-      </c>
-      <c r="D25" s="132" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="D25" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="132" t="str">
+      <c r="A26" s="135" t="str">
         <f>'Team Task Chart'!C8</f>
         <v>Drive System</v>
       </c>
-      <c r="B26" s="138">
+      <c r="B26" s="141">
         <f>'Team Task Chart'!F8</f>
         <v>43051</v>
       </c>
-      <c r="C26" s="139">
+      <c r="C26" s="142">
         <f>'Team Task Chart'!H8</f>
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="132" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="D26" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="132" t="str">
+      <c r="A27" s="135" t="str">
         <f>'Team Task Chart'!C9</f>
         <v>Do Research in needed Domains</v>
       </c>
-      <c r="B27" s="138">
+      <c r="B27" s="141">
         <f>'Team Task Chart'!F9</f>
         <v>43051</v>
       </c>
-      <c r="C27" s="139">
+      <c r="C27" s="142">
         <f>'Team Task Chart'!H9</f>
         <v>0.9</v>
       </c>
-      <c r="D27" s="132" t="s">
+      <c r="D27" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="132" t="str">
+      <c r="A28" s="135" t="str">
         <f>'Team Task Chart'!C10</f>
         <v>Power Systems</v>
       </c>
-      <c r="B28" s="138">
+      <c r="B28" s="141">
         <f>'Team Task Chart'!F10</f>
         <v>43051</v>
       </c>
-      <c r="C28" s="139">
+      <c r="C28" s="142">
         <f>'Team Task Chart'!H10</f>
-        <v>0.4</v>
-      </c>
-      <c r="D28" s="132" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="D28" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="132" t="str">
+      <c r="A29" s="135" t="str">
         <f>'Team Task Chart'!C11</f>
         <v>Control Systems</v>
       </c>
-      <c r="B29" s="138">
+      <c r="B29" s="141">
         <f>'Team Task Chart'!F11</f>
         <v>43051</v>
       </c>
-      <c r="C29" s="139">
+      <c r="C29" s="142">
         <f>'Team Task Chart'!H11</f>
-        <v>0.7</v>
-      </c>
-      <c r="D29" s="132" t="s">
+        <v>0.95</v>
+      </c>
+      <c r="D29" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="132" t="str">
+      <c r="A30" s="135" t="str">
         <f>'Team Task Chart'!C12</f>
         <v>Firmware</v>
       </c>
-      <c r="B30" s="138">
+      <c r="B30" s="141">
         <f>'Team Task Chart'!F12</f>
         <v>43051</v>
       </c>
-      <c r="C30" s="139">
+      <c r="C30" s="142">
         <f>'Team Task Chart'!H12</f>
-        <v>0.3</v>
-      </c>
-      <c r="D30" s="132" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="132" t="str">
+      <c r="A31" s="135" t="str">
         <f>'Team Task Chart'!C13</f>
         <v>Circuits/CAD</v>
       </c>
-      <c r="B31" s="138">
+      <c r="B31" s="141">
         <f>'Team Task Chart'!F13</f>
         <v>43051</v>
       </c>
-      <c r="C31" s="139">
+      <c r="C31" s="142">
         <f>'Team Task Chart'!H13</f>
-        <v>0.3</v>
-      </c>
-      <c r="D31" s="132" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="D31" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="132">
+      <c r="A32" s="135">
         <f>'Team Task Chart'!C14</f>
         <v>0</v>
       </c>
-      <c r="B32" s="138">
+      <c r="B32" s="141">
         <f>'Team Task Chart'!F14</f>
         <v>0</v>
       </c>
-      <c r="C32" s="139">
+      <c r="C32" s="142">
         <f>'Team Task Chart'!H14</f>
         <v>0</v>
       </c>
-      <c r="D32" s="132" t="s">
+      <c r="D32" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="132" t="str">
+      <c r="A33" s="135" t="str">
         <f>'Team Task Chart'!C15</f>
         <v>Refinement</v>
       </c>
-      <c r="B33" s="138">
+      <c r="B33" s="141">
         <f>'Team Task Chart'!F15</f>
         <v>43066</v>
       </c>
-      <c r="C33" s="139">
+      <c r="C33" s="142">
         <f>'Team Task Chart'!H15</f>
         <v>0</v>
       </c>
-      <c r="D33" s="132" t="s">
+      <c r="D33" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="132" t="str">
+      <c r="A34" s="135" t="str">
         <f>'Team Task Chart'!C16</f>
         <v>Firmware</v>
       </c>
-      <c r="B34" s="138">
+      <c r="B34" s="141">
         <f>'Team Task Chart'!F16</f>
         <v>43066</v>
       </c>
-      <c r="C34" s="139">
+      <c r="C34" s="142">
         <f>'Team Task Chart'!H16</f>
         <v>0</v>
       </c>
-      <c r="D34" s="132" t="s">
+      <c r="D34" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="132" t="str">
+      <c r="A35" s="135" t="str">
         <f>'Team Task Chart'!C17</f>
         <v>Circuits</v>
       </c>
-      <c r="B35" s="138">
+      <c r="B35" s="141">
         <f>'Team Task Chart'!F17</f>
         <v>43066</v>
       </c>
-      <c r="C35" s="139">
+      <c r="C35" s="142">
         <f>'Team Task Chart'!H17</f>
         <v>0</v>
       </c>
-      <c r="D35" s="132" t="s">
+      <c r="D35" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="132" t="str">
+      <c r="A36" s="135" t="str">
         <f>'Team Task Chart'!C18</f>
         <v>Controls</v>
       </c>
-      <c r="B36" s="138">
+      <c r="B36" s="141">
         <f>'Team Task Chart'!F18</f>
         <v>43066</v>
       </c>
-      <c r="C36" s="139">
+      <c r="C36" s="142">
         <f>'Team Task Chart'!H18</f>
         <v>0</v>
       </c>
-      <c r="D36" s="132" t="s">
+      <c r="D36" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="132">
+      <c r="A37" s="135">
         <f>'Team Task Chart'!C19</f>
         <v>0</v>
       </c>
-      <c r="B37" s="138">
+      <c r="B37" s="141">
         <f>'Team Task Chart'!F19</f>
         <v>0</v>
       </c>
-      <c r="C37" s="139">
+      <c r="C37" s="142">
         <f>'Team Task Chart'!H19</f>
         <v>0</v>
       </c>
-      <c r="D37" s="132" t="s">
+      <c r="D37" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="132" t="str">
+      <c r="A38" s="135" t="str">
         <f>'Team Task Chart'!C20</f>
         <v>Arm Control</v>
       </c>
-      <c r="B38" s="138">
+      <c r="B38" s="141">
         <f>'Team Task Chart'!F20</f>
         <v>43072</v>
       </c>
-      <c r="C38" s="139">
+      <c r="C38" s="142">
         <f>'Team Task Chart'!H20</f>
         <v>0</v>
       </c>
-      <c r="D38" s="132" t="s">
+      <c r="D38" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="132" t="str">
+      <c r="A39" s="135" t="str">
         <f>'Team Task Chart'!C21</f>
         <v>Hardware Drivers</v>
       </c>
-      <c r="B39" s="138">
+      <c r="B39" s="141">
         <f>'Team Task Chart'!F21</f>
         <v>43072</v>
       </c>
-      <c r="C39" s="139">
+      <c r="C39" s="142">
         <f>'Team Task Chart'!H21</f>
         <v>0</v>
       </c>
-      <c r="D39" s="132" t="s">
+      <c r="D39" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="132" t="str">
+      <c r="A40" s="135" t="str">
         <f>'Team Task Chart'!C22</f>
         <v>Firmware Drivers</v>
       </c>
-      <c r="B40" s="138">
+      <c r="B40" s="141">
         <f>'Team Task Chart'!F22</f>
         <v>43072</v>
       </c>
-      <c r="C40" s="139">
+      <c r="C40" s="142">
         <f>'Team Task Chart'!H22</f>
         <v>0</v>
       </c>
-      <c r="D40" s="132" t="s">
+      <c r="D40" s="135" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="132" t="str">
+      <c r="A41" s="135" t="str">
         <f>'Team Task Chart'!C23</f>
         <v>Controls</v>
       </c>
-      <c r="B41" s="138">
+      <c r="B41" s="141">
         <f>'Team Task Chart'!F23</f>
         <v>43072</v>
       </c>
-      <c r="C41" s="139">
+      <c r="C41" s="142">
         <f>'Team Task Chart'!H23</f>
         <v>0</v>
       </c>
-      <c r="D41" s="132" t="s">
+      <c r="D41" s="135" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2462,7 +2462,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2563,228 +2563,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="89" t="s">
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="90"/>
-      <c r="AI2" s="90"/>
-      <c r="AJ2" s="90"/>
-      <c r="AK2" s="90"/>
-      <c r="AL2" s="91"/>
-      <c r="AM2" s="92" t="s">
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="104"/>
+      <c r="AE2" s="104"/>
+      <c r="AF2" s="104"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="104"/>
+      <c r="AI2" s="104"/>
+      <c r="AJ2" s="104"/>
+      <c r="AK2" s="104"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="93"/>
-      <c r="AO2" s="93"/>
-      <c r="AP2" s="93"/>
-      <c r="AQ2" s="93"/>
-      <c r="AR2" s="93"/>
-      <c r="AS2" s="93"/>
-      <c r="AT2" s="93"/>
-      <c r="AU2" s="93"/>
-      <c r="AV2" s="93"/>
-      <c r="AW2" s="93"/>
-      <c r="AX2" s="93"/>
-      <c r="AY2" s="93"/>
-      <c r="AZ2" s="93"/>
-      <c r="BA2" s="94"/>
-      <c r="BB2" s="95" t="s">
+      <c r="AN2" s="107"/>
+      <c r="AO2" s="107"/>
+      <c r="AP2" s="107"/>
+      <c r="AQ2" s="107"/>
+      <c r="AR2" s="107"/>
+      <c r="AS2" s="107"/>
+      <c r="AT2" s="107"/>
+      <c r="AU2" s="107"/>
+      <c r="AV2" s="107"/>
+      <c r="AW2" s="107"/>
+      <c r="AX2" s="107"/>
+      <c r="AY2" s="107"/>
+      <c r="AZ2" s="107"/>
+      <c r="BA2" s="108"/>
+      <c r="BB2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="96"/>
-      <c r="BD2" s="96"/>
-      <c r="BE2" s="96"/>
-      <c r="BF2" s="96"/>
-      <c r="BG2" s="96"/>
-      <c r="BH2" s="96"/>
-      <c r="BI2" s="96"/>
-      <c r="BJ2" s="96"/>
-      <c r="BK2" s="96"/>
-      <c r="BL2" s="96"/>
-      <c r="BM2" s="96"/>
-      <c r="BN2" s="96"/>
-      <c r="BO2" s="96"/>
-      <c r="BP2" s="97"/>
-      <c r="BQ2" s="95" t="s">
+      <c r="BC2" s="92"/>
+      <c r="BD2" s="92"/>
+      <c r="BE2" s="92"/>
+      <c r="BF2" s="92"/>
+      <c r="BG2" s="92"/>
+      <c r="BH2" s="92"/>
+      <c r="BI2" s="92"/>
+      <c r="BJ2" s="92"/>
+      <c r="BK2" s="92"/>
+      <c r="BL2" s="92"/>
+      <c r="BM2" s="92"/>
+      <c r="BN2" s="92"/>
+      <c r="BO2" s="92"/>
+      <c r="BP2" s="93"/>
+      <c r="BQ2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="96"/>
-      <c r="BS2" s="96"/>
-      <c r="BT2" s="96"/>
-      <c r="BU2" s="96"/>
-      <c r="BV2" s="96"/>
-      <c r="BW2" s="96"/>
-      <c r="BX2" s="96"/>
-      <c r="BY2" s="96"/>
-      <c r="BZ2" s="96"/>
-      <c r="CA2" s="96"/>
-      <c r="CB2" s="96"/>
-      <c r="CC2" s="96"/>
-      <c r="CD2" s="96"/>
-      <c r="CE2" s="97"/>
+      <c r="BR2" s="92"/>
+      <c r="BS2" s="92"/>
+      <c r="BT2" s="92"/>
+      <c r="BU2" s="92"/>
+      <c r="BV2" s="92"/>
+      <c r="BW2" s="92"/>
+      <c r="BX2" s="92"/>
+      <c r="BY2" s="92"/>
+      <c r="BZ2" s="92"/>
+      <c r="CA2" s="92"/>
+      <c r="CB2" s="92"/>
+      <c r="CC2" s="92"/>
+      <c r="CD2" s="92"/>
+      <c r="CE2" s="93"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="102" t="s">
+      <c r="G3" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="106" t="s">
+      <c r="H3" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="I3" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109" t="s">
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="109" t="s">
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="111" t="s">
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="119"/>
+      <c r="X3" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="112" t="s">
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="112"/>
-      <c r="AE3" s="112"/>
-      <c r="AF3" s="112"/>
-      <c r="AG3" s="112"/>
-      <c r="AH3" s="112" t="s">
+      <c r="AD3" s="95"/>
+      <c r="AE3" s="95"/>
+      <c r="AF3" s="95"/>
+      <c r="AG3" s="95"/>
+      <c r="AH3" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="112"/>
-      <c r="AJ3" s="112"/>
-      <c r="AK3" s="112"/>
-      <c r="AL3" s="113"/>
-      <c r="AM3" s="114" t="s">
+      <c r="AI3" s="95"/>
+      <c r="AJ3" s="95"/>
+      <c r="AK3" s="95"/>
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="115"/>
-      <c r="AO3" s="115"/>
-      <c r="AP3" s="115"/>
-      <c r="AQ3" s="115"/>
-      <c r="AR3" s="115" t="s">
+      <c r="AN3" s="98"/>
+      <c r="AO3" s="98"/>
+      <c r="AP3" s="98"/>
+      <c r="AQ3" s="98"/>
+      <c r="AR3" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="115"/>
-      <c r="AT3" s="115"/>
-      <c r="AU3" s="115"/>
-      <c r="AV3" s="115"/>
-      <c r="AW3" s="115" t="s">
+      <c r="AS3" s="98"/>
+      <c r="AT3" s="98"/>
+      <c r="AU3" s="98"/>
+      <c r="AV3" s="98"/>
+      <c r="AW3" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="115"/>
-      <c r="AY3" s="115"/>
-      <c r="AZ3" s="115"/>
-      <c r="BA3" s="116"/>
-      <c r="BB3" s="104" t="s">
+      <c r="AX3" s="98"/>
+      <c r="AY3" s="98"/>
+      <c r="AZ3" s="98"/>
+      <c r="BA3" s="99"/>
+      <c r="BB3" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="105"/>
-      <c r="BD3" s="105"/>
-      <c r="BE3" s="105"/>
-      <c r="BF3" s="105"/>
-      <c r="BG3" s="105" t="s">
+      <c r="BC3" s="89"/>
+      <c r="BD3" s="89"/>
+      <c r="BE3" s="89"/>
+      <c r="BF3" s="89"/>
+      <c r="BG3" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="105"/>
-      <c r="BI3" s="105"/>
-      <c r="BJ3" s="105"/>
-      <c r="BK3" s="105"/>
-      <c r="BL3" s="105" t="s">
+      <c r="BH3" s="89"/>
+      <c r="BI3" s="89"/>
+      <c r="BJ3" s="89"/>
+      <c r="BK3" s="89"/>
+      <c r="BL3" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="105"/>
-      <c r="BN3" s="105"/>
-      <c r="BO3" s="105"/>
-      <c r="BP3" s="117"/>
-      <c r="BQ3" s="104" t="s">
+      <c r="BM3" s="89"/>
+      <c r="BN3" s="89"/>
+      <c r="BO3" s="89"/>
+      <c r="BP3" s="90"/>
+      <c r="BQ3" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="105"/>
-      <c r="BS3" s="105"/>
-      <c r="BT3" s="105"/>
-      <c r="BU3" s="105"/>
-      <c r="BV3" s="105" t="s">
+      <c r="BR3" s="89"/>
+      <c r="BS3" s="89"/>
+      <c r="BT3" s="89"/>
+      <c r="BU3" s="89"/>
+      <c r="BV3" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="105"/>
-      <c r="BX3" s="105"/>
-      <c r="BY3" s="105"/>
-      <c r="BZ3" s="105"/>
-      <c r="CA3" s="105" t="s">
+      <c r="BW3" s="89"/>
+      <c r="BX3" s="89"/>
+      <c r="BY3" s="89"/>
+      <c r="BZ3" s="89"/>
+      <c r="CA3" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="105"/>
-      <c r="CC3" s="105"/>
-      <c r="CD3" s="105"/>
-      <c r="CE3" s="117"/>
+      <c r="CB3" s="89"/>
+      <c r="CC3" s="89"/>
+      <c r="CD3" s="89"/>
+      <c r="CE3" s="90"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="99"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="107"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="116"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="32">
         <f>(2/3)*H6+(1/3)*H7</f>
-        <v>0.75</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="34"/>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="42">
-        <v>0.25</v>
+        <v>0.7</v>
       </c>
       <c r="I7" s="51" t="s">
         <v>77</v>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
@@ -3573,11 +3573,21 @@
       <c r="AV9" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="AW9" s="48"/>
-      <c r="AX9" s="48"/>
-      <c r="AY9" s="48"/>
-      <c r="AZ9" s="48"/>
-      <c r="BA9" s="54"/>
+      <c r="AW9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA9" s="54" t="s">
+        <v>77</v>
+      </c>
       <c r="BB9" s="55"/>
       <c r="BC9" s="48"/>
       <c r="BD9" s="48"/>
@@ -3626,7 +3636,7 @@
       </c>
       <c r="G10" s="41"/>
       <c r="H10" s="42">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="44"/>
@@ -3698,11 +3708,21 @@
       <c r="AV10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="AW10" s="52"/>
-      <c r="AX10" s="52"/>
-      <c r="AY10" s="52"/>
-      <c r="AZ10" s="52"/>
-      <c r="BA10" s="53"/>
+      <c r="AW10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA10" s="53" t="s">
+        <v>77</v>
+      </c>
       <c r="BB10" s="51"/>
       <c r="BC10" s="52"/>
       <c r="BD10" s="52"/>
@@ -3751,7 +3771,7 @@
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="42">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="44"/>
@@ -3820,29 +3840,39 @@
       <c r="AU11" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="AV11" s="140" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW11" s="140"/>
-      <c r="AX11" s="140"/>
-      <c r="AY11" s="140"/>
-      <c r="AZ11" s="140"/>
-      <c r="BA11" s="141"/>
-      <c r="BB11" s="142"/>
-      <c r="BC11" s="140"/>
-      <c r="BD11" s="140"/>
-      <c r="BE11" s="140"/>
-      <c r="BF11" s="140"/>
-      <c r="BG11" s="140"/>
-      <c r="BH11" s="140"/>
-      <c r="BI11" s="140"/>
-      <c r="BJ11" s="140"/>
-      <c r="BK11" s="140"/>
-      <c r="BL11" s="140"/>
-      <c r="BM11" s="140"/>
-      <c r="BN11" s="140"/>
-      <c r="BO11" s="140"/>
-      <c r="BP11" s="141"/>
+      <c r="AV11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA11" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB11" s="86"/>
+      <c r="BC11" s="84"/>
+      <c r="BD11" s="84"/>
+      <c r="BE11" s="84"/>
+      <c r="BF11" s="84"/>
+      <c r="BG11" s="84"/>
+      <c r="BH11" s="84"/>
+      <c r="BI11" s="84"/>
+      <c r="BJ11" s="84"/>
+      <c r="BK11" s="84"/>
+      <c r="BL11" s="84"/>
+      <c r="BM11" s="84"/>
+      <c r="BN11" s="84"/>
+      <c r="BO11" s="84"/>
+      <c r="BP11" s="85"/>
       <c r="BQ11" s="43"/>
       <c r="BR11" s="44"/>
       <c r="BS11" s="44"/>
@@ -3876,7 +3906,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -3948,11 +3978,21 @@
       <c r="AV12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="AW12" s="59"/>
-      <c r="AX12" s="59"/>
-      <c r="AY12" s="59"/>
-      <c r="AZ12" s="59"/>
-      <c r="BA12" s="60"/>
+      <c r="AW12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA12" s="60" t="s">
+        <v>77</v>
+      </c>
       <c r="BB12" s="61"/>
       <c r="BC12" s="59"/>
       <c r="BD12" s="59"/>
@@ -4001,7 +4041,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -4073,11 +4113,21 @@
       <c r="AV13" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="AW13" s="62"/>
-      <c r="AX13" s="62"/>
-      <c r="AY13" s="62"/>
-      <c r="AZ13" s="62"/>
-      <c r="BA13" s="63"/>
+      <c r="AW13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA13" s="63" t="s">
+        <v>77</v>
+      </c>
       <c r="BB13" s="64"/>
       <c r="BC13" s="62"/>
       <c r="BD13" s="62"/>
@@ -5729,17 +5779,6 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5756,6 +5795,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -5834,7 +5884,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5923,7 +5973,9 @@
       <c r="I2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -5933,7 +5985,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -5967,7 +6019,9 @@
       <c r="I3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -5977,7 +6031,7 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="7">
         <f t="shared" ref="R3:R9" si="0">COUNTIF(D3:Q3,"P")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -6011,7 +6065,9 @@
       <c r="I4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -6021,7 +6077,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6055,7 +6111,9 @@
       <c r="I5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -6065,7 +6123,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1">
@@ -6096,7 +6154,9 @@
       <c r="I6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -6106,7 +6166,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
Week 10 Update for E-Team
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -1170,116 +1170,8 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1290,40 +1182,148 @@
     <xf numFmtId="0" fontId="19" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,174 +1705,174 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="88"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="88"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
+      <c r="A8" s="105"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="88"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1889,512 +1889,512 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="122" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="122"/>
+    <col min="1" max="1" width="32.875" style="88" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="88"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="87" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="125" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="123" t="s">
+    <row r="2" spans="1:5" s="89" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A2" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="129"/>
+      <c r="C4" s="109"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="128" t="s">
+      <c r="A5" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="129"/>
+      <c r="C5" s="109"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="129"/>
+      <c r="C6" s="109"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="128" t="s">
+      <c r="A7" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="130">
-        <v>9</v>
+      <c r="B7" s="93">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="94" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="133">
+      <c r="B9" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="132" t="s">
+      <c r="A10" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="133">
+      <c r="B10" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="131" t="s">
+      <c r="A11" s="94" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="135" t="s">
+      <c r="B12" s="98" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="136"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="137"/>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
+      <c r="A15" s="106"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="137"/>
-      <c r="B16" s="137"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="137"/>
-      <c r="E16" s="137"/>
+      <c r="A16" s="106"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="137"/>
-      <c r="B17" s="137"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
+      <c r="A17" s="106"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="137"/>
-      <c r="B18" s="137"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="137"/>
-      <c r="B19" s="137"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
+      <c r="A19" s="106"/>
+      <c r="B19" s="106"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="137"/>
-      <c r="B20" s="137"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="138" t="s">
+      <c r="A21" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="139"/>
-      <c r="C21" s="139"/>
-      <c r="D21" s="139"/>
-      <c r="E21" s="139"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="140" t="s">
+      <c r="A22" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="140" t="s">
+      <c r="D22" s="101" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="135" t="str">
+      <c r="A23" s="98" t="str">
         <f>'Team Task Chart'!C5</f>
         <v>Setting Up</v>
       </c>
-      <c r="B23" s="141">
+      <c r="B23" s="102">
         <f>'Team Task Chart'!F5</f>
         <v>42984</v>
       </c>
-      <c r="C23" s="142">
+      <c r="C23" s="103">
         <f>'Team Task Chart'!H5</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="D23" s="135" t="s">
+      <c r="D23" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="135" t="str">
+      <c r="A24" s="98" t="str">
         <f>'Team Task Chart'!C6</f>
         <v>Assign Roles (Domain Areas)</v>
       </c>
-      <c r="B24" s="141">
+      <c r="B24" s="102">
         <f>'Team Task Chart'!F6</f>
         <v>42998</v>
       </c>
-      <c r="C24" s="142">
+      <c r="C24" s="103">
         <f>'Team Task Chart'!H6</f>
         <v>1</v>
       </c>
-      <c r="D24" s="135" t="s">
+      <c r="D24" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="135" t="str">
+      <c r="A25" s="98" t="str">
         <f>'Team Task Chart'!C7</f>
         <v>Get an E-Box from mechanical</v>
       </c>
-      <c r="B25" s="141">
+      <c r="B25" s="102">
         <f>'Team Task Chart'!F7</f>
         <v>43005</v>
       </c>
-      <c r="C25" s="142">
+      <c r="C25" s="103">
         <f>'Team Task Chart'!H7</f>
         <v>0.7</v>
       </c>
-      <c r="D25" s="135" t="s">
+      <c r="D25" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="135" t="str">
+      <c r="A26" s="98" t="str">
         <f>'Team Task Chart'!C8</f>
         <v>Drive System</v>
       </c>
-      <c r="B26" s="141">
+      <c r="B26" s="102">
         <f>'Team Task Chart'!F8</f>
         <v>43051</v>
       </c>
-      <c r="C26" s="142">
+      <c r="C26" s="103">
         <f>'Team Task Chart'!H8</f>
         <v>0.7</v>
       </c>
-      <c r="D26" s="135" t="s">
+      <c r="D26" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="135" t="str">
+      <c r="A27" s="98" t="str">
         <f>'Team Task Chart'!C9</f>
         <v>Do Research in needed Domains</v>
       </c>
-      <c r="B27" s="141">
+      <c r="B27" s="102">
         <f>'Team Task Chart'!F9</f>
         <v>43051</v>
       </c>
-      <c r="C27" s="142">
+      <c r="C27" s="103">
         <f>'Team Task Chart'!H9</f>
         <v>0.9</v>
       </c>
-      <c r="D27" s="135" t="s">
+      <c r="D27" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="135" t="str">
+      <c r="A28" s="98" t="str">
         <f>'Team Task Chart'!C10</f>
         <v>Power Systems</v>
       </c>
-      <c r="B28" s="141">
+      <c r="B28" s="102">
         <f>'Team Task Chart'!F10</f>
         <v>43051</v>
       </c>
-      <c r="C28" s="142">
+      <c r="C28" s="103">
         <f>'Team Task Chart'!H10</f>
         <v>0.6</v>
       </c>
-      <c r="D28" s="135" t="s">
+      <c r="D28" s="98" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="135" t="str">
+      <c r="A29" s="98" t="str">
         <f>'Team Task Chart'!C11</f>
         <v>Control Systems</v>
       </c>
-      <c r="B29" s="141">
+      <c r="B29" s="102">
         <f>'Team Task Chart'!F11</f>
         <v>43051</v>
       </c>
-      <c r="C29" s="142">
+      <c r="C29" s="103">
         <f>'Team Task Chart'!H11</f>
-        <v>0.95</v>
-      </c>
-      <c r="D29" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="135" t="str">
+      <c r="A30" s="98" t="str">
         <f>'Team Task Chart'!C12</f>
         <v>Firmware</v>
       </c>
-      <c r="B30" s="141">
+      <c r="B30" s="102">
         <f>'Team Task Chart'!F12</f>
         <v>43051</v>
       </c>
-      <c r="C30" s="142">
+      <c r="C30" s="103">
         <f>'Team Task Chart'!H12</f>
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="135" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="D30" s="98" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="135" t="str">
+      <c r="A31" s="98" t="str">
         <f>'Team Task Chart'!C13</f>
         <v>Circuits/CAD</v>
       </c>
-      <c r="B31" s="141">
+      <c r="B31" s="102">
         <f>'Team Task Chart'!F13</f>
         <v>43051</v>
       </c>
-      <c r="C31" s="142">
+      <c r="C31" s="103">
         <f>'Team Task Chart'!H13</f>
-        <v>0.4</v>
-      </c>
-      <c r="D31" s="135" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="98" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="135">
+      <c r="A32" s="98">
         <f>'Team Task Chart'!C14</f>
         <v>0</v>
       </c>
-      <c r="B32" s="141">
+      <c r="B32" s="102">
         <f>'Team Task Chart'!F14</f>
         <v>0</v>
       </c>
-      <c r="C32" s="142">
+      <c r="C32" s="103">
         <f>'Team Task Chart'!H14</f>
         <v>0</v>
       </c>
-      <c r="D32" s="135" t="s">
+      <c r="D32" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="135" t="str">
+      <c r="A33" s="98" t="str">
         <f>'Team Task Chart'!C15</f>
         <v>Refinement</v>
       </c>
-      <c r="B33" s="141">
+      <c r="B33" s="102">
         <f>'Team Task Chart'!F15</f>
         <v>43066</v>
       </c>
-      <c r="C33" s="142">
+      <c r="C33" s="103">
         <f>'Team Task Chart'!H15</f>
         <v>0</v>
       </c>
-      <c r="D33" s="135" t="s">
+      <c r="D33" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="135" t="str">
+      <c r="A34" s="98" t="str">
         <f>'Team Task Chart'!C16</f>
         <v>Firmware</v>
       </c>
-      <c r="B34" s="141">
+      <c r="B34" s="102">
         <f>'Team Task Chart'!F16</f>
         <v>43066</v>
       </c>
-      <c r="C34" s="142">
+      <c r="C34" s="103">
         <f>'Team Task Chart'!H16</f>
         <v>0</v>
       </c>
-      <c r="D34" s="135" t="s">
+      <c r="D34" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="135" t="str">
+      <c r="A35" s="98" t="str">
         <f>'Team Task Chart'!C17</f>
         <v>Circuits</v>
       </c>
-      <c r="B35" s="141">
+      <c r="B35" s="102">
         <f>'Team Task Chart'!F17</f>
         <v>43066</v>
       </c>
-      <c r="C35" s="142">
+      <c r="C35" s="103">
         <f>'Team Task Chart'!H17</f>
         <v>0</v>
       </c>
-      <c r="D35" s="135" t="s">
+      <c r="D35" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="135" t="str">
+      <c r="A36" s="98" t="str">
         <f>'Team Task Chart'!C18</f>
         <v>Controls</v>
       </c>
-      <c r="B36" s="141">
+      <c r="B36" s="102">
         <f>'Team Task Chart'!F18</f>
         <v>43066</v>
       </c>
-      <c r="C36" s="142">
+      <c r="C36" s="103">
         <f>'Team Task Chart'!H18</f>
         <v>0</v>
       </c>
-      <c r="D36" s="135" t="s">
+      <c r="D36" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="135">
+      <c r="A37" s="98">
         <f>'Team Task Chart'!C19</f>
         <v>0</v>
       </c>
-      <c r="B37" s="141">
+      <c r="B37" s="102">
         <f>'Team Task Chart'!F19</f>
         <v>0</v>
       </c>
-      <c r="C37" s="142">
+      <c r="C37" s="103">
         <f>'Team Task Chart'!H19</f>
         <v>0</v>
       </c>
-      <c r="D37" s="135" t="s">
+      <c r="D37" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="135" t="str">
+      <c r="A38" s="98" t="str">
         <f>'Team Task Chart'!C20</f>
         <v>Arm Control</v>
       </c>
-      <c r="B38" s="141">
+      <c r="B38" s="102">
         <f>'Team Task Chart'!F20</f>
         <v>43072</v>
       </c>
-      <c r="C38" s="142">
+      <c r="C38" s="103">
         <f>'Team Task Chart'!H20</f>
         <v>0</v>
       </c>
-      <c r="D38" s="135" t="s">
+      <c r="D38" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="135" t="str">
+      <c r="A39" s="98" t="str">
         <f>'Team Task Chart'!C21</f>
         <v>Hardware Drivers</v>
       </c>
-      <c r="B39" s="141">
+      <c r="B39" s="102">
         <f>'Team Task Chart'!F21</f>
         <v>43072</v>
       </c>
-      <c r="C39" s="142">
+      <c r="C39" s="103">
         <f>'Team Task Chart'!H21</f>
         <v>0</v>
       </c>
-      <c r="D39" s="135" t="s">
+      <c r="D39" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="135" t="str">
+      <c r="A40" s="98" t="str">
         <f>'Team Task Chart'!C22</f>
         <v>Firmware Drivers</v>
       </c>
-      <c r="B40" s="141">
+      <c r="B40" s="102">
         <f>'Team Task Chart'!F22</f>
         <v>43072</v>
       </c>
-      <c r="C40" s="142">
+      <c r="C40" s="103">
         <f>'Team Task Chart'!H22</f>
         <v>0</v>
       </c>
-      <c r="D40" s="135" t="s">
+      <c r="D40" s="98" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="135" t="str">
+      <c r="A41" s="98" t="str">
         <f>'Team Task Chart'!C23</f>
         <v>Controls</v>
       </c>
-      <c r="B41" s="141">
+      <c r="B41" s="102">
         <f>'Team Task Chart'!F23</f>
         <v>43072</v>
       </c>
-      <c r="C41" s="142">
+      <c r="C41" s="103">
         <f>'Team Task Chart'!H23</f>
         <v>0</v>
       </c>
-      <c r="D41" s="135" t="s">
+      <c r="D41" s="98" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2460,9 +2460,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="BG13" sqref="BG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2563,228 +2563,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="103" t="s">
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="104"/>
-      <c r="AI2" s="104"/>
-      <c r="AJ2" s="104"/>
-      <c r="AK2" s="104"/>
-      <c r="AL2" s="105"/>
-      <c r="AM2" s="106" t="s">
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
+      <c r="AA2" s="115"/>
+      <c r="AB2" s="115"/>
+      <c r="AC2" s="115"/>
+      <c r="AD2" s="115"/>
+      <c r="AE2" s="115"/>
+      <c r="AF2" s="115"/>
+      <c r="AG2" s="115"/>
+      <c r="AH2" s="115"/>
+      <c r="AI2" s="115"/>
+      <c r="AJ2" s="115"/>
+      <c r="AK2" s="115"/>
+      <c r="AL2" s="116"/>
+      <c r="AM2" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="107"/>
-      <c r="AO2" s="107"/>
-      <c r="AP2" s="107"/>
-      <c r="AQ2" s="107"/>
-      <c r="AR2" s="107"/>
-      <c r="AS2" s="107"/>
-      <c r="AT2" s="107"/>
-      <c r="AU2" s="107"/>
-      <c r="AV2" s="107"/>
-      <c r="AW2" s="107"/>
-      <c r="AX2" s="107"/>
-      <c r="AY2" s="107"/>
-      <c r="AZ2" s="107"/>
-      <c r="BA2" s="108"/>
-      <c r="BB2" s="91" t="s">
+      <c r="AN2" s="118"/>
+      <c r="AO2" s="118"/>
+      <c r="AP2" s="118"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="118"/>
+      <c r="AS2" s="118"/>
+      <c r="AT2" s="118"/>
+      <c r="AU2" s="118"/>
+      <c r="AV2" s="118"/>
+      <c r="AW2" s="118"/>
+      <c r="AX2" s="118"/>
+      <c r="AY2" s="118"/>
+      <c r="AZ2" s="118"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="92"/>
-      <c r="BD2" s="92"/>
-      <c r="BE2" s="92"/>
-      <c r="BF2" s="92"/>
-      <c r="BG2" s="92"/>
-      <c r="BH2" s="92"/>
-      <c r="BI2" s="92"/>
-      <c r="BJ2" s="92"/>
-      <c r="BK2" s="92"/>
-      <c r="BL2" s="92"/>
-      <c r="BM2" s="92"/>
-      <c r="BN2" s="92"/>
-      <c r="BO2" s="92"/>
-      <c r="BP2" s="93"/>
-      <c r="BQ2" s="91" t="s">
+      <c r="BC2" s="121"/>
+      <c r="BD2" s="121"/>
+      <c r="BE2" s="121"/>
+      <c r="BF2" s="121"/>
+      <c r="BG2" s="121"/>
+      <c r="BH2" s="121"/>
+      <c r="BI2" s="121"/>
+      <c r="BJ2" s="121"/>
+      <c r="BK2" s="121"/>
+      <c r="BL2" s="121"/>
+      <c r="BM2" s="121"/>
+      <c r="BN2" s="121"/>
+      <c r="BO2" s="121"/>
+      <c r="BP2" s="122"/>
+      <c r="BQ2" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="92"/>
-      <c r="BS2" s="92"/>
-      <c r="BT2" s="92"/>
-      <c r="BU2" s="92"/>
-      <c r="BV2" s="92"/>
-      <c r="BW2" s="92"/>
-      <c r="BX2" s="92"/>
-      <c r="BY2" s="92"/>
-      <c r="BZ2" s="92"/>
-      <c r="CA2" s="92"/>
-      <c r="CB2" s="92"/>
-      <c r="CC2" s="92"/>
-      <c r="CD2" s="92"/>
-      <c r="CE2" s="93"/>
+      <c r="BR2" s="121"/>
+      <c r="BS2" s="121"/>
+      <c r="BT2" s="121"/>
+      <c r="BU2" s="121"/>
+      <c r="BV2" s="121"/>
+      <c r="BW2" s="121"/>
+      <c r="BX2" s="121"/>
+      <c r="BY2" s="121"/>
+      <c r="BZ2" s="121"/>
+      <c r="CA2" s="121"/>
+      <c r="CB2" s="121"/>
+      <c r="CC2" s="121"/>
+      <c r="CD2" s="121"/>
+      <c r="CE2" s="122"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="113" t="s">
+      <c r="G3" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118" t="s">
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118" t="s">
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="119"/>
-      <c r="X3" s="120" t="s">
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95" t="s">
+      <c r="Y3" s="137"/>
+      <c r="Z3" s="137"/>
+      <c r="AA3" s="137"/>
+      <c r="AB3" s="137"/>
+      <c r="AC3" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="95"/>
-      <c r="AE3" s="95"/>
-      <c r="AF3" s="95"/>
-      <c r="AG3" s="95"/>
-      <c r="AH3" s="95" t="s">
+      <c r="AD3" s="137"/>
+      <c r="AE3" s="137"/>
+      <c r="AF3" s="137"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="95"/>
-      <c r="AJ3" s="95"/>
-      <c r="AK3" s="95"/>
-      <c r="AL3" s="96"/>
-      <c r="AM3" s="97" t="s">
+      <c r="AI3" s="137"/>
+      <c r="AJ3" s="137"/>
+      <c r="AK3" s="137"/>
+      <c r="AL3" s="138"/>
+      <c r="AM3" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="98"/>
-      <c r="AO3" s="98"/>
-      <c r="AP3" s="98"/>
-      <c r="AQ3" s="98"/>
-      <c r="AR3" s="98" t="s">
+      <c r="AN3" s="140"/>
+      <c r="AO3" s="140"/>
+      <c r="AP3" s="140"/>
+      <c r="AQ3" s="140"/>
+      <c r="AR3" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="98"/>
-      <c r="AT3" s="98"/>
-      <c r="AU3" s="98"/>
-      <c r="AV3" s="98"/>
-      <c r="AW3" s="98" t="s">
+      <c r="AS3" s="140"/>
+      <c r="AT3" s="140"/>
+      <c r="AU3" s="140"/>
+      <c r="AV3" s="140"/>
+      <c r="AW3" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="98"/>
-      <c r="AY3" s="98"/>
-      <c r="AZ3" s="98"/>
-      <c r="BA3" s="99"/>
-      <c r="BB3" s="94" t="s">
+      <c r="AX3" s="140"/>
+      <c r="AY3" s="140"/>
+      <c r="AZ3" s="140"/>
+      <c r="BA3" s="141"/>
+      <c r="BB3" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="89"/>
-      <c r="BD3" s="89"/>
-      <c r="BE3" s="89"/>
-      <c r="BF3" s="89"/>
-      <c r="BG3" s="89" t="s">
+      <c r="BC3" s="130"/>
+      <c r="BD3" s="130"/>
+      <c r="BE3" s="130"/>
+      <c r="BF3" s="130"/>
+      <c r="BG3" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="89"/>
-      <c r="BI3" s="89"/>
-      <c r="BJ3" s="89"/>
-      <c r="BK3" s="89"/>
-      <c r="BL3" s="89" t="s">
+      <c r="BH3" s="130"/>
+      <c r="BI3" s="130"/>
+      <c r="BJ3" s="130"/>
+      <c r="BK3" s="130"/>
+      <c r="BL3" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="89"/>
-      <c r="BN3" s="89"/>
-      <c r="BO3" s="89"/>
-      <c r="BP3" s="90"/>
-      <c r="BQ3" s="94" t="s">
+      <c r="BM3" s="130"/>
+      <c r="BN3" s="130"/>
+      <c r="BO3" s="130"/>
+      <c r="BP3" s="142"/>
+      <c r="BQ3" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="89"/>
-      <c r="BS3" s="89"/>
-      <c r="BT3" s="89"/>
-      <c r="BU3" s="89"/>
-      <c r="BV3" s="89" t="s">
+      <c r="BR3" s="130"/>
+      <c r="BS3" s="130"/>
+      <c r="BT3" s="130"/>
+      <c r="BU3" s="130"/>
+      <c r="BV3" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="89"/>
-      <c r="BX3" s="89"/>
-      <c r="BY3" s="89"/>
-      <c r="BZ3" s="89"/>
-      <c r="CA3" s="89" t="s">
+      <c r="BW3" s="130"/>
+      <c r="BX3" s="130"/>
+      <c r="BY3" s="130"/>
+      <c r="BZ3" s="130"/>
+      <c r="CA3" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="89"/>
-      <c r="CC3" s="89"/>
-      <c r="CD3" s="89"/>
-      <c r="CE3" s="90"/>
+      <c r="CB3" s="130"/>
+      <c r="CC3" s="130"/>
+      <c r="CD3" s="130"/>
+      <c r="CE3" s="142"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="110"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="116"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="132"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3588,11 +3588,21 @@
       <c r="BA9" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="BB9" s="55"/>
-      <c r="BC9" s="48"/>
-      <c r="BD9" s="48"/>
-      <c r="BE9" s="48"/>
-      <c r="BF9" s="48"/>
+      <c r="BB9" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF9" s="48" t="s">
+        <v>77</v>
+      </c>
       <c r="BG9" s="48"/>
       <c r="BH9" s="48"/>
       <c r="BI9" s="48"/>
@@ -3723,11 +3733,21 @@
       <c r="BA10" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="BB10" s="51"/>
-      <c r="BC10" s="52"/>
-      <c r="BD10" s="52"/>
-      <c r="BE10" s="52"/>
-      <c r="BF10" s="52"/>
+      <c r="BB10" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF10" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="BG10" s="52"/>
       <c r="BH10" s="52"/>
       <c r="BI10" s="52"/>
@@ -3771,7 +3791,7 @@
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="42">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="44"/>
@@ -3858,11 +3878,21 @@
       <c r="BA11" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="BB11" s="86"/>
-      <c r="BC11" s="84"/>
-      <c r="BD11" s="84"/>
-      <c r="BE11" s="84"/>
-      <c r="BF11" s="84"/>
+      <c r="BB11" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF11" s="84" t="s">
+        <v>77</v>
+      </c>
       <c r="BG11" s="84"/>
       <c r="BH11" s="84"/>
       <c r="BI11" s="84"/>
@@ -3906,7 +3936,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -3993,11 +4023,21 @@
       <c r="BA12" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="BB12" s="61"/>
-      <c r="BC12" s="59"/>
-      <c r="BD12" s="59"/>
-      <c r="BE12" s="59"/>
-      <c r="BF12" s="59"/>
+      <c r="BB12" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF12" s="59" t="s">
+        <v>77</v>
+      </c>
       <c r="BG12" s="59"/>
       <c r="BH12" s="59"/>
       <c r="BI12" s="59"/>
@@ -4041,7 +4081,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -4128,11 +4168,21 @@
       <c r="BA13" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="BB13" s="64"/>
-      <c r="BC13" s="62"/>
-      <c r="BD13" s="62"/>
-      <c r="BE13" s="62"/>
-      <c r="BF13" s="62"/>
+      <c r="BB13" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF13" s="62" t="s">
+        <v>77</v>
+      </c>
       <c r="BG13" s="62"/>
       <c r="BH13" s="62"/>
       <c r="BI13" s="62"/>
@@ -5779,6 +5829,17 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5795,17 +5856,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -5884,7 +5934,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5976,7 +6026,9 @@
       <c r="J2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -5985,7 +6037,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -6022,7 +6074,9 @@
       <c r="J3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="8"/>
+      <c r="K3" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6068,7 +6122,9 @@
       <c r="J4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -6077,7 +6133,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6114,7 +6170,9 @@
       <c r="J5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -6123,7 +6181,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1">
@@ -6157,7 +6215,9 @@
       <c r="J6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -6166,7 +6226,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
E-Team report week 10
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>The team is still strugling with getting power to the motors. We don't have information on obtaining batteries yet, and haven't completed motor power consumption calculations (started). I've been sick, so some of the component selection has not gotten as far as I wanted.</t>
+    <t>We are assembling the E-Box, but we still aren't sure of our power systems. I've reached out to a couple EE advisor options, but haven't heard back. I've been informed that the mechanical components for the suspension are not yet complete, and as such, we will proibably not be driving by our milestone. We plan to have the control system working.</t>
   </si>
 </sst>
 </file>
@@ -998,7 +998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1228,6 +1228,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1255,15 +1288,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,12 +1306,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1306,23 +1324,8 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1889,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2002,7 +2005,7 @@
       <c r="D13" s="110"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="143" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="106"/>
@@ -2460,9 +2463,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BG13" sqref="BG13"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2563,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="111" t="s">
+      <c r="I2" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="114" t="s">
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="124"/>
+      <c r="X2" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="115"/>
-      <c r="AF2" s="115"/>
-      <c r="AG2" s="115"/>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="116"/>
-      <c r="AM2" s="117" t="s">
+      <c r="Y2" s="126"/>
+      <c r="Z2" s="126"/>
+      <c r="AA2" s="126"/>
+      <c r="AB2" s="126"/>
+      <c r="AC2" s="126"/>
+      <c r="AD2" s="126"/>
+      <c r="AE2" s="126"/>
+      <c r="AF2" s="126"/>
+      <c r="AG2" s="126"/>
+      <c r="AH2" s="126"/>
+      <c r="AI2" s="126"/>
+      <c r="AJ2" s="126"/>
+      <c r="AK2" s="126"/>
+      <c r="AL2" s="127"/>
+      <c r="AM2" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="118"/>
-      <c r="AO2" s="118"/>
-      <c r="AP2" s="118"/>
-      <c r="AQ2" s="118"/>
-      <c r="AR2" s="118"/>
-      <c r="AS2" s="118"/>
-      <c r="AT2" s="118"/>
-      <c r="AU2" s="118"/>
-      <c r="AV2" s="118"/>
-      <c r="AW2" s="118"/>
-      <c r="AX2" s="118"/>
-      <c r="AY2" s="118"/>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="119"/>
-      <c r="BB2" s="120" t="s">
+      <c r="AN2" s="129"/>
+      <c r="AO2" s="129"/>
+      <c r="AP2" s="129"/>
+      <c r="AQ2" s="129"/>
+      <c r="AR2" s="129"/>
+      <c r="AS2" s="129"/>
+      <c r="AT2" s="129"/>
+      <c r="AU2" s="129"/>
+      <c r="AV2" s="129"/>
+      <c r="AW2" s="129"/>
+      <c r="AX2" s="129"/>
+      <c r="AY2" s="129"/>
+      <c r="AZ2" s="129"/>
+      <c r="BA2" s="130"/>
+      <c r="BB2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="121"/>
-      <c r="BD2" s="121"/>
-      <c r="BE2" s="121"/>
-      <c r="BF2" s="121"/>
-      <c r="BG2" s="121"/>
-      <c r="BH2" s="121"/>
-      <c r="BI2" s="121"/>
-      <c r="BJ2" s="121"/>
-      <c r="BK2" s="121"/>
-      <c r="BL2" s="121"/>
-      <c r="BM2" s="121"/>
-      <c r="BN2" s="121"/>
-      <c r="BO2" s="121"/>
-      <c r="BP2" s="122"/>
-      <c r="BQ2" s="120" t="s">
+      <c r="BC2" s="114"/>
+      <c r="BD2" s="114"/>
+      <c r="BE2" s="114"/>
+      <c r="BF2" s="114"/>
+      <c r="BG2" s="114"/>
+      <c r="BH2" s="114"/>
+      <c r="BI2" s="114"/>
+      <c r="BJ2" s="114"/>
+      <c r="BK2" s="114"/>
+      <c r="BL2" s="114"/>
+      <c r="BM2" s="114"/>
+      <c r="BN2" s="114"/>
+      <c r="BO2" s="114"/>
+      <c r="BP2" s="115"/>
+      <c r="BQ2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="121"/>
-      <c r="BS2" s="121"/>
-      <c r="BT2" s="121"/>
-      <c r="BU2" s="121"/>
-      <c r="BV2" s="121"/>
-      <c r="BW2" s="121"/>
-      <c r="BX2" s="121"/>
-      <c r="BY2" s="121"/>
-      <c r="BZ2" s="121"/>
-      <c r="CA2" s="121"/>
-      <c r="CB2" s="121"/>
-      <c r="CC2" s="121"/>
-      <c r="CD2" s="121"/>
-      <c r="CE2" s="122"/>
+      <c r="BR2" s="114"/>
+      <c r="BS2" s="114"/>
+      <c r="BT2" s="114"/>
+      <c r="BU2" s="114"/>
+      <c r="BV2" s="114"/>
+      <c r="BW2" s="114"/>
+      <c r="BX2" s="114"/>
+      <c r="BY2" s="114"/>
+      <c r="BZ2" s="114"/>
+      <c r="CA2" s="114"/>
+      <c r="CB2" s="114"/>
+      <c r="CC2" s="114"/>
+      <c r="CD2" s="114"/>
+      <c r="CE2" s="115"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="127" t="s">
+      <c r="E3" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="127" t="s">
+      <c r="F3" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="G3" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="133" t="s">
+      <c r="I3" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134" t="s">
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134" t="s">
+      <c r="O3" s="140"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="136" t="s">
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="137"/>
-      <c r="Z3" s="137"/>
-      <c r="AA3" s="137"/>
-      <c r="AB3" s="137"/>
-      <c r="AC3" s="137" t="s">
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="137"/>
-      <c r="AE3" s="137"/>
-      <c r="AF3" s="137"/>
-      <c r="AG3" s="137"/>
-      <c r="AH3" s="137" t="s">
+      <c r="AD3" s="117"/>
+      <c r="AE3" s="117"/>
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
+      <c r="AH3" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="137"/>
-      <c r="AJ3" s="137"/>
-      <c r="AK3" s="137"/>
-      <c r="AL3" s="138"/>
-      <c r="AM3" s="139" t="s">
+      <c r="AI3" s="117"/>
+      <c r="AJ3" s="117"/>
+      <c r="AK3" s="117"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="140"/>
-      <c r="AO3" s="140"/>
-      <c r="AP3" s="140"/>
-      <c r="AQ3" s="140"/>
-      <c r="AR3" s="140" t="s">
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="120"/>
+      <c r="AP3" s="120"/>
+      <c r="AQ3" s="120"/>
+      <c r="AR3" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="140"/>
-      <c r="AT3" s="140"/>
-      <c r="AU3" s="140"/>
-      <c r="AV3" s="140"/>
-      <c r="AW3" s="140" t="s">
+      <c r="AS3" s="120"/>
+      <c r="AT3" s="120"/>
+      <c r="AU3" s="120"/>
+      <c r="AV3" s="120"/>
+      <c r="AW3" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="140"/>
-      <c r="AY3" s="140"/>
-      <c r="AZ3" s="140"/>
-      <c r="BA3" s="141"/>
-      <c r="BB3" s="129" t="s">
+      <c r="AX3" s="120"/>
+      <c r="AY3" s="120"/>
+      <c r="AZ3" s="120"/>
+      <c r="BA3" s="121"/>
+      <c r="BB3" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="130"/>
-      <c r="BD3" s="130"/>
-      <c r="BE3" s="130"/>
-      <c r="BF3" s="130"/>
-      <c r="BG3" s="130" t="s">
+      <c r="BC3" s="111"/>
+      <c r="BD3" s="111"/>
+      <c r="BE3" s="111"/>
+      <c r="BF3" s="111"/>
+      <c r="BG3" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="130"/>
-      <c r="BI3" s="130"/>
-      <c r="BJ3" s="130"/>
-      <c r="BK3" s="130"/>
-      <c r="BL3" s="130" t="s">
+      <c r="BH3" s="111"/>
+      <c r="BI3" s="111"/>
+      <c r="BJ3" s="111"/>
+      <c r="BK3" s="111"/>
+      <c r="BL3" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="130"/>
-      <c r="BN3" s="130"/>
-      <c r="BO3" s="130"/>
-      <c r="BP3" s="142"/>
-      <c r="BQ3" s="129" t="s">
+      <c r="BM3" s="111"/>
+      <c r="BN3" s="111"/>
+      <c r="BO3" s="111"/>
+      <c r="BP3" s="112"/>
+      <c r="BQ3" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="130"/>
-      <c r="BS3" s="130"/>
-      <c r="BT3" s="130"/>
-      <c r="BU3" s="130"/>
-      <c r="BV3" s="130" t="s">
+      <c r="BR3" s="111"/>
+      <c r="BS3" s="111"/>
+      <c r="BT3" s="111"/>
+      <c r="BU3" s="111"/>
+      <c r="BV3" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="130"/>
-      <c r="BX3" s="130"/>
-      <c r="BY3" s="130"/>
-      <c r="BZ3" s="130"/>
-      <c r="CA3" s="130" t="s">
+      <c r="BW3" s="111"/>
+      <c r="BX3" s="111"/>
+      <c r="BY3" s="111"/>
+      <c r="BZ3" s="111"/>
+      <c r="CA3" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="130"/>
-      <c r="CC3" s="130"/>
-      <c r="CD3" s="130"/>
-      <c r="CE3" s="142"/>
+      <c r="CB3" s="111"/>
+      <c r="CC3" s="111"/>
+      <c r="CD3" s="111"/>
+      <c r="CE3" s="112"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="124"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="132"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="138"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -5829,17 +5832,6 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5856,6 +5848,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
E-Team weekly report week 11
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16305" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We are assembling the E-Box, but we still aren't sure of our power systems. I've reached out to a couple EE advisor options, but haven't heard back. I've been informed that the mechanical components for the suspension are not yet complete, and as such, we will proibably not be driving by our milestone. We plan to have the control system working.</t>
+    <t>We are working on the E-Box, things are a bit behind due to some hicups on the mounting systems.</t>
   </si>
 </sst>
 </file>
@@ -1215,6 +1215,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1228,104 +1231,101 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1892,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1908,13 +1908,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="89" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="90" t="s">
@@ -1929,35 +1929,35 @@
       <c r="A4" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="109"/>
+      <c r="C4" s="110"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="110" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="109"/>
+      <c r="C5" s="110"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="109"/>
+      <c r="C6" s="110"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="92" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="93">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B9" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1997,63 +1997,63 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="106"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="106"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
+      <c r="A15" s="107"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="106"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
+      <c r="A16" s="107"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="106"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
+      <c r="A17" s="107"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="106"/>
-      <c r="B18" s="106"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="107"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="106"/>
-      <c r="B19" s="106"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
+      <c r="A19" s="107"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="106"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="106"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="106"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="99" t="s">
@@ -2174,10 +2174,10 @@
       </c>
       <c r="C28" s="103">
         <f>'Team Task Chart'!H10</f>
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D28" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="C30" s="103">
         <f>'Team Task Chart'!H12</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D30" s="98" t="s">
         <v>59</v>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="C31" s="103">
         <f>'Team Task Chart'!H13</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D31" s="98" t="s">
         <v>59</v>
@@ -2463,9 +2463,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AH1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="BY15" sqref="BY15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2566,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="122" t="s">
+      <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="123"/>
-      <c r="O2" s="123"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="123"/>
-      <c r="S2" s="123"/>
-      <c r="T2" s="123"/>
-      <c r="U2" s="123"/>
-      <c r="V2" s="123"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="125" t="s">
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="114"/>
+      <c r="X2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
-      <c r="AA2" s="126"/>
-      <c r="AB2" s="126"/>
-      <c r="AC2" s="126"/>
-      <c r="AD2" s="126"/>
-      <c r="AE2" s="126"/>
-      <c r="AF2" s="126"/>
-      <c r="AG2" s="126"/>
-      <c r="AH2" s="126"/>
-      <c r="AI2" s="126"/>
-      <c r="AJ2" s="126"/>
-      <c r="AK2" s="126"/>
-      <c r="AL2" s="127"/>
-      <c r="AM2" s="128" t="s">
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="116"/>
+      <c r="AJ2" s="116"/>
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="129"/>
-      <c r="AO2" s="129"/>
-      <c r="AP2" s="129"/>
-      <c r="AQ2" s="129"/>
-      <c r="AR2" s="129"/>
-      <c r="AS2" s="129"/>
-      <c r="AT2" s="129"/>
-      <c r="AU2" s="129"/>
-      <c r="AV2" s="129"/>
-      <c r="AW2" s="129"/>
-      <c r="AX2" s="129"/>
-      <c r="AY2" s="129"/>
-      <c r="AZ2" s="129"/>
-      <c r="BA2" s="130"/>
-      <c r="BB2" s="113" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="114"/>
-      <c r="BD2" s="114"/>
-      <c r="BE2" s="114"/>
-      <c r="BF2" s="114"/>
-      <c r="BG2" s="114"/>
-      <c r="BH2" s="114"/>
-      <c r="BI2" s="114"/>
-      <c r="BJ2" s="114"/>
-      <c r="BK2" s="114"/>
-      <c r="BL2" s="114"/>
-      <c r="BM2" s="114"/>
-      <c r="BN2" s="114"/>
-      <c r="BO2" s="114"/>
-      <c r="BP2" s="115"/>
-      <c r="BQ2" s="113" t="s">
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="122"/>
+      <c r="BF2" s="122"/>
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="123"/>
+      <c r="BQ2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="114"/>
-      <c r="BS2" s="114"/>
-      <c r="BT2" s="114"/>
-      <c r="BU2" s="114"/>
-      <c r="BV2" s="114"/>
-      <c r="BW2" s="114"/>
-      <c r="BX2" s="114"/>
-      <c r="BY2" s="114"/>
-      <c r="BZ2" s="114"/>
-      <c r="CA2" s="114"/>
-      <c r="CB2" s="114"/>
-      <c r="CC2" s="114"/>
-      <c r="CD2" s="114"/>
-      <c r="CE2" s="115"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="122"/>
+      <c r="BV2" s="122"/>
+      <c r="BW2" s="122"/>
+      <c r="BX2" s="122"/>
+      <c r="BY2" s="122"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="122"/>
+      <c r="CB2" s="122"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="122"/>
+      <c r="CE2" s="123"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="135" t="s">
+      <c r="D3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="135" t="s">
+      <c r="E3" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="135" t="s">
+      <c r="G3" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="137" t="s">
+      <c r="H3" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="139" t="s">
+      <c r="I3" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140" t="s">
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
-      <c r="R3" s="140"/>
-      <c r="S3" s="140" t="s">
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="140"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="141"/>
-      <c r="X3" s="142" t="s">
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
-      <c r="AB3" s="117"/>
-      <c r="AC3" s="117" t="s">
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="138"/>
+      <c r="AC3" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="117"/>
-      <c r="AE3" s="117"/>
-      <c r="AF3" s="117"/>
-      <c r="AG3" s="117"/>
-      <c r="AH3" s="117" t="s">
+      <c r="AD3" s="138"/>
+      <c r="AE3" s="138"/>
+      <c r="AF3" s="138"/>
+      <c r="AG3" s="138"/>
+      <c r="AH3" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="117"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="117"/>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="119" t="s">
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="138"/>
+      <c r="AK3" s="138"/>
+      <c r="AL3" s="139"/>
+      <c r="AM3" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="120"/>
-      <c r="AO3" s="120"/>
-      <c r="AP3" s="120"/>
-      <c r="AQ3" s="120"/>
-      <c r="AR3" s="120" t="s">
+      <c r="AN3" s="141"/>
+      <c r="AO3" s="141"/>
+      <c r="AP3" s="141"/>
+      <c r="AQ3" s="141"/>
+      <c r="AR3" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="120"/>
-      <c r="AT3" s="120"/>
-      <c r="AU3" s="120"/>
-      <c r="AV3" s="120"/>
-      <c r="AW3" s="120" t="s">
+      <c r="AS3" s="141"/>
+      <c r="AT3" s="141"/>
+      <c r="AU3" s="141"/>
+      <c r="AV3" s="141"/>
+      <c r="AW3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="120"/>
-      <c r="AY3" s="120"/>
-      <c r="AZ3" s="120"/>
-      <c r="BA3" s="121"/>
-      <c r="BB3" s="116" t="s">
+      <c r="AX3" s="141"/>
+      <c r="AY3" s="141"/>
+      <c r="AZ3" s="141"/>
+      <c r="BA3" s="142"/>
+      <c r="BB3" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="111"/>
-      <c r="BD3" s="111"/>
-      <c r="BE3" s="111"/>
-      <c r="BF3" s="111"/>
-      <c r="BG3" s="111" t="s">
+      <c r="BC3" s="131"/>
+      <c r="BD3" s="131"/>
+      <c r="BE3" s="131"/>
+      <c r="BF3" s="131"/>
+      <c r="BG3" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="111"/>
-      <c r="BI3" s="111"/>
-      <c r="BJ3" s="111"/>
-      <c r="BK3" s="111"/>
-      <c r="BL3" s="111" t="s">
+      <c r="BH3" s="131"/>
+      <c r="BI3" s="131"/>
+      <c r="BJ3" s="131"/>
+      <c r="BK3" s="131"/>
+      <c r="BL3" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="111"/>
-      <c r="BN3" s="111"/>
-      <c r="BO3" s="111"/>
-      <c r="BP3" s="112"/>
-      <c r="BQ3" s="116" t="s">
+      <c r="BM3" s="131"/>
+      <c r="BN3" s="131"/>
+      <c r="BO3" s="131"/>
+      <c r="BP3" s="143"/>
+      <c r="BQ3" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="111"/>
-      <c r="BS3" s="111"/>
-      <c r="BT3" s="111"/>
-      <c r="BU3" s="111"/>
-      <c r="BV3" s="111" t="s">
+      <c r="BR3" s="131"/>
+      <c r="BS3" s="131"/>
+      <c r="BT3" s="131"/>
+      <c r="BU3" s="131"/>
+      <c r="BV3" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="111"/>
-      <c r="BX3" s="111"/>
-      <c r="BY3" s="111"/>
-      <c r="BZ3" s="111"/>
-      <c r="CA3" s="111" t="s">
+      <c r="BW3" s="131"/>
+      <c r="BX3" s="131"/>
+      <c r="BY3" s="131"/>
+      <c r="BZ3" s="131"/>
+      <c r="CA3" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="111"/>
-      <c r="CC3" s="111"/>
-      <c r="CD3" s="111"/>
-      <c r="CE3" s="112"/>
+      <c r="CB3" s="131"/>
+      <c r="CC3" s="131"/>
+      <c r="CD3" s="131"/>
+      <c r="CE3" s="143"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="132"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="138"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="133"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3606,11 +3606,21 @@
       <c r="BF9" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="BG9" s="48"/>
-      <c r="BH9" s="48"/>
-      <c r="BI9" s="48"/>
-      <c r="BJ9" s="48"/>
-      <c r="BK9" s="48"/>
+      <c r="BG9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK9" s="48" t="s">
+        <v>77</v>
+      </c>
       <c r="BL9" s="48"/>
       <c r="BM9" s="48"/>
       <c r="BN9" s="48"/>
@@ -3649,7 +3659,7 @@
       </c>
       <c r="G10" s="41"/>
       <c r="H10" s="42">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="44"/>
@@ -3751,11 +3761,21 @@
       <c r="BF10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="BG10" s="52"/>
-      <c r="BH10" s="52"/>
-      <c r="BI10" s="52"/>
-      <c r="BJ10" s="52"/>
-      <c r="BK10" s="52"/>
+      <c r="BG10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK10" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="BL10" s="52"/>
       <c r="BM10" s="52"/>
       <c r="BN10" s="52"/>
@@ -3896,11 +3916,21 @@
       <c r="BF11" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="BG11" s="84"/>
-      <c r="BH11" s="84"/>
-      <c r="BI11" s="84"/>
-      <c r="BJ11" s="84"/>
-      <c r="BK11" s="84"/>
+      <c r="BG11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK11" s="84" t="s">
+        <v>77</v>
+      </c>
       <c r="BL11" s="84"/>
       <c r="BM11" s="84"/>
       <c r="BN11" s="84"/>
@@ -3939,7 +3969,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -4041,11 +4071,21 @@
       <c r="BF12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="BG12" s="59"/>
-      <c r="BH12" s="59"/>
-      <c r="BI12" s="59"/>
-      <c r="BJ12" s="59"/>
-      <c r="BK12" s="59"/>
+      <c r="BG12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK12" s="59" t="s">
+        <v>77</v>
+      </c>
       <c r="BL12" s="59"/>
       <c r="BM12" s="59"/>
       <c r="BN12" s="59"/>
@@ -4084,7 +4124,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -4186,11 +4226,21 @@
       <c r="BF13" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="BG13" s="62"/>
-      <c r="BH13" s="62"/>
-      <c r="BI13" s="62"/>
-      <c r="BJ13" s="62"/>
-      <c r="BK13" s="62"/>
+      <c r="BG13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK13" s="62" t="s">
+        <v>77</v>
+      </c>
       <c r="BL13" s="62"/>
       <c r="BM13" s="62"/>
       <c r="BN13" s="62"/>
@@ -5832,6 +5882,17 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5848,17 +5909,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -5936,8 +5986,8 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6032,7 +6082,9 @@
       <c r="K2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -6040,7 +6092,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -6080,7 +6132,9 @@
       <c r="K3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -6088,7 +6142,7 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="7">
         <f t="shared" ref="R3:R9" si="0">COUNTIF(D3:Q3,"P")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -6128,7 +6182,9 @@
       <c r="K4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -6136,7 +6192,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6176,7 +6232,9 @@
       <c r="K5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -6184,7 +6242,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1">
@@ -6221,7 +6279,9 @@
       <c r="K6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -6229,7 +6289,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
E-Teaam update for Week 12
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16305" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17235" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We are working on the E-Box, things are a bit behind due to some hicups on the mounting systems.</t>
+    <t>We have milestone 1 due Sunday (drive system). I've been working on the report. The team has gotten the control system working (getting the control signal from source to destination and translating between forms). We don't have a chassis, suspension, or E-box, so we'll be getting a bit creative with the video to show it working.</t>
   </si>
 </sst>
 </file>
@@ -1231,6 +1231,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1258,15 +1291,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1285,12 +1309,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1307,24 +1325,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1892,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1957,7 +1957,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="93">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B9" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="B10" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1993,7 +1993,7 @@
         <v>70</v>
       </c>
       <c r="B12" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C27" s="103">
         <f>'Team Task Chart'!H9</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D27" s="98" t="s">
         <v>58</v>
@@ -2208,10 +2208,10 @@
       </c>
       <c r="C30" s="103">
         <f>'Team Task Chart'!H12</f>
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D30" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2225,10 +2225,10 @@
       </c>
       <c r="C31" s="103">
         <f>'Team Task Chart'!H13</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D31" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2463,9 +2463,9 @@
   </sheetPr>
   <dimension ref="B1:CE35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AH1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BY15" sqref="BY15"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2566,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="114"/>
-      <c r="X2" s="115" t="s">
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="116"/>
-      <c r="AA2" s="116"/>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="116"/>
-      <c r="AD2" s="116"/>
-      <c r="AE2" s="116"/>
-      <c r="AF2" s="116"/>
-      <c r="AG2" s="116"/>
-      <c r="AH2" s="116"/>
-      <c r="AI2" s="116"/>
-      <c r="AJ2" s="116"/>
-      <c r="AK2" s="116"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="118" t="s">
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+      <c r="AL2" s="128"/>
+      <c r="AM2" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="119"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="119"/>
-      <c r="AX2" s="119"/>
-      <c r="AY2" s="119"/>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="120"/>
-      <c r="BB2" s="121" t="s">
+      <c r="AN2" s="130"/>
+      <c r="AO2" s="130"/>
+      <c r="AP2" s="130"/>
+      <c r="AQ2" s="130"/>
+      <c r="AR2" s="130"/>
+      <c r="AS2" s="130"/>
+      <c r="AT2" s="130"/>
+      <c r="AU2" s="130"/>
+      <c r="AV2" s="130"/>
+      <c r="AW2" s="130"/>
+      <c r="AX2" s="130"/>
+      <c r="AY2" s="130"/>
+      <c r="AZ2" s="130"/>
+      <c r="BA2" s="131"/>
+      <c r="BB2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="122"/>
-      <c r="BD2" s="122"/>
-      <c r="BE2" s="122"/>
-      <c r="BF2" s="122"/>
-      <c r="BG2" s="122"/>
-      <c r="BH2" s="122"/>
-      <c r="BI2" s="122"/>
-      <c r="BJ2" s="122"/>
-      <c r="BK2" s="122"/>
-      <c r="BL2" s="122"/>
-      <c r="BM2" s="122"/>
-      <c r="BN2" s="122"/>
-      <c r="BO2" s="122"/>
-      <c r="BP2" s="123"/>
-      <c r="BQ2" s="121" t="s">
+      <c r="BC2" s="115"/>
+      <c r="BD2" s="115"/>
+      <c r="BE2" s="115"/>
+      <c r="BF2" s="115"/>
+      <c r="BG2" s="115"/>
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="115"/>
+      <c r="BJ2" s="115"/>
+      <c r="BK2" s="115"/>
+      <c r="BL2" s="115"/>
+      <c r="BM2" s="115"/>
+      <c r="BN2" s="115"/>
+      <c r="BO2" s="115"/>
+      <c r="BP2" s="116"/>
+      <c r="BQ2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="122"/>
-      <c r="BS2" s="122"/>
-      <c r="BT2" s="122"/>
-      <c r="BU2" s="122"/>
-      <c r="BV2" s="122"/>
-      <c r="BW2" s="122"/>
-      <c r="BX2" s="122"/>
-      <c r="BY2" s="122"/>
-      <c r="BZ2" s="122"/>
-      <c r="CA2" s="122"/>
-      <c r="CB2" s="122"/>
-      <c r="CC2" s="122"/>
-      <c r="CD2" s="122"/>
-      <c r="CE2" s="123"/>
+      <c r="BR2" s="115"/>
+      <c r="BS2" s="115"/>
+      <c r="BT2" s="115"/>
+      <c r="BU2" s="115"/>
+      <c r="BV2" s="115"/>
+      <c r="BW2" s="115"/>
+      <c r="BX2" s="115"/>
+      <c r="BY2" s="115"/>
+      <c r="BZ2" s="115"/>
+      <c r="CA2" s="115"/>
+      <c r="CB2" s="115"/>
+      <c r="CC2" s="115"/>
+      <c r="CD2" s="115"/>
+      <c r="CE2" s="116"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="132" t="s">
+      <c r="H3" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="134" t="s">
+      <c r="I3" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135" t="s">
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135" t="s">
+      <c r="O3" s="141"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="137" t="s">
+      <c r="T3" s="141"/>
+      <c r="U3" s="141"/>
+      <c r="V3" s="141"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="138"/>
-      <c r="AC3" s="138" t="s">
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="138"/>
-      <c r="AE3" s="138"/>
-      <c r="AF3" s="138"/>
-      <c r="AG3" s="138"/>
-      <c r="AH3" s="138" t="s">
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="118"/>
+      <c r="AH3" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="138"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="138"/>
-      <c r="AL3" s="139"/>
-      <c r="AM3" s="140" t="s">
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="119"/>
+      <c r="AM3" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="141"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="141" t="s">
+      <c r="AN3" s="121"/>
+      <c r="AO3" s="121"/>
+      <c r="AP3" s="121"/>
+      <c r="AQ3" s="121"/>
+      <c r="AR3" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="141"/>
-      <c r="AT3" s="141"/>
-      <c r="AU3" s="141"/>
-      <c r="AV3" s="141"/>
-      <c r="AW3" s="141" t="s">
+      <c r="AS3" s="121"/>
+      <c r="AT3" s="121"/>
+      <c r="AU3" s="121"/>
+      <c r="AV3" s="121"/>
+      <c r="AW3" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="141"/>
-      <c r="AY3" s="141"/>
-      <c r="AZ3" s="141"/>
-      <c r="BA3" s="142"/>
-      <c r="BB3" s="130" t="s">
+      <c r="AX3" s="121"/>
+      <c r="AY3" s="121"/>
+      <c r="AZ3" s="121"/>
+      <c r="BA3" s="122"/>
+      <c r="BB3" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="131"/>
-      <c r="BD3" s="131"/>
-      <c r="BE3" s="131"/>
-      <c r="BF3" s="131"/>
-      <c r="BG3" s="131" t="s">
+      <c r="BC3" s="112"/>
+      <c r="BD3" s="112"/>
+      <c r="BE3" s="112"/>
+      <c r="BF3" s="112"/>
+      <c r="BG3" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="131"/>
-      <c r="BI3" s="131"/>
-      <c r="BJ3" s="131"/>
-      <c r="BK3" s="131"/>
-      <c r="BL3" s="131" t="s">
+      <c r="BH3" s="112"/>
+      <c r="BI3" s="112"/>
+      <c r="BJ3" s="112"/>
+      <c r="BK3" s="112"/>
+      <c r="BL3" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="131"/>
-      <c r="BN3" s="131"/>
-      <c r="BO3" s="131"/>
-      <c r="BP3" s="143"/>
-      <c r="BQ3" s="130" t="s">
+      <c r="BM3" s="112"/>
+      <c r="BN3" s="112"/>
+      <c r="BO3" s="112"/>
+      <c r="BP3" s="113"/>
+      <c r="BQ3" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="131"/>
-      <c r="BS3" s="131"/>
-      <c r="BT3" s="131"/>
-      <c r="BU3" s="131"/>
-      <c r="BV3" s="131" t="s">
+      <c r="BR3" s="112"/>
+      <c r="BS3" s="112"/>
+      <c r="BT3" s="112"/>
+      <c r="BU3" s="112"/>
+      <c r="BV3" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="131"/>
-      <c r="BX3" s="131"/>
-      <c r="BY3" s="131"/>
-      <c r="BZ3" s="131"/>
-      <c r="CA3" s="131" t="s">
+      <c r="BW3" s="112"/>
+      <c r="BX3" s="112"/>
+      <c r="BY3" s="112"/>
+      <c r="BZ3" s="112"/>
+      <c r="CA3" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="131"/>
-      <c r="CC3" s="131"/>
-      <c r="CD3" s="131"/>
-      <c r="CE3" s="143"/>
+      <c r="CB3" s="112"/>
+      <c r="CC3" s="112"/>
+      <c r="CD3" s="112"/>
+      <c r="CE3" s="113"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="125"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="133"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="139"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3490,7 +3490,7 @@
       </c>
       <c r="G9" s="41"/>
       <c r="H9" s="42">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I9" s="43"/>
       <c r="J9" s="44"/>
@@ -3621,11 +3621,21 @@
       <c r="BK9" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="BL9" s="48"/>
-      <c r="BM9" s="48"/>
-      <c r="BN9" s="48"/>
-      <c r="BO9" s="48"/>
-      <c r="BP9" s="54"/>
+      <c r="BL9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP9" s="54" t="s">
+        <v>77</v>
+      </c>
       <c r="BQ9" s="43"/>
       <c r="BR9" s="44"/>
       <c r="BS9" s="44"/>
@@ -3776,11 +3786,21 @@
       <c r="BK10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="BL10" s="52"/>
-      <c r="BM10" s="52"/>
-      <c r="BN10" s="52"/>
-      <c r="BO10" s="52"/>
-      <c r="BP10" s="53"/>
+      <c r="BL10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP10" s="53" t="s">
+        <v>77</v>
+      </c>
       <c r="BQ10" s="43"/>
       <c r="BR10" s="44"/>
       <c r="BS10" s="44"/>
@@ -3931,11 +3951,21 @@
       <c r="BK11" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="BL11" s="84"/>
-      <c r="BM11" s="84"/>
-      <c r="BN11" s="84"/>
-      <c r="BO11" s="84"/>
-      <c r="BP11" s="85"/>
+      <c r="BL11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP11" s="85" t="s">
+        <v>77</v>
+      </c>
       <c r="BQ11" s="43"/>
       <c r="BR11" s="44"/>
       <c r="BS11" s="44"/>
@@ -3969,7 +3999,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -4086,11 +4116,21 @@
       <c r="BK12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="BL12" s="59"/>
-      <c r="BM12" s="59"/>
-      <c r="BN12" s="59"/>
-      <c r="BO12" s="59"/>
-      <c r="BP12" s="60"/>
+      <c r="BL12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP12" s="60" t="s">
+        <v>77</v>
+      </c>
       <c r="BQ12" s="43"/>
       <c r="BR12" s="44"/>
       <c r="BS12" s="44"/>
@@ -4124,7 +4164,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -4241,11 +4281,21 @@
       <c r="BK13" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="BL13" s="62"/>
-      <c r="BM13" s="62"/>
-      <c r="BN13" s="62"/>
-      <c r="BO13" s="62"/>
-      <c r="BP13" s="63"/>
+      <c r="BL13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO13" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP13" s="63" t="s">
+        <v>77</v>
+      </c>
       <c r="BQ13" s="43"/>
       <c r="BR13" s="44"/>
       <c r="BS13" s="44"/>
@@ -5882,17 +5932,6 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5909,6 +5948,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -5986,8 +6036,8 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6085,14 +6135,16 @@
       <c r="L2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -6135,7 +6187,9 @@
       <c r="L3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="8"/>
+      <c r="M3" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
@@ -6185,14 +6239,16 @@
       <c r="L4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6235,7 +6291,9 @@
       <c r="L5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -6282,14 +6340,16 @@
       <c r="L6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
E-Team report week 13
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17235" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18165" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We have milestone 1 due Sunday (drive system). I've been working on the report. The team has gotten the control system working (getting the control signal from source to destination and translating between forms). We don't have a chassis, suspension, or E-box, so we'll be getting a bit creative with the video to show it working.</t>
+    <t>We do not have an E-Box yet. We are working on the connector board for the drive system, and on refing the drive system code to allow for more robust control. We are a bit behind due to setbacks from other teams. This includes a lack of enclosures to add wiring to. We are having some trouble finding desirable connectors, due to a lack of experience with the naming conventions and such.</t>
   </si>
 </sst>
 </file>
@@ -1231,22 +1231,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1264,67 +1324,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1892,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1957,7 +1957,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="93">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B9" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2126,7 +2126,7 @@
         <v>0.7</v>
       </c>
       <c r="D25" s="98" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="C28" s="103">
         <f>'Team Task Chart'!H10</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D28" s="98" t="s">
         <v>58</v>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="C30" s="103">
         <f>'Team Task Chart'!H12</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="D30" s="98" t="s">
         <v>58</v>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="C31" s="103">
         <f>'Team Task Chart'!H13</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D31" s="98" t="s">
         <v>58</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="C33" s="103">
         <f>'Team Task Chart'!H15</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D33" s="98" t="s">
         <v>58</v>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="C34" s="103">
         <f>'Team Task Chart'!H16</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D34" s="98" t="s">
         <v>58</v>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="C35" s="103">
         <f>'Team Task Chart'!H17</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D35" s="98" t="s">
         <v>58</v>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="C36" s="103">
         <f>'Team Task Chart'!H18</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D36" s="98" t="s">
         <v>58</v>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="98" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2465,7 +2465,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2566,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="123" t="s">
+      <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="126" t="s">
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="114"/>
+      <c r="X2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="127"/>
-      <c r="AB2" s="127"/>
-      <c r="AC2" s="127"/>
-      <c r="AD2" s="127"/>
-      <c r="AE2" s="127"/>
-      <c r="AF2" s="127"/>
-      <c r="AG2" s="127"/>
-      <c r="AH2" s="127"/>
-      <c r="AI2" s="127"/>
-      <c r="AJ2" s="127"/>
-      <c r="AK2" s="127"/>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="129" t="s">
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="116"/>
+      <c r="AJ2" s="116"/>
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="130"/>
-      <c r="AO2" s="130"/>
-      <c r="AP2" s="130"/>
-      <c r="AQ2" s="130"/>
-      <c r="AR2" s="130"/>
-      <c r="AS2" s="130"/>
-      <c r="AT2" s="130"/>
-      <c r="AU2" s="130"/>
-      <c r="AV2" s="130"/>
-      <c r="AW2" s="130"/>
-      <c r="AX2" s="130"/>
-      <c r="AY2" s="130"/>
-      <c r="AZ2" s="130"/>
-      <c r="BA2" s="131"/>
-      <c r="BB2" s="114" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="115"/>
-      <c r="BD2" s="115"/>
-      <c r="BE2" s="115"/>
-      <c r="BF2" s="115"/>
-      <c r="BG2" s="115"/>
-      <c r="BH2" s="115"/>
-      <c r="BI2" s="115"/>
-      <c r="BJ2" s="115"/>
-      <c r="BK2" s="115"/>
-      <c r="BL2" s="115"/>
-      <c r="BM2" s="115"/>
-      <c r="BN2" s="115"/>
-      <c r="BO2" s="115"/>
-      <c r="BP2" s="116"/>
-      <c r="BQ2" s="114" t="s">
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="122"/>
+      <c r="BF2" s="122"/>
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="123"/>
+      <c r="BQ2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="115"/>
-      <c r="BS2" s="115"/>
-      <c r="BT2" s="115"/>
-      <c r="BU2" s="115"/>
-      <c r="BV2" s="115"/>
-      <c r="BW2" s="115"/>
-      <c r="BX2" s="115"/>
-      <c r="BY2" s="115"/>
-      <c r="BZ2" s="115"/>
-      <c r="CA2" s="115"/>
-      <c r="CB2" s="115"/>
-      <c r="CC2" s="115"/>
-      <c r="CD2" s="115"/>
-      <c r="CE2" s="116"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="122"/>
+      <c r="BV2" s="122"/>
+      <c r="BW2" s="122"/>
+      <c r="BX2" s="122"/>
+      <c r="BY2" s="122"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="122"/>
+      <c r="CB2" s="122"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="122"/>
+      <c r="CE2" s="123"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="136" t="s">
+      <c r="G3" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="138" t="s">
+      <c r="H3" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="140" t="s">
+      <c r="I3" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="141" t="s">
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="141" t="s">
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="141"/>
-      <c r="U3" s="141"/>
-      <c r="V3" s="141"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="143" t="s">
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="118" t="s">
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="138"/>
+      <c r="AC3" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="118"/>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118"/>
-      <c r="AH3" s="118" t="s">
+      <c r="AD3" s="138"/>
+      <c r="AE3" s="138"/>
+      <c r="AF3" s="138"/>
+      <c r="AG3" s="138"/>
+      <c r="AH3" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118"/>
-      <c r="AK3" s="118"/>
-      <c r="AL3" s="119"/>
-      <c r="AM3" s="120" t="s">
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="138"/>
+      <c r="AK3" s="138"/>
+      <c r="AL3" s="139"/>
+      <c r="AM3" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="121"/>
-      <c r="AO3" s="121"/>
-      <c r="AP3" s="121"/>
-      <c r="AQ3" s="121"/>
-      <c r="AR3" s="121" t="s">
+      <c r="AN3" s="141"/>
+      <c r="AO3" s="141"/>
+      <c r="AP3" s="141"/>
+      <c r="AQ3" s="141"/>
+      <c r="AR3" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="121"/>
-      <c r="AT3" s="121"/>
-      <c r="AU3" s="121"/>
-      <c r="AV3" s="121"/>
-      <c r="AW3" s="121" t="s">
+      <c r="AS3" s="141"/>
+      <c r="AT3" s="141"/>
+      <c r="AU3" s="141"/>
+      <c r="AV3" s="141"/>
+      <c r="AW3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="121"/>
-      <c r="AY3" s="121"/>
-      <c r="AZ3" s="121"/>
-      <c r="BA3" s="122"/>
-      <c r="BB3" s="117" t="s">
+      <c r="AX3" s="141"/>
+      <c r="AY3" s="141"/>
+      <c r="AZ3" s="141"/>
+      <c r="BA3" s="142"/>
+      <c r="BB3" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="112"/>
-      <c r="BD3" s="112"/>
-      <c r="BE3" s="112"/>
-      <c r="BF3" s="112"/>
-      <c r="BG3" s="112" t="s">
+      <c r="BC3" s="131"/>
+      <c r="BD3" s="131"/>
+      <c r="BE3" s="131"/>
+      <c r="BF3" s="131"/>
+      <c r="BG3" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="112"/>
-      <c r="BI3" s="112"/>
-      <c r="BJ3" s="112"/>
-      <c r="BK3" s="112"/>
-      <c r="BL3" s="112" t="s">
+      <c r="BH3" s="131"/>
+      <c r="BI3" s="131"/>
+      <c r="BJ3" s="131"/>
+      <c r="BK3" s="131"/>
+      <c r="BL3" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="112"/>
-      <c r="BN3" s="112"/>
-      <c r="BO3" s="112"/>
-      <c r="BP3" s="113"/>
-      <c r="BQ3" s="117" t="s">
+      <c r="BM3" s="131"/>
+      <c r="BN3" s="131"/>
+      <c r="BO3" s="131"/>
+      <c r="BP3" s="143"/>
+      <c r="BQ3" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="112"/>
-      <c r="BS3" s="112"/>
-      <c r="BT3" s="112"/>
-      <c r="BU3" s="112"/>
-      <c r="BV3" s="112" t="s">
+      <c r="BR3" s="131"/>
+      <c r="BS3" s="131"/>
+      <c r="BT3" s="131"/>
+      <c r="BU3" s="131"/>
+      <c r="BV3" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="112"/>
-      <c r="BX3" s="112"/>
-      <c r="BY3" s="112"/>
-      <c r="BZ3" s="112"/>
-      <c r="CA3" s="112" t="s">
+      <c r="BW3" s="131"/>
+      <c r="BX3" s="131"/>
+      <c r="BY3" s="131"/>
+      <c r="BZ3" s="131"/>
+      <c r="CA3" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="112"/>
-      <c r="CC3" s="112"/>
-      <c r="CD3" s="112"/>
-      <c r="CE3" s="113"/>
+      <c r="CB3" s="131"/>
+      <c r="CC3" s="131"/>
+      <c r="CD3" s="131"/>
+      <c r="CE3" s="143"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="133"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="139"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="133"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="G10" s="41"/>
       <c r="H10" s="42">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="44"/>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="42">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="44"/>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="42">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
@@ -4411,7 +4411,9 @@
         <v>43066</v>
       </c>
       <c r="G15" s="68"/>
-      <c r="H15" s="69"/>
+      <c r="H15" s="69">
+        <v>0.5</v>
+      </c>
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -4505,7 +4507,7 @@
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="42">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="44"/>
@@ -4600,7 +4602,7 @@
       </c>
       <c r="G17" s="41"/>
       <c r="H17" s="42">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="44"/>
@@ -4693,7 +4695,7 @@
       </c>
       <c r="G18" s="41"/>
       <c r="H18" s="42">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="44"/>
@@ -5932,6 +5934,17 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5948,17 +5961,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -6036,8 +6038,8 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6138,13 +6140,15 @@
       <c r="M2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -6190,13 +6194,15 @@
       <c r="M3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="7">
         <f t="shared" ref="R3:R9" si="0">COUNTIF(D3:Q3,"P")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -6242,13 +6248,15 @@
       <c r="M4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6294,13 +6302,15 @@
       <c r="M5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="8"/>
+      <c r="N5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1">
@@ -6343,13 +6353,15 @@
       <c r="M6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
E-Team report Week 14
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18165" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="118">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -1231,6 +1231,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1258,15 +1291,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1285,12 +1309,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1307,24 +1325,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1892,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1957,7 +1957,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="93">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B9" s="96">
         <f>COUNTIF('Attendance Records'!D2:Q9,"P")</f>
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="C23" s="103">
         <f>'Team Task Chart'!H5</f>
-        <v>0.89999999999999991</v>
+        <v>1</v>
       </c>
       <c r="D23" s="98" t="s">
         <v>58</v>
@@ -2123,10 +2123,10 @@
       </c>
       <c r="C25" s="103">
         <f>'Team Task Chart'!H7</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D25" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="C26" s="103">
         <f>'Team Task Chart'!H8</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D26" s="98" t="s">
         <v>58</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="C33" s="103">
         <f>'Team Task Chart'!H15</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D33" s="98" t="s">
         <v>58</v>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="C34" s="103">
         <f>'Team Task Chart'!H16</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D34" s="98" t="s">
         <v>58</v>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="C35" s="103">
         <f>'Team Task Chart'!H17</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D35" s="98" t="s">
         <v>58</v>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="C36" s="103">
         <f>'Team Task Chart'!H18</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D36" s="98" t="s">
         <v>58</v>
@@ -2344,10 +2344,10 @@
       </c>
       <c r="C38" s="103">
         <f>'Team Task Chart'!H20</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D38" s="98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="C39" s="103">
         <f>'Team Task Chart'!H21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="98" t="s">
         <v>58</v>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="C40" s="103">
         <f>'Team Task Chart'!H22</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D40" s="98" t="s">
         <v>58</v>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="C41" s="103">
         <f>'Team Task Chart'!H23</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D41" s="98" t="s">
         <v>58</v>
@@ -2465,7 +2465,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2566,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="114"/>
-      <c r="X2" s="115" t="s">
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="116"/>
-      <c r="AA2" s="116"/>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="116"/>
-      <c r="AD2" s="116"/>
-      <c r="AE2" s="116"/>
-      <c r="AF2" s="116"/>
-      <c r="AG2" s="116"/>
-      <c r="AH2" s="116"/>
-      <c r="AI2" s="116"/>
-      <c r="AJ2" s="116"/>
-      <c r="AK2" s="116"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="118" t="s">
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+      <c r="AL2" s="128"/>
+      <c r="AM2" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="119"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="119"/>
-      <c r="AX2" s="119"/>
-      <c r="AY2" s="119"/>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="120"/>
-      <c r="BB2" s="121" t="s">
+      <c r="AN2" s="130"/>
+      <c r="AO2" s="130"/>
+      <c r="AP2" s="130"/>
+      <c r="AQ2" s="130"/>
+      <c r="AR2" s="130"/>
+      <c r="AS2" s="130"/>
+      <c r="AT2" s="130"/>
+      <c r="AU2" s="130"/>
+      <c r="AV2" s="130"/>
+      <c r="AW2" s="130"/>
+      <c r="AX2" s="130"/>
+      <c r="AY2" s="130"/>
+      <c r="AZ2" s="130"/>
+      <c r="BA2" s="131"/>
+      <c r="BB2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="122"/>
-      <c r="BD2" s="122"/>
-      <c r="BE2" s="122"/>
-      <c r="BF2" s="122"/>
-      <c r="BG2" s="122"/>
-      <c r="BH2" s="122"/>
-      <c r="BI2" s="122"/>
-      <c r="BJ2" s="122"/>
-      <c r="BK2" s="122"/>
-      <c r="BL2" s="122"/>
-      <c r="BM2" s="122"/>
-      <c r="BN2" s="122"/>
-      <c r="BO2" s="122"/>
-      <c r="BP2" s="123"/>
-      <c r="BQ2" s="121" t="s">
+      <c r="BC2" s="115"/>
+      <c r="BD2" s="115"/>
+      <c r="BE2" s="115"/>
+      <c r="BF2" s="115"/>
+      <c r="BG2" s="115"/>
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="115"/>
+      <c r="BJ2" s="115"/>
+      <c r="BK2" s="115"/>
+      <c r="BL2" s="115"/>
+      <c r="BM2" s="115"/>
+      <c r="BN2" s="115"/>
+      <c r="BO2" s="115"/>
+      <c r="BP2" s="116"/>
+      <c r="BQ2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="122"/>
-      <c r="BS2" s="122"/>
-      <c r="BT2" s="122"/>
-      <c r="BU2" s="122"/>
-      <c r="BV2" s="122"/>
-      <c r="BW2" s="122"/>
-      <c r="BX2" s="122"/>
-      <c r="BY2" s="122"/>
-      <c r="BZ2" s="122"/>
-      <c r="CA2" s="122"/>
-      <c r="CB2" s="122"/>
-      <c r="CC2" s="122"/>
-      <c r="CD2" s="122"/>
-      <c r="CE2" s="123"/>
+      <c r="BR2" s="115"/>
+      <c r="BS2" s="115"/>
+      <c r="BT2" s="115"/>
+      <c r="BU2" s="115"/>
+      <c r="BV2" s="115"/>
+      <c r="BW2" s="115"/>
+      <c r="BX2" s="115"/>
+      <c r="BY2" s="115"/>
+      <c r="BZ2" s="115"/>
+      <c r="CA2" s="115"/>
+      <c r="CB2" s="115"/>
+      <c r="CC2" s="115"/>
+      <c r="CD2" s="115"/>
+      <c r="CE2" s="116"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="132" t="s">
+      <c r="H3" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="134" t="s">
+      <c r="I3" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135" t="s">
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135" t="s">
+      <c r="O3" s="141"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="137" t="s">
+      <c r="T3" s="141"/>
+      <c r="U3" s="141"/>
+      <c r="V3" s="141"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="138"/>
-      <c r="AC3" s="138" t="s">
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="138"/>
-      <c r="AE3" s="138"/>
-      <c r="AF3" s="138"/>
-      <c r="AG3" s="138"/>
-      <c r="AH3" s="138" t="s">
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="118"/>
+      <c r="AH3" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="138"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="138"/>
-      <c r="AL3" s="139"/>
-      <c r="AM3" s="140" t="s">
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="119"/>
+      <c r="AM3" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="141"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="141" t="s">
+      <c r="AN3" s="121"/>
+      <c r="AO3" s="121"/>
+      <c r="AP3" s="121"/>
+      <c r="AQ3" s="121"/>
+      <c r="AR3" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="141"/>
-      <c r="AT3" s="141"/>
-      <c r="AU3" s="141"/>
-      <c r="AV3" s="141"/>
-      <c r="AW3" s="141" t="s">
+      <c r="AS3" s="121"/>
+      <c r="AT3" s="121"/>
+      <c r="AU3" s="121"/>
+      <c r="AV3" s="121"/>
+      <c r="AW3" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="141"/>
-      <c r="AY3" s="141"/>
-      <c r="AZ3" s="141"/>
-      <c r="BA3" s="142"/>
-      <c r="BB3" s="130" t="s">
+      <c r="AX3" s="121"/>
+      <c r="AY3" s="121"/>
+      <c r="AZ3" s="121"/>
+      <c r="BA3" s="122"/>
+      <c r="BB3" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="131"/>
-      <c r="BD3" s="131"/>
-      <c r="BE3" s="131"/>
-      <c r="BF3" s="131"/>
-      <c r="BG3" s="131" t="s">
+      <c r="BC3" s="112"/>
+      <c r="BD3" s="112"/>
+      <c r="BE3" s="112"/>
+      <c r="BF3" s="112"/>
+      <c r="BG3" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="131"/>
-      <c r="BI3" s="131"/>
-      <c r="BJ3" s="131"/>
-      <c r="BK3" s="131"/>
-      <c r="BL3" s="131" t="s">
+      <c r="BH3" s="112"/>
+      <c r="BI3" s="112"/>
+      <c r="BJ3" s="112"/>
+      <c r="BK3" s="112"/>
+      <c r="BL3" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="131"/>
-      <c r="BN3" s="131"/>
-      <c r="BO3" s="131"/>
-      <c r="BP3" s="143"/>
-      <c r="BQ3" s="130" t="s">
+      <c r="BM3" s="112"/>
+      <c r="BN3" s="112"/>
+      <c r="BO3" s="112"/>
+      <c r="BP3" s="113"/>
+      <c r="BQ3" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="131"/>
-      <c r="BS3" s="131"/>
-      <c r="BT3" s="131"/>
-      <c r="BU3" s="131"/>
-      <c r="BV3" s="131" t="s">
+      <c r="BR3" s="112"/>
+      <c r="BS3" s="112"/>
+      <c r="BT3" s="112"/>
+      <c r="BU3" s="112"/>
+      <c r="BV3" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="131"/>
-      <c r="BX3" s="131"/>
-      <c r="BY3" s="131"/>
-      <c r="BZ3" s="131"/>
-      <c r="CA3" s="131" t="s">
+      <c r="BW3" s="112"/>
+      <c r="BX3" s="112"/>
+      <c r="BY3" s="112"/>
+      <c r="BZ3" s="112"/>
+      <c r="CA3" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="131"/>
-      <c r="CC3" s="131"/>
-      <c r="CD3" s="131"/>
-      <c r="CE3" s="143"/>
+      <c r="CB3" s="112"/>
+      <c r="CC3" s="112"/>
+      <c r="CD3" s="112"/>
+      <c r="CE3" s="113"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="125"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="133"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="139"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3029,7 +3029,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="32">
         <f>(2/3)*H6+(1/3)*H7</f>
-        <v>0.89999999999999991</v>
+        <v>1</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="34"/>
@@ -3233,7 +3233,7 @@
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="42">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I7" s="51" t="s">
         <v>77</v>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
@@ -3483,7 +3483,10 @@
       <c r="D9" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="40">
+        <f>$F$7</f>
+        <v>43005</v>
+      </c>
       <c r="F9" s="40">
         <f>$F$8</f>
         <v>43051</v>
@@ -3662,9 +3665,12 @@
       <c r="D10" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="40">
+        <f t="shared" ref="E10:E13" si="0">$F$7</f>
+        <v>43005</v>
+      </c>
       <c r="F10" s="40">
-        <f t="shared" ref="F10:F13" si="0">$F$8</f>
+        <f t="shared" ref="F10:F13" si="1">$F$8</f>
         <v>43051</v>
       </c>
       <c r="G10" s="41"/>
@@ -3827,9 +3833,12 @@
       <c r="D11" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="40">
+        <f t="shared" si="0"/>
+        <v>43005</v>
+      </c>
       <c r="F11" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43051</v>
       </c>
       <c r="G11" s="41"/>
@@ -3992,9 +4001,12 @@
       <c r="D12" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="40">
+        <f t="shared" si="0"/>
+        <v>43005</v>
+      </c>
       <c r="F12" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43051</v>
       </c>
       <c r="G12" s="41"/>
@@ -4157,9 +4169,12 @@
       <c r="D13" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="40">
+        <f t="shared" si="0"/>
+        <v>43005</v>
+      </c>
       <c r="F13" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43051</v>
       </c>
       <c r="G13" s="41"/>
@@ -4412,7 +4427,7 @@
       </c>
       <c r="G15" s="68"/>
       <c r="H15" s="69">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
@@ -4500,14 +4515,17 @@
       <c r="D16" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="40">
+        <f>$F$13</f>
+        <v>43051</v>
+      </c>
       <c r="F16" s="40">
         <f>$F$15</f>
         <v>43066</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="42">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="44"/>
@@ -4569,11 +4587,21 @@
       <c r="BN16" s="44"/>
       <c r="BO16" s="44"/>
       <c r="BP16" s="49"/>
-      <c r="BQ16" s="43"/>
-      <c r="BR16" s="44"/>
-      <c r="BS16" s="44"/>
-      <c r="BT16" s="44"/>
-      <c r="BU16" s="44"/>
+      <c r="BQ16" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR16" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS16" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BT16" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU16" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="BV16" s="36"/>
       <c r="BW16" s="36"/>
       <c r="BX16" s="36"/>
@@ -4595,14 +4623,17 @@
       <c r="D17" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="40">
+        <f t="shared" ref="E17:E18" si="2">$F$13</f>
+        <v>43051</v>
+      </c>
       <c r="F17" s="40">
-        <f t="shared" ref="F17:F18" si="1">$F$15</f>
+        <f t="shared" ref="F17:F18" si="3">$F$15</f>
         <v>43066</v>
       </c>
       <c r="G17" s="41"/>
       <c r="H17" s="42">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="44"/>
@@ -4664,11 +4695,21 @@
       <c r="BN17" s="44"/>
       <c r="BO17" s="44"/>
       <c r="BP17" s="49"/>
-      <c r="BQ17" s="43"/>
-      <c r="BR17" s="44"/>
-      <c r="BS17" s="44"/>
-      <c r="BT17" s="44"/>
-      <c r="BU17" s="44"/>
+      <c r="BQ17" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR17" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS17" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BT17" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU17" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="BV17" s="36"/>
       <c r="BW17" s="36"/>
       <c r="BX17" s="36"/>
@@ -4688,14 +4729,17 @@
       <c r="D18" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="40">
+        <f t="shared" si="2"/>
+        <v>43051</v>
+      </c>
       <c r="F18" s="40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43066</v>
       </c>
       <c r="G18" s="41"/>
       <c r="H18" s="42">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="44"/>
@@ -4757,11 +4801,21 @@
       <c r="BN18" s="44"/>
       <c r="BO18" s="44"/>
       <c r="BP18" s="49"/>
-      <c r="BQ18" s="43"/>
-      <c r="BR18" s="44"/>
-      <c r="BS18" s="44"/>
-      <c r="BT18" s="44"/>
-      <c r="BU18" s="44"/>
+      <c r="BQ18" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR18" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS18" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BT18" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU18" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="BV18" s="36"/>
       <c r="BW18" s="36"/>
       <c r="BX18" s="36"/>
@@ -4843,11 +4897,21 @@
       <c r="BN19" s="44"/>
       <c r="BO19" s="44"/>
       <c r="BP19" s="49"/>
-      <c r="BQ19" s="43"/>
-      <c r="BR19" s="44"/>
-      <c r="BS19" s="44"/>
-      <c r="BT19" s="44"/>
-      <c r="BU19" s="44"/>
+      <c r="BQ19" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR19" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS19" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BT19" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU19" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="BV19" s="36"/>
       <c r="BW19" s="36"/>
       <c r="BX19" s="36"/>
@@ -4872,7 +4936,9 @@
         <v>43072</v>
       </c>
       <c r="G20" s="68"/>
-      <c r="H20" s="69"/>
+      <c r="H20" s="69">
+        <v>0.6</v>
+      </c>
       <c r="I20" s="33"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -4959,14 +5025,17 @@
       <c r="D21" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="40">
+        <f>$F$18</f>
+        <v>43066</v>
+      </c>
       <c r="F21" s="40">
         <f>$F$20</f>
         <v>43072</v>
       </c>
       <c r="G21" s="41"/>
       <c r="H21" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="44"/>
@@ -5054,14 +5123,17 @@
       <c r="D22" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="40">
+        <f t="shared" ref="E22:E24" si="4">$F$18</f>
+        <v>43066</v>
+      </c>
       <c r="F22" s="40">
-        <f t="shared" ref="F22:F24" si="2">$F$20</f>
+        <f t="shared" ref="F22:F24" si="5">$F$20</f>
         <v>43072</v>
       </c>
       <c r="G22" s="41"/>
       <c r="H22" s="42">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I22" s="43"/>
       <c r="J22" s="44"/>
@@ -5149,14 +5221,17 @@
       <c r="D23" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" s="40">
+        <f t="shared" si="4"/>
+        <v>43066</v>
+      </c>
       <c r="F23" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>43072</v>
       </c>
       <c r="G23" s="41"/>
       <c r="H23" s="42">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I23" s="43"/>
       <c r="J23" s="44"/>
@@ -5244,14 +5319,17 @@
       <c r="D24" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="40">
+        <f t="shared" si="4"/>
+        <v>43066</v>
+      </c>
       <c r="F24" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>43072</v>
       </c>
       <c r="G24" s="41"/>
       <c r="H24" s="42">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="44"/>
@@ -5934,17 +6012,6 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5961,6 +6028,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">
@@ -6039,7 +6117,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6143,12 +6221,14 @@
       <c r="N2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="3">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -6197,12 +6277,14 @@
       <c r="N3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="8"/>
+      <c r="O3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="7">
         <f t="shared" ref="R3:R9" si="0">COUNTIF(D3:Q3,"P")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -6251,12 +6333,14 @@
       <c r="N4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -6305,12 +6389,14 @@
       <c r="N5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1">
@@ -6356,12 +6442,14 @@
       <c r="N6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="4"/>
+      <c r="O6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:21">

</xml_diff>

<commit_message>
Update to Week 14 report
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20025" yWindow="0" windowWidth="27840" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -384,7 +384,7 @@
     <t>Controls</t>
   </si>
   <si>
-    <t>We do not have an E-Box yet. We are working on the connector board for the drive system, and on refing the drive system code to allow for more robust control. We are a bit behind due to setbacks from other teams. This includes a lack of enclosures to add wiring to. We are having some trouble finding desirable connectors, due to a lack of experience with the naming conventions and such.</t>
+    <t>We have an E-box now. We will be wiring what we can with the E-Box, and using the old motor controllers (VEX Victor SP) to control the arm DC motors. I have been looking at power regulation for the arm (15A @12V). The load is higher than I can find for regulators online, but not crazy high, I'm checking with some EEs.</t>
   </si>
 </sst>
 </file>
@@ -1231,22 +1231,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1264,67 +1324,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2566,228 +2566,228 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="123" t="s">
+      <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="126" t="s">
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="114"/>
+      <c r="X2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="127"/>
-      <c r="AB2" s="127"/>
-      <c r="AC2" s="127"/>
-      <c r="AD2" s="127"/>
-      <c r="AE2" s="127"/>
-      <c r="AF2" s="127"/>
-      <c r="AG2" s="127"/>
-      <c r="AH2" s="127"/>
-      <c r="AI2" s="127"/>
-      <c r="AJ2" s="127"/>
-      <c r="AK2" s="127"/>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="129" t="s">
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="116"/>
+      <c r="AJ2" s="116"/>
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="130"/>
-      <c r="AO2" s="130"/>
-      <c r="AP2" s="130"/>
-      <c r="AQ2" s="130"/>
-      <c r="AR2" s="130"/>
-      <c r="AS2" s="130"/>
-      <c r="AT2" s="130"/>
-      <c r="AU2" s="130"/>
-      <c r="AV2" s="130"/>
-      <c r="AW2" s="130"/>
-      <c r="AX2" s="130"/>
-      <c r="AY2" s="130"/>
-      <c r="AZ2" s="130"/>
-      <c r="BA2" s="131"/>
-      <c r="BB2" s="114" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="115"/>
-      <c r="BD2" s="115"/>
-      <c r="BE2" s="115"/>
-      <c r="BF2" s="115"/>
-      <c r="BG2" s="115"/>
-      <c r="BH2" s="115"/>
-      <c r="BI2" s="115"/>
-      <c r="BJ2" s="115"/>
-      <c r="BK2" s="115"/>
-      <c r="BL2" s="115"/>
-      <c r="BM2" s="115"/>
-      <c r="BN2" s="115"/>
-      <c r="BO2" s="115"/>
-      <c r="BP2" s="116"/>
-      <c r="BQ2" s="114" t="s">
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="122"/>
+      <c r="BF2" s="122"/>
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="123"/>
+      <c r="BQ2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="115"/>
-      <c r="BS2" s="115"/>
-      <c r="BT2" s="115"/>
-      <c r="BU2" s="115"/>
-      <c r="BV2" s="115"/>
-      <c r="BW2" s="115"/>
-      <c r="BX2" s="115"/>
-      <c r="BY2" s="115"/>
-      <c r="BZ2" s="115"/>
-      <c r="CA2" s="115"/>
-      <c r="CB2" s="115"/>
-      <c r="CC2" s="115"/>
-      <c r="CD2" s="115"/>
-      <c r="CE2" s="116"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="122"/>
+      <c r="BV2" s="122"/>
+      <c r="BW2" s="122"/>
+      <c r="BX2" s="122"/>
+      <c r="BY2" s="122"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="122"/>
+      <c r="CB2" s="122"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="122"/>
+      <c r="CE2" s="123"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="136" t="s">
+      <c r="G3" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="138" t="s">
+      <c r="H3" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="140" t="s">
+      <c r="I3" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="141" t="s">
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="141" t="s">
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="141"/>
-      <c r="U3" s="141"/>
-      <c r="V3" s="141"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="143" t="s">
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="118" t="s">
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="138"/>
+      <c r="AC3" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="118"/>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118"/>
-      <c r="AH3" s="118" t="s">
+      <c r="AD3" s="138"/>
+      <c r="AE3" s="138"/>
+      <c r="AF3" s="138"/>
+      <c r="AG3" s="138"/>
+      <c r="AH3" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118"/>
-      <c r="AK3" s="118"/>
-      <c r="AL3" s="119"/>
-      <c r="AM3" s="120" t="s">
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="138"/>
+      <c r="AK3" s="138"/>
+      <c r="AL3" s="139"/>
+      <c r="AM3" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="121"/>
-      <c r="AO3" s="121"/>
-      <c r="AP3" s="121"/>
-      <c r="AQ3" s="121"/>
-      <c r="AR3" s="121" t="s">
+      <c r="AN3" s="141"/>
+      <c r="AO3" s="141"/>
+      <c r="AP3" s="141"/>
+      <c r="AQ3" s="141"/>
+      <c r="AR3" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="121"/>
-      <c r="AT3" s="121"/>
-      <c r="AU3" s="121"/>
-      <c r="AV3" s="121"/>
-      <c r="AW3" s="121" t="s">
+      <c r="AS3" s="141"/>
+      <c r="AT3" s="141"/>
+      <c r="AU3" s="141"/>
+      <c r="AV3" s="141"/>
+      <c r="AW3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="121"/>
-      <c r="AY3" s="121"/>
-      <c r="AZ3" s="121"/>
-      <c r="BA3" s="122"/>
-      <c r="BB3" s="117" t="s">
+      <c r="AX3" s="141"/>
+      <c r="AY3" s="141"/>
+      <c r="AZ3" s="141"/>
+      <c r="BA3" s="142"/>
+      <c r="BB3" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="112"/>
-      <c r="BD3" s="112"/>
-      <c r="BE3" s="112"/>
-      <c r="BF3" s="112"/>
-      <c r="BG3" s="112" t="s">
+      <c r="BC3" s="131"/>
+      <c r="BD3" s="131"/>
+      <c r="BE3" s="131"/>
+      <c r="BF3" s="131"/>
+      <c r="BG3" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="112"/>
-      <c r="BI3" s="112"/>
-      <c r="BJ3" s="112"/>
-      <c r="BK3" s="112"/>
-      <c r="BL3" s="112" t="s">
+      <c r="BH3" s="131"/>
+      <c r="BI3" s="131"/>
+      <c r="BJ3" s="131"/>
+      <c r="BK3" s="131"/>
+      <c r="BL3" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="112"/>
-      <c r="BN3" s="112"/>
-      <c r="BO3" s="112"/>
-      <c r="BP3" s="113"/>
-      <c r="BQ3" s="117" t="s">
+      <c r="BM3" s="131"/>
+      <c r="BN3" s="131"/>
+      <c r="BO3" s="131"/>
+      <c r="BP3" s="143"/>
+      <c r="BQ3" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="BR3" s="112"/>
-      <c r="BS3" s="112"/>
-      <c r="BT3" s="112"/>
-      <c r="BU3" s="112"/>
-      <c r="BV3" s="112" t="s">
+      <c r="BR3" s="131"/>
+      <c r="BS3" s="131"/>
+      <c r="BT3" s="131"/>
+      <c r="BU3" s="131"/>
+      <c r="BV3" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="BW3" s="112"/>
-      <c r="BX3" s="112"/>
-      <c r="BY3" s="112"/>
-      <c r="BZ3" s="112"/>
-      <c r="CA3" s="112" t="s">
+      <c r="BW3" s="131"/>
+      <c r="BX3" s="131"/>
+      <c r="BY3" s="131"/>
+      <c r="BZ3" s="131"/>
+      <c r="CA3" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="CB3" s="112"/>
-      <c r="CC3" s="112"/>
-      <c r="CD3" s="112"/>
-      <c r="CE3" s="113"/>
+      <c r="CB3" s="131"/>
+      <c r="CC3" s="131"/>
+      <c r="CD3" s="131"/>
+      <c r="CE3" s="143"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="133"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="139"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="133"/>
       <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
@@ -6012,6 +6012,17 @@
     <row r="35" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -6028,17 +6039,6 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7 H9:H31">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
E-Team Week 11 (school week 10)
</commit_message>
<xml_diff>
--- a/Weekly Reports/E-Team.xlsx
+++ b/Weekly Reports/E-Team.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-General\Weekly Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64526218-16D3-4961-9916-D2D1310CF591}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="27870" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="27870" windowHeight="12495" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="115">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -371,7 +372,10 @@
     <t>[Depends on Mech]</t>
   </si>
   <si>
-    <t>We finished installing our bus bars and have tested our system's control of the wheels via the PWM HAT. Unfortunately we have learned that our battery charger does not work. It will power its fans off of the batteries, but recieves no power from the wall plug. This results in a discahrge of the batteries rather than a charge. This was a recent development, so I don't have a workaround yet. Diue to manufacturing delays, not all wheels are installed, and our testing capacity will be severely limited.</t>
+    <t>With charged batteries and the updated PWM drivers, we have tested the drive system to the limits of the mechanical hardware (there are some temporary 3D-printed) motor mounts that we have been told not to exectue turns with. We also learned that we were rejected from competition, so the team is adjusting some timelines to reduce the need for temporary solutions (e.g. the mechanical team is putting more time into arm design before manufacturing). Our priorities are autonomous navigation and the science system. Some aspects of the mechanical design of the science system are posing problems for power transmission to some of the motors. Also, as we will not have an arm to wire, develop controls for, or test, those systems are off track.</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -634,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -981,12 +985,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1162,6 +1177,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1187,6 +1204,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1214,15 +1264,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1241,12 +1282,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1265,26 +1300,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,180 +1716,180 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="80"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1889,10 +1905,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AV46"/>
+  <dimension ref="A1:AV47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1906,13 +1922,13 @@
       </c>
     </row>
     <row r="2" spans="1:48" s="68" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
     </row>
     <row r="3" spans="1:48">
       <c r="A3" s="67" t="s">
@@ -1927,28 +1943,28 @@
       <c r="A4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="88"/>
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="86"/>
+      <c r="C5" s="88"/>
     </row>
     <row r="6" spans="1:48">
       <c r="A6" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="86"/>
+      <c r="C6" s="88"/>
       <c r="AR6" s="75"/>
       <c r="AS6" s="75"/>
       <c r="AT6" s="75"/>
@@ -1960,7 +1976,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="63">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AR7" s="75"/>
       <c r="AS7" s="75"/>
@@ -1978,7 +1994,7 @@
         <v>45</v>
       </c>
       <c r="B9" s="57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AR9" s="75"/>
       <c r="AS9" s="75"/>
@@ -2023,21 +2039,21 @@
       <c r="AV12" s="75"/>
     </row>
     <row r="13" spans="1:48">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:48" ht="141.75" customHeight="1">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="83"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="85"/>
       <c r="H14" s="76"/>
       <c r="AR14" s="75"/>
       <c r="AS14" s="75"/>
@@ -2082,7 +2098,7 @@
       </c>
       <c r="C17" s="62">
         <f>'Team Task Chart'!H5</f>
-        <v>0.72916666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D17" s="60" t="s">
         <v>36</v>
@@ -2101,7 +2117,7 @@
       </c>
       <c r="C18" s="62">
         <f>'Team Task Chart'!H6</f>
-        <v>0.85000000000000009</v>
+        <v>1</v>
       </c>
       <c r="D18" s="60" t="s">
         <v>36</v>
@@ -2135,7 +2151,7 @@
       </c>
       <c r="C19" s="62">
         <f>'Team Task Chart'!H7</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>36</v>
@@ -2154,7 +2170,7 @@
       </c>
       <c r="C20" s="62">
         <f>'Team Task Chart'!H8</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D20" s="60" t="s">
         <v>36</v>
@@ -2173,7 +2189,7 @@
       </c>
       <c r="C21" s="62">
         <f>'Team Task Chart'!H9</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D21" s="60" t="s">
         <v>36</v>
@@ -2192,7 +2208,7 @@
       </c>
       <c r="C22" s="62">
         <f>'Team Task Chart'!H10</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D22" s="60" t="s">
         <v>36</v>
@@ -2210,7 +2226,7 @@
       </c>
       <c r="C23" s="62">
         <f>'Team Task Chart'!H11</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D23" s="60" t="s">
         <v>36</v>
@@ -2279,10 +2295,10 @@
       </c>
       <c r="C27" s="62">
         <f>'Team Task Chart'!H15</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D27" s="60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:48">
@@ -2296,7 +2312,7 @@
       </c>
       <c r="C28" s="62">
         <f>'Team Task Chart'!H16</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D28" s="60" t="s">
         <v>36</v>
@@ -2317,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:48">
@@ -2402,7 +2418,7 @@
         <v>0.25</v>
       </c>
       <c r="D34" s="60" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2504,7 +2520,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="D40" s="60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2521,7 +2537,7 @@
         <v>0.1</v>
       </c>
       <c r="D41" s="60" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2555,7 +2571,7 @@
         <v>0.2</v>
       </c>
       <c r="D43" s="60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2572,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2589,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2606,7 +2622,12 @@
         <v>0</v>
       </c>
       <c r="D46" s="60" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="D47" s="122" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2633,7 +2654,7 @@
       <formula>NOT(ISERROR(SEARCH("On Track",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 D26:D28 D30:D33 D35:D38 D40:D43 D45:D46 D16 D18:D19 D21:D22">
+  <conditionalFormatting sqref="D24 D26:D28 D30:D33 D35:D38 D40:D43 D16 D18:D19 D21:D22 D45:D47">
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="High Risk">
       <formula>NOT(ISERROR(SEARCH("High Risk",D16)))</formula>
     </cfRule>
@@ -2686,11 +2707,11 @@
   <dimension ref="B1:CE38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="4" topLeftCell="AO9" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D14" sqref="D14"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
-      <selection pane="bottomRight" activeCell="BO29" sqref="BO29"/>
+      <pane xSplit="8" ySplit="4" topLeftCell="AU5" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="D47" sqref="D47"/>
+      <selection pane="topRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="BD16" sqref="BD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2790,228 +2811,228 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="88" t="s">
+      <c r="I2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="91" t="s">
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="92"/>
-      <c r="AA2" s="92"/>
-      <c r="AB2" s="92"/>
-      <c r="AC2" s="92"/>
-      <c r="AD2" s="92"/>
-      <c r="AE2" s="92"/>
-      <c r="AF2" s="92"/>
-      <c r="AG2" s="92"/>
-      <c r="AH2" s="92"/>
-      <c r="AI2" s="92"/>
-      <c r="AJ2" s="92"/>
-      <c r="AK2" s="92"/>
-      <c r="AL2" s="93"/>
-      <c r="AM2" s="94" t="s">
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="106"/>
+      <c r="AM2" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="95"/>
-      <c r="AO2" s="95"/>
-      <c r="AP2" s="95"/>
-      <c r="AQ2" s="95"/>
-      <c r="AR2" s="95"/>
-      <c r="AS2" s="95"/>
-      <c r="AT2" s="95"/>
-      <c r="AU2" s="95"/>
-      <c r="AV2" s="95"/>
-      <c r="AW2" s="95"/>
-      <c r="AX2" s="95"/>
-      <c r="AY2" s="95"/>
-      <c r="AZ2" s="95"/>
-      <c r="BA2" s="96"/>
-      <c r="BB2" s="97" t="s">
+      <c r="AN2" s="108"/>
+      <c r="AO2" s="108"/>
+      <c r="AP2" s="108"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="108"/>
+      <c r="AS2" s="108"/>
+      <c r="AT2" s="108"/>
+      <c r="AU2" s="108"/>
+      <c r="AV2" s="108"/>
+      <c r="AW2" s="108"/>
+      <c r="AX2" s="108"/>
+      <c r="AY2" s="108"/>
+      <c r="AZ2" s="108"/>
+      <c r="BA2" s="109"/>
+      <c r="BB2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="98"/>
-      <c r="BD2" s="98"/>
-      <c r="BE2" s="98"/>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="98"/>
-      <c r="BH2" s="98"/>
-      <c r="BI2" s="98"/>
-      <c r="BJ2" s="98"/>
-      <c r="BK2" s="98"/>
-      <c r="BL2" s="98"/>
-      <c r="BM2" s="98"/>
-      <c r="BN2" s="98"/>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="99"/>
-      <c r="BQ2" s="97" t="s">
+      <c r="BC2" s="93"/>
+      <c r="BD2" s="93"/>
+      <c r="BE2" s="93"/>
+      <c r="BF2" s="93"/>
+      <c r="BG2" s="93"/>
+      <c r="BH2" s="93"/>
+      <c r="BI2" s="93"/>
+      <c r="BJ2" s="93"/>
+      <c r="BK2" s="93"/>
+      <c r="BL2" s="93"/>
+      <c r="BM2" s="93"/>
+      <c r="BN2" s="93"/>
+      <c r="BO2" s="93"/>
+      <c r="BP2" s="94"/>
+      <c r="BQ2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="98"/>
-      <c r="BS2" s="98"/>
-      <c r="BT2" s="98"/>
-      <c r="BU2" s="98"/>
-      <c r="BV2" s="98"/>
-      <c r="BW2" s="98"/>
-      <c r="BX2" s="98"/>
-      <c r="BY2" s="98"/>
-      <c r="BZ2" s="98"/>
-      <c r="CA2" s="98"/>
-      <c r="CB2" s="98"/>
-      <c r="CC2" s="98"/>
-      <c r="CD2" s="98"/>
-      <c r="CE2" s="99"/>
+      <c r="BR2" s="93"/>
+      <c r="BS2" s="93"/>
+      <c r="BT2" s="93"/>
+      <c r="BU2" s="93"/>
+      <c r="BV2" s="93"/>
+      <c r="BW2" s="93"/>
+      <c r="BX2" s="93"/>
+      <c r="BY2" s="93"/>
+      <c r="BZ2" s="93"/>
+      <c r="CA2" s="93"/>
+      <c r="CB2" s="93"/>
+      <c r="CC2" s="93"/>
+      <c r="CD2" s="93"/>
+      <c r="CE2" s="94"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="104" t="s">
+      <c r="F3" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="104" t="s">
+      <c r="G3" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="H3" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="110" t="s">
+      <c r="I3" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="111" t="s">
+      <c r="J3" s="119"/>
+      <c r="K3" s="119"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="111"/>
-      <c r="P3" s="111"/>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111" t="s">
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="111"/>
-      <c r="U3" s="111"/>
-      <c r="V3" s="111"/>
-      <c r="W3" s="112"/>
-      <c r="X3" s="113" t="s">
+      <c r="T3" s="119"/>
+      <c r="U3" s="119"/>
+      <c r="V3" s="119"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="114"/>
-      <c r="Z3" s="114"/>
-      <c r="AA3" s="114"/>
-      <c r="AB3" s="114"/>
-      <c r="AC3" s="114" t="s">
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="96"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="114"/>
-      <c r="AE3" s="114"/>
-      <c r="AF3" s="114"/>
-      <c r="AG3" s="114"/>
-      <c r="AH3" s="114" t="s">
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AH3" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="114"/>
-      <c r="AJ3" s="114"/>
-      <c r="AK3" s="114"/>
-      <c r="AL3" s="115"/>
-      <c r="AM3" s="116" t="s">
+      <c r="AI3" s="96"/>
+      <c r="AJ3" s="96"/>
+      <c r="AK3" s="96"/>
+      <c r="AL3" s="97"/>
+      <c r="AM3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="117"/>
-      <c r="AO3" s="117"/>
-      <c r="AP3" s="117"/>
-      <c r="AQ3" s="117"/>
-      <c r="AR3" s="117" t="s">
+      <c r="AN3" s="99"/>
+      <c r="AO3" s="99"/>
+      <c r="AP3" s="99"/>
+      <c r="AQ3" s="99"/>
+      <c r="AR3" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="117"/>
-      <c r="AT3" s="117"/>
-      <c r="AU3" s="117"/>
-      <c r="AV3" s="117"/>
-      <c r="AW3" s="117" t="s">
+      <c r="AS3" s="99"/>
+      <c r="AT3" s="99"/>
+      <c r="AU3" s="99"/>
+      <c r="AV3" s="99"/>
+      <c r="AW3" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="117"/>
-      <c r="AY3" s="117"/>
-      <c r="AZ3" s="117"/>
-      <c r="BA3" s="118"/>
-      <c r="BB3" s="106" t="s">
+      <c r="AX3" s="99"/>
+      <c r="AY3" s="99"/>
+      <c r="AZ3" s="99"/>
+      <c r="BA3" s="100"/>
+      <c r="BB3" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="107"/>
-      <c r="BD3" s="107"/>
-      <c r="BE3" s="107"/>
-      <c r="BF3" s="107"/>
-      <c r="BG3" s="107" t="s">
+      <c r="BC3" s="90"/>
+      <c r="BD3" s="90"/>
+      <c r="BE3" s="90"/>
+      <c r="BF3" s="90"/>
+      <c r="BG3" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="107"/>
-      <c r="BI3" s="107"/>
-      <c r="BJ3" s="107"/>
-      <c r="BK3" s="107"/>
-      <c r="BL3" s="107" t="s">
+      <c r="BH3" s="90"/>
+      <c r="BI3" s="90"/>
+      <c r="BJ3" s="90"/>
+      <c r="BK3" s="90"/>
+      <c r="BL3" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="107"/>
-      <c r="BN3" s="107"/>
-      <c r="BO3" s="107"/>
-      <c r="BP3" s="119"/>
-      <c r="BQ3" s="106" t="s">
+      <c r="BM3" s="90"/>
+      <c r="BN3" s="90"/>
+      <c r="BO3" s="90"/>
+      <c r="BP3" s="91"/>
+      <c r="BQ3" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="BR3" s="107"/>
-      <c r="BS3" s="107"/>
-      <c r="BT3" s="107"/>
-      <c r="BU3" s="107"/>
-      <c r="BV3" s="107" t="s">
+      <c r="BR3" s="90"/>
+      <c r="BS3" s="90"/>
+      <c r="BT3" s="90"/>
+      <c r="BU3" s="90"/>
+      <c r="BV3" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="BW3" s="107"/>
-      <c r="BX3" s="107"/>
-      <c r="BY3" s="107"/>
-      <c r="BZ3" s="107"/>
-      <c r="CA3" s="107" t="s">
+      <c r="BW3" s="90"/>
+      <c r="BX3" s="90"/>
+      <c r="BY3" s="90"/>
+      <c r="BZ3" s="90"/>
+      <c r="CA3" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="CB3" s="107"/>
-      <c r="CC3" s="107"/>
-      <c r="CD3" s="107"/>
-      <c r="CE3" s="119"/>
+      <c r="CB3" s="90"/>
+      <c r="CC3" s="90"/>
+      <c r="CD3" s="90"/>
+      <c r="CE3" s="91"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="101"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="109"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="117"/>
       <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3255,7 +3276,7 @@
       <c r="G5" s="18"/>
       <c r="H5" s="19">
         <f>AVERAGE(H6,H9,H12,H15)</f>
-        <v>0.72916666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="21"/>
@@ -3350,7 +3371,7 @@
       <c r="G6" s="27"/>
       <c r="H6" s="28">
         <f>AVERAGE(H7:H8)</f>
-        <v>0.85000000000000009</v>
+        <v>1</v>
       </c>
       <c r="I6" s="29"/>
       <c r="J6" s="30"/>
@@ -3397,16 +3418,16 @@
       <c r="AY6" s="69"/>
       <c r="AZ6" s="69"/>
       <c r="BA6" s="74"/>
-      <c r="BB6" s="29"/>
-      <c r="BC6" s="30"/>
-      <c r="BD6" s="30"/>
-      <c r="BE6" s="30"/>
-      <c r="BF6" s="30"/>
-      <c r="BG6" s="35"/>
-      <c r="BH6" s="35"/>
-      <c r="BI6" s="35"/>
-      <c r="BJ6" s="35"/>
-      <c r="BK6" s="35"/>
+      <c r="BB6" s="73"/>
+      <c r="BC6" s="69"/>
+      <c r="BD6" s="69"/>
+      <c r="BE6" s="69"/>
+      <c r="BF6" s="69"/>
+      <c r="BG6" s="69"/>
+      <c r="BH6" s="69"/>
+      <c r="BI6" s="69"/>
+      <c r="BJ6" s="69"/>
+      <c r="BK6" s="69"/>
       <c r="BL6" s="30"/>
       <c r="BM6" s="30"/>
       <c r="BN6" s="30"/>
@@ -3446,7 +3467,7 @@
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="28">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="30"/>
@@ -3493,16 +3514,16 @@
       <c r="AY7" s="69"/>
       <c r="AZ7" s="69"/>
       <c r="BA7" s="74"/>
-      <c r="BB7" s="29"/>
-      <c r="BC7" s="30"/>
-      <c r="BD7" s="30"/>
-      <c r="BE7" s="30"/>
-      <c r="BF7" s="30"/>
-      <c r="BG7" s="35"/>
-      <c r="BH7" s="35"/>
-      <c r="BI7" s="35"/>
-      <c r="BJ7" s="35"/>
-      <c r="BK7" s="35"/>
+      <c r="BB7" s="73"/>
+      <c r="BC7" s="69"/>
+      <c r="BD7" s="69"/>
+      <c r="BE7" s="69"/>
+      <c r="BF7" s="69"/>
+      <c r="BG7" s="69"/>
+      <c r="BH7" s="69"/>
+      <c r="BI7" s="69"/>
+      <c r="BJ7" s="69"/>
+      <c r="BK7" s="69"/>
       <c r="BL7" s="30"/>
       <c r="BM7" s="30"/>
       <c r="BN7" s="30"/>
@@ -3542,7 +3563,7 @@
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="28">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I8" s="29"/>
       <c r="J8" s="30"/>
@@ -3589,16 +3610,16 @@
       <c r="AY8" s="30"/>
       <c r="AZ8" s="30"/>
       <c r="BA8" s="32"/>
-      <c r="BB8" s="29"/>
-      <c r="BC8" s="30"/>
-      <c r="BD8" s="30"/>
-      <c r="BE8" s="30"/>
-      <c r="BF8" s="30"/>
-      <c r="BG8" s="35"/>
-      <c r="BH8" s="35"/>
-      <c r="BI8" s="35"/>
-      <c r="BJ8" s="35"/>
-      <c r="BK8" s="35"/>
+      <c r="BB8" s="73"/>
+      <c r="BC8" s="69"/>
+      <c r="BD8" s="69"/>
+      <c r="BE8" s="69"/>
+      <c r="BF8" s="69"/>
+      <c r="BG8" s="69"/>
+      <c r="BH8" s="69"/>
+      <c r="BI8" s="69"/>
+      <c r="BJ8" s="69"/>
+      <c r="BK8" s="69"/>
       <c r="BL8" s="30"/>
       <c r="BM8" s="30"/>
       <c r="BN8" s="30"/>
@@ -3639,7 +3660,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="28">
         <f>AVERAGE(H10:H11)</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I9" s="29"/>
       <c r="J9" s="30"/>
@@ -3686,16 +3707,16 @@
       <c r="AY9" s="69"/>
       <c r="AZ9" s="69"/>
       <c r="BA9" s="74"/>
-      <c r="BB9" s="29"/>
-      <c r="BC9" s="30"/>
-      <c r="BD9" s="30"/>
-      <c r="BE9" s="30"/>
-      <c r="BF9" s="30"/>
+      <c r="BB9" s="73"/>
+      <c r="BC9" s="69"/>
+      <c r="BD9" s="69"/>
+      <c r="BE9" s="69"/>
+      <c r="BF9" s="69"/>
       <c r="BG9" s="35"/>
       <c r="BH9" s="35"/>
       <c r="BI9" s="35"/>
       <c r="BJ9" s="35"/>
-      <c r="BK9" s="35"/>
+      <c r="BK9" s="69"/>
       <c r="BL9" s="30"/>
       <c r="BM9" s="30"/>
       <c r="BN9" s="30"/>
@@ -3735,7 +3756,7 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="28">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I10" s="29"/>
       <c r="J10" s="30"/>
@@ -3786,12 +3807,12 @@
       <c r="BC10" s="30"/>
       <c r="BD10" s="30"/>
       <c r="BE10" s="30"/>
-      <c r="BF10" s="30"/>
+      <c r="BF10" s="69"/>
       <c r="BG10" s="35"/>
       <c r="BH10" s="35"/>
       <c r="BI10" s="35"/>
       <c r="BJ10" s="35"/>
-      <c r="BK10" s="35"/>
+      <c r="BK10" s="69"/>
       <c r="BL10" s="30"/>
       <c r="BM10" s="30"/>
       <c r="BN10" s="30"/>
@@ -3831,7 +3852,7 @@
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="28">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I11" s="73"/>
       <c r="J11" s="69"/>
@@ -3882,11 +3903,11 @@
       <c r="BC11" s="30"/>
       <c r="BD11" s="30"/>
       <c r="BE11" s="30"/>
-      <c r="BF11" s="30"/>
+      <c r="BF11" s="69"/>
       <c r="BG11" s="35"/>
       <c r="BH11" s="35"/>
       <c r="BI11" s="35"/>
-      <c r="BJ11" s="35"/>
+      <c r="BJ11" s="69"/>
       <c r="BK11" s="35"/>
       <c r="BL11" s="30"/>
       <c r="BM11" s="30"/>
@@ -4162,11 +4183,11 @@
       <c r="AT14" s="34"/>
       <c r="AU14" s="34"/>
       <c r="AV14" s="34"/>
-      <c r="AW14" s="120"/>
-      <c r="AX14" s="120"/>
-      <c r="AY14" s="120"/>
-      <c r="AZ14" s="120"/>
-      <c r="BA14" s="121"/>
+      <c r="AW14" s="79"/>
+      <c r="AX14" s="79"/>
+      <c r="AY14" s="79"/>
+      <c r="AZ14" s="79"/>
+      <c r="BA14" s="80"/>
       <c r="BB14" s="29"/>
       <c r="BC14" s="30"/>
       <c r="BD14" s="30"/>
@@ -4218,7 +4239,7 @@
       <c r="G15" s="27"/>
       <c r="H15" s="28">
         <f>AVERAGE(H16:H18)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="30"/>
@@ -4313,7 +4334,7 @@
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="30"/>
@@ -4917,36 +4938,36 @@
       <c r="AE22" s="33"/>
       <c r="AF22" s="33"/>
       <c r="AG22" s="33"/>
-      <c r="AH22" s="30"/>
-      <c r="AI22" s="30"/>
-      <c r="AJ22" s="30"/>
-      <c r="AK22" s="30"/>
-      <c r="AL22" s="32"/>
-      <c r="AM22" s="29"/>
-      <c r="AN22" s="30"/>
-      <c r="AO22" s="30"/>
-      <c r="AP22" s="30"/>
-      <c r="AQ22" s="30"/>
-      <c r="AR22" s="34"/>
-      <c r="AS22" s="34"/>
-      <c r="AT22" s="34"/>
-      <c r="AU22" s="34"/>
-      <c r="AV22" s="34"/>
-      <c r="AW22" s="30"/>
-      <c r="AX22" s="30"/>
-      <c r="AY22" s="30"/>
-      <c r="AZ22" s="30"/>
-      <c r="BA22" s="32"/>
-      <c r="BB22" s="29"/>
-      <c r="BC22" s="30"/>
-      <c r="BD22" s="30"/>
-      <c r="BE22" s="30"/>
-      <c r="BF22" s="30"/>
-      <c r="BG22" s="35"/>
-      <c r="BH22" s="35"/>
-      <c r="BI22" s="35"/>
-      <c r="BJ22" s="35"/>
-      <c r="BK22" s="35"/>
+      <c r="AH22" s="69"/>
+      <c r="AI22" s="69"/>
+      <c r="AJ22" s="69"/>
+      <c r="AK22" s="69"/>
+      <c r="AL22" s="74"/>
+      <c r="AM22" s="73"/>
+      <c r="AN22" s="69"/>
+      <c r="AO22" s="69"/>
+      <c r="AP22" s="69"/>
+      <c r="AQ22" s="69"/>
+      <c r="AR22" s="69"/>
+      <c r="AS22" s="69"/>
+      <c r="AT22" s="69"/>
+      <c r="AU22" s="69"/>
+      <c r="AV22" s="69"/>
+      <c r="AW22" s="69"/>
+      <c r="AX22" s="69"/>
+      <c r="AY22" s="69"/>
+      <c r="AZ22" s="69"/>
+      <c r="BA22" s="74"/>
+      <c r="BB22" s="73"/>
+      <c r="BC22" s="69"/>
+      <c r="BD22" s="69"/>
+      <c r="BE22" s="69"/>
+      <c r="BF22" s="69"/>
+      <c r="BG22" s="69"/>
+      <c r="BH22" s="69"/>
+      <c r="BI22" s="69"/>
+      <c r="BJ22" s="69"/>
+      <c r="BK22" s="69"/>
       <c r="BL22" s="30"/>
       <c r="BM22" s="30"/>
       <c r="BN22" s="30"/>
@@ -5131,16 +5152,16 @@
       <c r="AY24" s="69"/>
       <c r="AZ24" s="69"/>
       <c r="BA24" s="74"/>
-      <c r="BB24" s="29"/>
-      <c r="BC24" s="30"/>
-      <c r="BD24" s="30"/>
-      <c r="BE24" s="30"/>
-      <c r="BF24" s="30"/>
-      <c r="BG24" s="35"/>
-      <c r="BH24" s="35"/>
-      <c r="BI24" s="35"/>
-      <c r="BJ24" s="35"/>
-      <c r="BK24" s="35"/>
+      <c r="BB24" s="73"/>
+      <c r="BC24" s="69"/>
+      <c r="BD24" s="69"/>
+      <c r="BE24" s="69"/>
+      <c r="BF24" s="69"/>
+      <c r="BG24" s="69"/>
+      <c r="BH24" s="69"/>
+      <c r="BI24" s="69"/>
+      <c r="BJ24" s="69"/>
+      <c r="BK24" s="69"/>
       <c r="BL24" s="30"/>
       <c r="BM24" s="30"/>
       <c r="BN24" s="30"/>
@@ -5224,21 +5245,21 @@
       <c r="AT25" s="69"/>
       <c r="AU25" s="69"/>
       <c r="AV25" s="69"/>
-      <c r="AW25" s="30"/>
-      <c r="AX25" s="30"/>
-      <c r="AY25" s="30"/>
-      <c r="AZ25" s="30"/>
-      <c r="BA25" s="32"/>
-      <c r="BB25" s="29"/>
-      <c r="BC25" s="30"/>
-      <c r="BD25" s="30"/>
-      <c r="BE25" s="30"/>
-      <c r="BF25" s="30"/>
-      <c r="BG25" s="35"/>
-      <c r="BH25" s="35"/>
-      <c r="BI25" s="35"/>
-      <c r="BJ25" s="35"/>
-      <c r="BK25" s="35"/>
+      <c r="AW25" s="69"/>
+      <c r="AX25" s="69"/>
+      <c r="AY25" s="69"/>
+      <c r="AZ25" s="69"/>
+      <c r="BA25" s="74"/>
+      <c r="BB25" s="73"/>
+      <c r="BC25" s="69"/>
+      <c r="BD25" s="69"/>
+      <c r="BE25" s="69"/>
+      <c r="BF25" s="69"/>
+      <c r="BG25" s="69"/>
+      <c r="BH25" s="69"/>
+      <c r="BI25" s="69"/>
+      <c r="BJ25" s="69"/>
+      <c r="BK25" s="69"/>
       <c r="BL25" s="30"/>
       <c r="BM25" s="30"/>
       <c r="BN25" s="30"/>
@@ -5311,31 +5332,31 @@
       <c r="AJ26" s="30"/>
       <c r="AK26" s="30"/>
       <c r="AL26" s="32"/>
-      <c r="AM26" s="29"/>
-      <c r="AN26" s="30"/>
-      <c r="AO26" s="30"/>
-      <c r="AP26" s="30"/>
-      <c r="AQ26" s="30"/>
-      <c r="AR26" s="34"/>
-      <c r="AS26" s="34"/>
-      <c r="AT26" s="34"/>
-      <c r="AU26" s="34"/>
-      <c r="AV26" s="34"/>
-      <c r="AW26" s="30"/>
-      <c r="AX26" s="30"/>
-      <c r="AY26" s="30"/>
-      <c r="AZ26" s="30"/>
-      <c r="BA26" s="32"/>
-      <c r="BB26" s="29"/>
-      <c r="BC26" s="30"/>
-      <c r="BD26" s="30"/>
-      <c r="BE26" s="30"/>
-      <c r="BF26" s="30"/>
-      <c r="BG26" s="35"/>
-      <c r="BH26" s="35"/>
-      <c r="BI26" s="35"/>
-      <c r="BJ26" s="35"/>
-      <c r="BK26" s="35"/>
+      <c r="AM26" s="73"/>
+      <c r="AN26" s="69"/>
+      <c r="AO26" s="69"/>
+      <c r="AP26" s="69"/>
+      <c r="AQ26" s="69"/>
+      <c r="AR26" s="69"/>
+      <c r="AS26" s="69"/>
+      <c r="AT26" s="69"/>
+      <c r="AU26" s="69"/>
+      <c r="AV26" s="69"/>
+      <c r="AW26" s="69"/>
+      <c r="AX26" s="69"/>
+      <c r="AY26" s="69"/>
+      <c r="AZ26" s="69"/>
+      <c r="BA26" s="74"/>
+      <c r="BB26" s="73"/>
+      <c r="BC26" s="69"/>
+      <c r="BD26" s="69"/>
+      <c r="BE26" s="69"/>
+      <c r="BF26" s="69"/>
+      <c r="BG26" s="69"/>
+      <c r="BH26" s="69"/>
+      <c r="BI26" s="69"/>
+      <c r="BJ26" s="69"/>
+      <c r="BK26" s="69"/>
       <c r="BL26" s="30"/>
       <c r="BM26" s="30"/>
       <c r="BN26" s="30"/>
@@ -5415,24 +5436,24 @@
       <c r="AQ27" s="30"/>
       <c r="AR27" s="34"/>
       <c r="AS27" s="34"/>
-      <c r="AT27" s="34"/>
-      <c r="AU27" s="34"/>
-      <c r="AV27" s="34"/>
-      <c r="AW27" s="30"/>
-      <c r="AX27" s="30"/>
-      <c r="AY27" s="30"/>
-      <c r="AZ27" s="30"/>
-      <c r="BA27" s="32"/>
-      <c r="BB27" s="29"/>
-      <c r="BC27" s="30"/>
-      <c r="BD27" s="30"/>
-      <c r="BE27" s="30"/>
-      <c r="BF27" s="30"/>
-      <c r="BG27" s="35"/>
-      <c r="BH27" s="35"/>
-      <c r="BI27" s="35"/>
-      <c r="BJ27" s="35"/>
-      <c r="BK27" s="35"/>
+      <c r="AT27" s="69"/>
+      <c r="AU27" s="69"/>
+      <c r="AV27" s="69"/>
+      <c r="AW27" s="69"/>
+      <c r="AX27" s="69"/>
+      <c r="AY27" s="69"/>
+      <c r="AZ27" s="69"/>
+      <c r="BA27" s="74"/>
+      <c r="BB27" s="73"/>
+      <c r="BC27" s="69"/>
+      <c r="BD27" s="69"/>
+      <c r="BE27" s="69"/>
+      <c r="BF27" s="69"/>
+      <c r="BG27" s="69"/>
+      <c r="BH27" s="69"/>
+      <c r="BI27" s="69"/>
+      <c r="BJ27" s="69"/>
+      <c r="BK27" s="69"/>
       <c r="BL27" s="30"/>
       <c r="BM27" s="30"/>
       <c r="BN27" s="30"/>
@@ -6123,17 +6144,6 @@
     <row r="38" spans="2:83" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -6150,6 +6160,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H34">
     <cfRule type="dataBar" priority="1">

</xml_diff>